<commit_message>
Added USA test case model script RECC_USA_TestCase_V1.0.py.
</commit_message>
<xml_diff>
--- a/RECC_Config.xlsx
+++ b/RECC_Config.xlsx
@@ -9,20 +9,21 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21156" windowHeight="10320" tabRatio="844" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8652" windowHeight="4896" tabRatio="844" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="5" r:id="rId1"/>
-    <sheet name="RECC_Main_Development_1" sheetId="7" r:id="rId2"/>
-    <sheet name="GDP_Test" sheetId="8" r:id="rId3"/>
-    <sheet name="Setting_TestRun_1" sheetId="6" r:id="rId4"/>
+    <sheet name="RECC_USA_TestCase_V1.0" sheetId="9" r:id="rId2"/>
+    <sheet name="RECC_Main_Development_1" sheetId="7" r:id="rId3"/>
+    <sheet name="GDP_Test" sheetId="8" r:id="rId4"/>
+    <sheet name="Setting_TestRun_1" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1010" uniqueCount="458">
   <si>
     <t>Description</t>
   </si>
@@ -850,6 +851,552 @@
   </si>
   <si>
     <t>gUr</t>
+  </si>
+  <si>
+    <t>[31]</t>
+  </si>
+  <si>
+    <t>PlotStocks</t>
+  </si>
+  <si>
+    <t>PlotMaterialDemand</t>
+  </si>
+  <si>
+    <t>PlotTotalGHGEmissions</t>
+  </si>
+  <si>
+    <t>True</t>
+  </si>
+  <si>
+    <t>[315:361)</t>
+  </si>
+  <si>
+    <t>Evaluate six RE strategies for US, pilot case study</t>
+  </si>
+  <si>
+    <t>Scenario_RCP</t>
+  </si>
+  <si>
+    <t>RCP scenarios</t>
+  </si>
+  <si>
+    <t>RCP_Scenarios</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>[0,2,6,8,9,10]</t>
+  </si>
+  <si>
+    <t>Nergy (energy)</t>
+  </si>
+  <si>
+    <t>[0,1,5,7,8,14,20]</t>
+  </si>
+  <si>
+    <t>[18]</t>
+  </si>
+  <si>
+    <t>2_P_RECC_Population_SSP_32R_V1.0</t>
+  </si>
+  <si>
+    <t>2_P_RECC_Population_SSP_32R</t>
+  </si>
+  <si>
+    <t>exogenous population scenarios, SSP</t>
+  </si>
+  <si>
+    <t>SSP_Population_model</t>
+  </si>
+  <si>
+    <t>Population model used for SSP scenarios</t>
+  </si>
+  <si>
+    <t>SSP population Model</t>
+  </si>
+  <si>
+    <t>UUID</t>
+  </si>
+  <si>
+    <t>4a47a61a-9a89-431f-970c-78e98f86591c</t>
+  </si>
+  <si>
+    <t>2_S_RECC_FinalProducts_2015_USA_V1.0</t>
+  </si>
+  <si>
+    <t>2_S_RECC_FinalProducts_2015_USA</t>
+  </si>
+  <si>
+    <t>in-use stock by age-cohort</t>
+  </si>
+  <si>
+    <t>8e4c8a8d-933a-4249-b994-d9f04c1ade68</t>
+  </si>
+  <si>
+    <t>tcgr</t>
+  </si>
+  <si>
+    <t>2_S_RECC_FinalProducts_Future_USA_V1.0</t>
+  </si>
+  <si>
+    <t>2_S_RECC_FinalProducts_Future_USA</t>
+  </si>
+  <si>
+    <t>future in-use stock scenarios</t>
+  </si>
+  <si>
+    <t>df62e207-4851-4cfd-966e-2d092d33528b</t>
+  </si>
+  <si>
+    <t>Stgr</t>
+  </si>
+  <si>
+    <t>RECC_Classifications_Master_V1.0</t>
+  </si>
+  <si>
+    <t>USA_TestCase_V1.0</t>
+  </si>
+  <si>
+    <t>RECC_USA_TestCase_V1.0</t>
+  </si>
+  <si>
+    <t>1.0</t>
+  </si>
+  <si>
+    <t>3_EI_Products_UsePhase_USA_V1.0</t>
+  </si>
+  <si>
+    <t>3_IU_Products_UsePhase_USA_V1.0</t>
+  </si>
+  <si>
+    <t>3_EI_Products_UsePhase_USA</t>
+  </si>
+  <si>
+    <t>3_IU_Products_UsePhase_USA</t>
+  </si>
+  <si>
+    <t>energy intensity of products in use phase</t>
+  </si>
+  <si>
+    <t>intensity of use of products in use phase</t>
+  </si>
+  <si>
+    <t>089dbb1a-d9c0-4592-8899-08eaa59e8bfb</t>
+  </si>
+  <si>
+    <t>tgrS</t>
+  </si>
+  <si>
+    <t>[0,1,2,3,4]</t>
+  </si>
+  <si>
+    <t>66c92395-cf6f-46bd-869a-24c56337b6ab</t>
+  </si>
+  <si>
+    <t>3_LT_RECC_ProductLifetime_V1.0</t>
+  </si>
+  <si>
+    <t>9e5e93e6-9025-452f-99f8-2300bcd92629</t>
+  </si>
+  <si>
+    <t>lifetime of products in use phase</t>
+  </si>
+  <si>
+    <t>3_MC_RECC_FinalProducts_Buildings_USA_V1.0</t>
+  </si>
+  <si>
+    <t>7b338d57-00d6-4883-987b-f450545047f9</t>
+  </si>
+  <si>
+    <t>material composition scenarios, buildings</t>
+  </si>
+  <si>
+    <t>3_LT_RECC_ProductLifetime</t>
+  </si>
+  <si>
+    <t>3_MC_RECC_FinalProducts_Buildings_USA</t>
+  </si>
+  <si>
+    <t>Component</t>
+  </si>
+  <si>
+    <t>Component of good</t>
+  </si>
+  <si>
+    <t>Products_components_m3</t>
+  </si>
+  <si>
+    <t>[0,6]</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>komponent</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>engineering Materials</t>
+  </si>
+  <si>
+    <t>ckmgr</t>
+  </si>
+  <si>
+    <t>a1fdd7fb-401a-4324-af87-086e973ebd5b</t>
+  </si>
+  <si>
+    <t>3_MC_RECC_FinalProducts_Vehicles_USA_V1.0</t>
+  </si>
+  <si>
+    <t>material composition scenarios, vehicles</t>
+  </si>
+  <si>
+    <t>3_MC_RECC_FinalProducts_Vehicles_USA</t>
+  </si>
+  <si>
+    <t>3_PR_RECC_CO2Price_SSP_32R_V1.0</t>
+  </si>
+  <si>
+    <t>3_PR_RECC_CO2Price_SSP_32R</t>
+  </si>
+  <si>
+    <t>CO2 price by scenario</t>
+  </si>
+  <si>
+    <t>1f504d97-7063-4479-b1b9-3392cc7ab69a</t>
+  </si>
+  <si>
+    <t>RtrS</t>
+  </si>
+  <si>
+    <t>3_SHA_RECC_REStrategyScaleUp_SSP_32R_V1.0</t>
+  </si>
+  <si>
+    <t>RE strategy scaleup factors</t>
+  </si>
+  <si>
+    <t>3_SHA_RECC_REStrategyScaleUp_SSP_32R</t>
+  </si>
+  <si>
+    <t>b1c77efe-7e1e-4753-97a0-7526800fc205</t>
+  </si>
+  <si>
+    <t>4_PE_GHGIntensityEnergySupply_V1.0</t>
+  </si>
+  <si>
+    <t>XnSt</t>
+  </si>
+  <si>
+    <t>5fdb83c8-c5d3-40ea-909b-f9630d48cc96</t>
+  </si>
+  <si>
+    <t>GHG intensity of energy supply</t>
+  </si>
+  <si>
+    <t>4_PE_ProcessExtensions_USA_V1.0</t>
+  </si>
+  <si>
+    <t>4_PY_EoL_RR_USA_V1.0</t>
+  </si>
+  <si>
+    <t>4_PE_GHGIntensityEnergySupply</t>
+  </si>
+  <si>
+    <t>4_PE_ProcessExtensions_USA</t>
+  </si>
+  <si>
+    <t>4_PY_EoL_RR_USA</t>
+  </si>
+  <si>
+    <t>9607b234-7ca3-4d97-b028-b26a51f16b21</t>
+  </si>
+  <si>
+    <t>recovery rate of scrap from EoL processes</t>
+  </si>
+  <si>
+    <t>lrmw</t>
+  </si>
+  <si>
+    <t>4_PY_Manufacturing_USA_V1.0</t>
+  </si>
+  <si>
+    <t>4_PY_Manufacturing_USA</t>
+  </si>
+  <si>
+    <t>manufacturing yield loss rate</t>
+  </si>
+  <si>
+    <t>394bfd3b-c19e-4cc1-b5e6-36831b184329</t>
+  </si>
+  <si>
+    <t>4_PY_MaterialProductionRemelting_V1.0</t>
+  </si>
+  <si>
+    <t>4_PY_MaterialProductionRemelting</t>
+  </si>
+  <si>
+    <t>remelting yields</t>
+  </si>
+  <si>
+    <t>b21dd6a3-1b1b-43d9-8a8a-2dcec2520b41</t>
+  </si>
+  <si>
+    <t>1c1ffc13-78a2-453e-8ebf-5a57bc711567</t>
+  </si>
+  <si>
+    <t>afa78aba-88ac-4677-9ebb-5bf5f762b63f</t>
+  </si>
+  <si>
+    <t>wmePtr</t>
+  </si>
+  <si>
+    <t>[0,1,2,3,4,5]</t>
+  </si>
+  <si>
+    <t>6_PR_EoL_RR_Improvement_USA_V1.0</t>
+  </si>
+  <si>
+    <t>5ec8367c-7ab5-4f02-a213-814c42c24fa3</t>
+  </si>
+  <si>
+    <t>6_PR_MoreIntenseUse_USA_V1.0</t>
+  </si>
+  <si>
+    <t>RE strategy: Improvement of the end-of-life recovery rate</t>
+  </si>
+  <si>
+    <t>RE strategy: More intense use</t>
+  </si>
+  <si>
+    <t>9672304f-0f90-4e93-8407-4ce60553f3bb</t>
+  </si>
+  <si>
+    <t>6_PR_EoL_RR_Improvement_USA</t>
+  </si>
+  <si>
+    <t>6_PR_MoreIntenseUse_USA</t>
+  </si>
+  <si>
+    <t>6e5be25b-792e-4c88-9cb4-ac84882fe3c0</t>
+  </si>
+  <si>
+    <t>6_PR_LightWeighting_USA_V1.0</t>
+  </si>
+  <si>
+    <t>RE strategy: light-weighting</t>
+  </si>
+  <si>
+    <t>6_PR_LightWeighting_USA</t>
+  </si>
+  <si>
+    <t>6_PR_LifeTimeExtension_USA_V1.0</t>
+  </si>
+  <si>
+    <t>6_PR_LifeTimeExtension_USA</t>
+  </si>
+  <si>
+    <t>RE strategy: useful product lifetime extension</t>
+  </si>
+  <si>
+    <t>48688221-e0b0-4ab4-8ab1-9bbcc95a38d1</t>
+  </si>
+  <si>
+    <t>RE strategy: fabrication yield improvement</t>
+  </si>
+  <si>
+    <t>6_PR_FabricationYieldImprovement_USA_V1.0</t>
+  </si>
+  <si>
+    <t>6_PR_FabricationYieldImprovement_USA</t>
+  </si>
+  <si>
+    <t>mgrS</t>
+  </si>
+  <si>
+    <t>6_PR_ReUse_USA_V1.0</t>
+  </si>
+  <si>
+    <t>6_PR_ReUse_USA</t>
+  </si>
+  <si>
+    <t>RE strategy: EoL product re-use</t>
+  </si>
+  <si>
+    <t>4_EI_ProcessEnergyIntensity_USA</t>
+  </si>
+  <si>
+    <t>Env. extensions of processes</t>
+  </si>
+  <si>
+    <t>specific energy consumption of processes</t>
+  </si>
+  <si>
+    <t>Pncr</t>
+  </si>
+  <si>
+    <t>market/distribution</t>
+  </si>
+  <si>
+    <t>industry/transformation</t>
+  </si>
+  <si>
+    <t>not included here</t>
+  </si>
+  <si>
+    <t>fabrication and manufacturing industries</t>
+  </si>
+  <si>
+    <t>market for consumer goods, buildings, vehicles, and other final products</t>
+  </si>
+  <si>
+    <t>use phase</t>
+  </si>
+  <si>
+    <t>EoL products distribution</t>
+  </si>
+  <si>
+    <t>waste management industries</t>
+  </si>
+  <si>
+    <t>waste and scrap markets</t>
+  </si>
+  <si>
+    <t>aggregated with m6</t>
+  </si>
+  <si>
+    <t>aggregated with i6</t>
+  </si>
+  <si>
+    <t>energy and service supply sectors</t>
+  </si>
+  <si>
+    <t>energy and service markets</t>
+  </si>
+  <si>
+    <t>End of file</t>
+  </si>
+  <si>
+    <t>all</t>
+  </si>
+  <si>
+    <t>[11]</t>
+  </si>
+  <si>
+    <t>[0:15)</t>
+  </si>
+  <si>
+    <t>PXcr</t>
+  </si>
+  <si>
+    <t>4_EI_ProcessEnergyIntensity_USA_V1.0</t>
+  </si>
+  <si>
+    <t>Include_REStrategy_ReUse</t>
+  </si>
+  <si>
+    <t>Include_REStrategy_MoreIntenseUse</t>
+  </si>
+  <si>
+    <t>Include_REStrategy_LightWeighting</t>
+  </si>
+  <si>
+    <t>Include_REStrategy_LifeTimeExtension</t>
+  </si>
+  <si>
+    <t>Include_REStrategy_FabYieldImprovement</t>
+  </si>
+  <si>
+    <t>Include_REStrategy_EoL_RR_Improvement</t>
+  </si>
+  <si>
+    <t>[200:361)</t>
+  </si>
+  <si>
+    <t>mwgFtr</t>
+  </si>
+  <si>
+    <t>False</t>
+  </si>
+  <si>
+    <t>cgnrS</t>
+  </si>
+  <si>
+    <t>6_PR_DirectEmissions</t>
+  </si>
+  <si>
+    <t>Direct GHG emissions by fuel type</t>
+  </si>
+  <si>
+    <t>6_PR_DirectEmissions_V1.0</t>
+  </si>
+  <si>
+    <t>Xn</t>
+  </si>
+  <si>
+    <t>d8986039-6b23-4829-9370-78edb57b255f</t>
+  </si>
+  <si>
+    <t>Selector*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    *) Selector: specify string to select index values, choose one of four options: 'All' or list of indices to select: '[0,1,10,15,28]', or 'All except [3,4,5,6,7]', or semi-open interval '[260:401)'</t>
+  </si>
+  <si>
+    <t>element composition of materials in existing stock</t>
+  </si>
+  <si>
+    <t>element composition of materials, primary production</t>
+  </si>
+  <si>
+    <t>3_MC_Elements_Materials_ExistingStock</t>
+  </si>
+  <si>
+    <t>3_MC_Elements_Materials_Primary</t>
+  </si>
+  <si>
+    <t>3_MC_Elements_Materials_ExistingStock_V1.0</t>
+  </si>
+  <si>
+    <t>3_MC_Elements_Materials_Primary_V1.0</t>
+  </si>
+  <si>
+    <t>032ef552-dbcf-4114-af35-cfd284a794d5</t>
+  </si>
+  <si>
+    <t>9366cf4b-f148-4751-b90c-5d9c1b80cb8f</t>
+  </si>
+  <si>
+    <t>me</t>
+  </si>
+  <si>
+    <t>[0, 13, 24, 26, 29,101]</t>
+  </si>
+  <si>
+    <t>primary material production</t>
+  </si>
+  <si>
+    <t>remelting industries</t>
+  </si>
+  <si>
+    <t>market for primary materials</t>
+  </si>
+  <si>
+    <t>secondary material markets</t>
+  </si>
+  <si>
+    <t>[0,1,2,3,4,5,6,7,8,9,11,12,13,14]</t>
+  </si>
+  <si>
+    <t>mining and refining</t>
+  </si>
+  <si>
+    <t>markets for ores and concentrates</t>
+  </si>
+  <si>
+    <t>[21:42)</t>
   </si>
 </sst>
 </file>
@@ -955,7 +1502,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -1033,11 +1580,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1140,10 +1696,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1427,7 +1985,7 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1470,7 +2028,7 @@
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="6" t="s">
-        <v>248</v>
+        <v>311</v>
       </c>
       <c r="G4" s="48"/>
     </row>
@@ -1503,20 +2061,18 @@
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
     </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="10"/>
       <c r="B9" s="16"/>
       <c r="C9" s="7"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
     </row>
-    <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="15"/>
       <c r="B10" s="17"/>
       <c r="C10" s="17"/>
-      <c r="D10" s="50" t="s">
-        <v>245</v>
-      </c>
+      <c r="D10" s="48"/>
       <c r="E10" s="5"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -1623,10 +2179,1675 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:K100"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="E10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="17.77734375" customWidth="1"/>
+    <col min="3" max="3" width="41.88671875" customWidth="1"/>
+    <col min="4" max="4" width="65.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="50.6640625" customWidth="1"/>
+    <col min="6" max="6" width="27.44140625" customWidth="1"/>
+    <col min="7" max="7" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="43.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B2" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="28"/>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C3" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" s="41" t="s">
+        <v>56</v>
+      </c>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="42" t="s">
+        <v>310</v>
+      </c>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="20"/>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="42" t="s">
+        <v>282</v>
+      </c>
+      <c r="I5" s="20"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="20"/>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="43" t="s">
+        <v>311</v>
+      </c>
+      <c r="I6" s="20"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="20"/>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="D7" s="11"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="20"/>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B8" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="28"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="20"/>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C9" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="D9" s="41" t="s">
+        <v>207</v>
+      </c>
+      <c r="E9" s="31"/>
+      <c r="F9" s="39"/>
+      <c r="G9" s="39"/>
+      <c r="H9" s="39"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="19"/>
+      <c r="K9" s="20"/>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="42" t="s">
+        <v>309</v>
+      </c>
+      <c r="I10" s="20"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="20"/>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C11" t="s">
+        <v>267</v>
+      </c>
+      <c r="D11" s="50" t="s">
+        <v>312</v>
+      </c>
+      <c r="I11" s="20"/>
+      <c r="J11" s="19"/>
+      <c r="K11" s="20"/>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C12" t="s">
+        <v>268</v>
+      </c>
+      <c r="D12" s="50" t="s">
+        <v>312</v>
+      </c>
+      <c r="I12" s="20"/>
+      <c r="J12" s="19"/>
+      <c r="K12" s="20"/>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="I13" s="20"/>
+      <c r="J13" s="25"/>
+      <c r="K13" s="20"/>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B14" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="C14" s="27"/>
+      <c r="D14" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="E14" s="27"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="27"/>
+      <c r="H14" s="28"/>
+      <c r="I14" s="36" t="s">
+        <v>439</v>
+      </c>
+      <c r="J14" s="20"/>
+      <c r="K14" s="20"/>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C15" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="E15" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15" s="31" t="s">
+        <v>438</v>
+      </c>
+      <c r="H15" s="30" t="s">
+        <v>186</v>
+      </c>
+      <c r="I15" s="52" t="s">
+        <v>187</v>
+      </c>
+      <c r="K15" s="20"/>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C16" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" t="s">
+        <v>28</v>
+      </c>
+      <c r="E16" t="s">
+        <v>16</v>
+      </c>
+      <c r="F16" t="s">
+        <v>16</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="H16" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="I16" s="20" t="s">
+        <v>188</v>
+      </c>
+      <c r="J16" s="20"/>
+      <c r="K16" s="20"/>
+    </row>
+    <row r="17" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C17" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" t="s">
+        <v>29</v>
+      </c>
+      <c r="E17" t="s">
+        <v>16</v>
+      </c>
+      <c r="F17" t="s">
+        <v>16</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>429</v>
+      </c>
+      <c r="H17" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="I17" s="20" t="s">
+        <v>189</v>
+      </c>
+      <c r="J17" s="20"/>
+      <c r="K17" s="20"/>
+    </row>
+    <row r="18" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C18" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" t="s">
+        <v>37</v>
+      </c>
+      <c r="E18" t="s">
+        <v>23</v>
+      </c>
+      <c r="F18" t="s">
+        <v>42</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>449</v>
+      </c>
+      <c r="H18" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="I18" s="20" t="s">
+        <v>190</v>
+      </c>
+      <c r="J18" s="20"/>
+      <c r="K18" s="20"/>
+    </row>
+    <row r="19" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C19" s="33" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" t="s">
+        <v>38</v>
+      </c>
+      <c r="E19" t="s">
+        <v>24</v>
+      </c>
+      <c r="F19" t="s">
+        <v>24</v>
+      </c>
+      <c r="G19" t="s">
+        <v>418</v>
+      </c>
+      <c r="H19" s="29">
+        <v>1</v>
+      </c>
+      <c r="I19" s="20" t="s">
+        <v>192</v>
+      </c>
+      <c r="J19" s="20"/>
+      <c r="K19" s="20"/>
+    </row>
+    <row r="20" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C20" s="33" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" t="s">
+        <v>31</v>
+      </c>
+      <c r="E20" t="s">
+        <v>39</v>
+      </c>
+      <c r="F20" t="s">
+        <v>40</v>
+      </c>
+      <c r="G20" t="s">
+        <v>276</v>
+      </c>
+      <c r="H20" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="I20" s="20" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="21" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C21" s="45" t="s">
+        <v>142</v>
+      </c>
+      <c r="D21" t="s">
+        <v>150</v>
+      </c>
+      <c r="E21" t="s">
+        <v>26</v>
+      </c>
+      <c r="F21" t="s">
+        <v>155</v>
+      </c>
+      <c r="G21" t="s">
+        <v>457</v>
+      </c>
+      <c r="H21" s="29" t="s">
+        <v>184</v>
+      </c>
+      <c r="I21" s="20" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="22" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C22" s="45" t="s">
+        <v>143</v>
+      </c>
+      <c r="D22" t="s">
+        <v>151</v>
+      </c>
+      <c r="E22" t="s">
+        <v>26</v>
+      </c>
+      <c r="F22" t="s">
+        <v>156</v>
+      </c>
+      <c r="G22" t="s">
+        <v>420</v>
+      </c>
+      <c r="H22" s="29" t="s">
+        <v>179</v>
+      </c>
+      <c r="I22" s="20" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="23" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C23" s="45" t="s">
+        <v>144</v>
+      </c>
+      <c r="D23" t="s">
+        <v>152</v>
+      </c>
+      <c r="E23" t="s">
+        <v>26</v>
+      </c>
+      <c r="F23" t="s">
+        <v>157</v>
+      </c>
+      <c r="G23" t="s">
+        <v>420</v>
+      </c>
+      <c r="H23" s="29" t="s">
+        <v>178</v>
+      </c>
+      <c r="I23" s="20" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C24" s="45" t="s">
+        <v>145</v>
+      </c>
+      <c r="D24" t="s">
+        <v>148</v>
+      </c>
+      <c r="E24" t="s">
+        <v>26</v>
+      </c>
+      <c r="F24" t="s">
+        <v>106</v>
+      </c>
+      <c r="G24" t="s">
+        <v>290</v>
+      </c>
+      <c r="H24" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="I24" s="20" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="25" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C25" s="45" t="s">
+        <v>163</v>
+      </c>
+      <c r="D25" t="s">
+        <v>159</v>
+      </c>
+      <c r="E25" t="s">
+        <v>21</v>
+      </c>
+      <c r="F25" t="s">
+        <v>134</v>
+      </c>
+      <c r="G25" t="s">
+        <v>454</v>
+      </c>
+      <c r="H25" s="29" t="s">
+        <v>337</v>
+      </c>
+      <c r="I25" s="20" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="26" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C26" s="45" t="s">
+        <v>20</v>
+      </c>
+      <c r="D26" t="s">
+        <v>32</v>
+      </c>
+      <c r="E26" t="s">
+        <v>21</v>
+      </c>
+      <c r="F26" t="s">
+        <v>105</v>
+      </c>
+      <c r="G26" t="s">
+        <v>420</v>
+      </c>
+      <c r="H26" s="29" t="s">
+        <v>181</v>
+      </c>
+      <c r="I26" s="20" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="27" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C27" s="45" t="s">
+        <v>331</v>
+      </c>
+      <c r="D27" t="s">
+        <v>332</v>
+      </c>
+      <c r="E27" t="s">
+        <v>21</v>
+      </c>
+      <c r="F27" t="s">
+        <v>333</v>
+      </c>
+      <c r="G27" t="s">
+        <v>334</v>
+      </c>
+      <c r="H27" s="29" t="s">
+        <v>335</v>
+      </c>
+      <c r="I27" s="20" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="28" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C28" s="45" t="s">
+        <v>164</v>
+      </c>
+      <c r="D28" t="s">
+        <v>165</v>
+      </c>
+      <c r="E28" t="s">
+        <v>21</v>
+      </c>
+      <c r="F28" t="s">
+        <v>166</v>
+      </c>
+      <c r="G28" t="s">
+        <v>420</v>
+      </c>
+      <c r="H28" s="29" t="s">
+        <v>205</v>
+      </c>
+      <c r="I28" s="20" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="29" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C29" s="45" t="s">
+        <v>22</v>
+      </c>
+      <c r="D29" t="s">
+        <v>34</v>
+      </c>
+      <c r="E29" t="s">
+        <v>21</v>
+      </c>
+      <c r="F29" t="s">
+        <v>117</v>
+      </c>
+      <c r="G29" t="s">
+        <v>289</v>
+      </c>
+      <c r="H29" s="29" t="s">
+        <v>182</v>
+      </c>
+      <c r="I29" s="20" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="30" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C30" s="45" t="s">
+        <v>167</v>
+      </c>
+      <c r="D30" t="s">
+        <v>170</v>
+      </c>
+      <c r="E30" t="s">
+        <v>169</v>
+      </c>
+      <c r="F30" t="s">
+        <v>168</v>
+      </c>
+      <c r="G30" t="s">
+        <v>287</v>
+      </c>
+      <c r="H30" s="29" t="s">
+        <v>185</v>
+      </c>
+      <c r="I30" s="20" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="31" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C31" s="45" t="s">
+        <v>25</v>
+      </c>
+      <c r="D31" t="s">
+        <v>171</v>
+      </c>
+      <c r="E31" t="s">
+        <v>25</v>
+      </c>
+      <c r="F31" t="s">
+        <v>41</v>
+      </c>
+      <c r="G31" t="s">
+        <v>418</v>
+      </c>
+      <c r="H31" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="I31" s="20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="32" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C32" s="45" t="s">
+        <v>173</v>
+      </c>
+      <c r="D32" t="s">
+        <v>174</v>
+      </c>
+      <c r="E32" t="s">
+        <v>173</v>
+      </c>
+      <c r="F32" t="s">
+        <v>172</v>
+      </c>
+      <c r="G32" s="5" t="s">
+        <v>419</v>
+      </c>
+      <c r="H32" s="29" t="s">
+        <v>183</v>
+      </c>
+      <c r="I32" s="20" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C33" s="33" t="s">
+        <v>283</v>
+      </c>
+      <c r="D33" t="s">
+        <v>284</v>
+      </c>
+      <c r="E33" t="s">
+        <v>25</v>
+      </c>
+      <c r="F33" t="s">
+        <v>285</v>
+      </c>
+      <c r="G33" s="20" t="s">
+        <v>418</v>
+      </c>
+      <c r="H33" s="29" t="s">
+        <v>286</v>
+      </c>
+      <c r="I33" s="20" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C34" s="45" t="s">
+        <v>294</v>
+      </c>
+      <c r="D34" t="s">
+        <v>295</v>
+      </c>
+      <c r="E34" t="s">
+        <v>25</v>
+      </c>
+      <c r="F34" t="s">
+        <v>251</v>
+      </c>
+      <c r="G34" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="H34" s="29" t="s">
+        <v>254</v>
+      </c>
+      <c r="I34" s="20" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B37" s="26" t="s">
+        <v>101</v>
+      </c>
+      <c r="C37" s="27"/>
+      <c r="D37" s="27"/>
+      <c r="E37" s="27"/>
+      <c r="F37" s="27"/>
+      <c r="G37" s="27"/>
+      <c r="H37" s="28"/>
+    </row>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C38" s="34" t="s">
+        <v>102</v>
+      </c>
+      <c r="D38" s="31" t="s">
+        <v>103</v>
+      </c>
+      <c r="E38" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="F38" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="G38" s="39"/>
+      <c r="H38" s="39"/>
+    </row>
+    <row r="39" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C39" s="53">
+        <v>1</v>
+      </c>
+      <c r="D39" t="s">
+        <v>455</v>
+      </c>
+      <c r="E39" t="s">
+        <v>405</v>
+      </c>
+      <c r="F39" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C40" s="53">
+        <v>2</v>
+      </c>
+      <c r="D40" t="s">
+        <v>456</v>
+      </c>
+      <c r="E40" t="s">
+        <v>404</v>
+      </c>
+      <c r="F40" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="41" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C41" s="53">
+        <v>3</v>
+      </c>
+      <c r="D41" t="s">
+        <v>450</v>
+      </c>
+      <c r="E41" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="42" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C42" s="53">
+        <v>4</v>
+      </c>
+      <c r="D42" t="s">
+        <v>452</v>
+      </c>
+      <c r="E42" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="43" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C43" s="53">
+        <v>5</v>
+      </c>
+      <c r="D43" t="s">
+        <v>451</v>
+      </c>
+      <c r="E43" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="44" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C44" s="53">
+        <v>6</v>
+      </c>
+      <c r="D44" t="s">
+        <v>453</v>
+      </c>
+      <c r="E44" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="45" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C45" s="53">
+        <v>7</v>
+      </c>
+      <c r="D45" t="s">
+        <v>407</v>
+      </c>
+      <c r="E45" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="46" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C46" s="53">
+        <v>8</v>
+      </c>
+      <c r="D46" t="s">
+        <v>408</v>
+      </c>
+      <c r="E46" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="47" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C47" s="53">
+        <v>9</v>
+      </c>
+      <c r="D47" t="s">
+        <v>409</v>
+      </c>
+      <c r="E47" t="s">
+        <v>405</v>
+      </c>
+      <c r="F47" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="48" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C48" s="53">
+        <v>10</v>
+      </c>
+      <c r="D48" t="s">
+        <v>410</v>
+      </c>
+      <c r="E48" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C49" s="53">
+        <v>11</v>
+      </c>
+      <c r="D49" t="s">
+        <v>411</v>
+      </c>
+      <c r="E49" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C50" s="53">
+        <v>12</v>
+      </c>
+      <c r="D50" t="s">
+        <v>412</v>
+      </c>
+      <c r="E50" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C51" s="53">
+        <v>13</v>
+      </c>
+      <c r="D51" t="s">
+        <v>415</v>
+      </c>
+      <c r="E51" t="s">
+        <v>405</v>
+      </c>
+      <c r="F51" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C52" s="53">
+        <v>14</v>
+      </c>
+      <c r="D52" t="s">
+        <v>416</v>
+      </c>
+      <c r="E52" t="s">
+        <v>404</v>
+      </c>
+      <c r="F52" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C53" s="5"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B55" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="C55" s="27"/>
+      <c r="D55" s="27"/>
+      <c r="E55" s="27"/>
+      <c r="F55" s="27"/>
+      <c r="G55" s="27"/>
+      <c r="H55" s="28"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C56" s="34" t="s">
+        <v>58</v>
+      </c>
+      <c r="D56" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="E56" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="F56" s="31" t="s">
+        <v>59</v>
+      </c>
+      <c r="G56" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="H56" s="31" t="s">
+        <v>60</v>
+      </c>
+      <c r="I56" s="51" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>0</v>
+      </c>
+      <c r="C57" s="35" t="s">
+        <v>292</v>
+      </c>
+      <c r="D57" t="s">
+        <v>293</v>
+      </c>
+      <c r="E57" s="20" t="s">
+        <v>291</v>
+      </c>
+      <c r="F57" s="24" t="s">
+        <v>263</v>
+      </c>
+      <c r="G57" t="s">
+        <v>239</v>
+      </c>
+      <c r="H57" t="s">
+        <v>61</v>
+      </c>
+      <c r="I57" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>1</v>
+      </c>
+      <c r="C58" s="35" t="s">
+        <v>300</v>
+      </c>
+      <c r="D58" t="s">
+        <v>301</v>
+      </c>
+      <c r="E58" s="20" t="s">
+        <v>299</v>
+      </c>
+      <c r="F58" s="46" t="s">
+        <v>303</v>
+      </c>
+      <c r="G58" s="20" t="s">
+        <v>239</v>
+      </c>
+      <c r="H58" t="s">
+        <v>61</v>
+      </c>
+      <c r="I58" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>2</v>
+      </c>
+      <c r="C59" s="35" t="s">
+        <v>305</v>
+      </c>
+      <c r="D59" t="s">
+        <v>306</v>
+      </c>
+      <c r="E59" s="20" t="s">
+        <v>304</v>
+      </c>
+      <c r="F59" s="46" t="s">
+        <v>308</v>
+      </c>
+      <c r="G59" s="20" t="s">
+        <v>239</v>
+      </c>
+      <c r="H59" t="s">
+        <v>61</v>
+      </c>
+      <c r="I59" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>3</v>
+      </c>
+      <c r="C60" s="35" t="s">
+        <v>315</v>
+      </c>
+      <c r="D60" s="20" t="s">
+        <v>317</v>
+      </c>
+      <c r="E60" t="s">
+        <v>313</v>
+      </c>
+      <c r="F60" s="46" t="s">
+        <v>432</v>
+      </c>
+      <c r="G60" s="20" t="s">
+        <v>321</v>
+      </c>
+      <c r="H60" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="I60" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>4</v>
+      </c>
+      <c r="C61" s="35" t="s">
+        <v>316</v>
+      </c>
+      <c r="D61" s="20" t="s">
+        <v>318</v>
+      </c>
+      <c r="E61" t="s">
+        <v>314</v>
+      </c>
+      <c r="F61" s="24" t="s">
+        <v>320</v>
+      </c>
+      <c r="G61" s="20" t="s">
+        <v>239</v>
+      </c>
+      <c r="H61" t="s">
+        <v>61</v>
+      </c>
+      <c r="I61" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>5</v>
+      </c>
+      <c r="C62" s="35" t="s">
+        <v>329</v>
+      </c>
+      <c r="D62" s="20" t="s">
+        <v>325</v>
+      </c>
+      <c r="E62" t="s">
+        <v>323</v>
+      </c>
+      <c r="F62" s="24" t="s">
+        <v>275</v>
+      </c>
+      <c r="G62" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="H62" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="I62" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>6</v>
+      </c>
+      <c r="C63" s="35" t="s">
+        <v>330</v>
+      </c>
+      <c r="D63" s="20" t="s">
+        <v>328</v>
+      </c>
+      <c r="E63" t="s">
+        <v>326</v>
+      </c>
+      <c r="F63" s="24" t="s">
+        <v>339</v>
+      </c>
+      <c r="G63" s="20" t="s">
+        <v>321</v>
+      </c>
+      <c r="H63" t="s">
+        <v>61</v>
+      </c>
+      <c r="I63" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <v>7</v>
+      </c>
+      <c r="C64" s="35" t="s">
+        <v>343</v>
+      </c>
+      <c r="D64" s="20" t="s">
+        <v>342</v>
+      </c>
+      <c r="E64" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="F64" s="24" t="s">
+        <v>339</v>
+      </c>
+      <c r="G64" s="20" t="s">
+        <v>321</v>
+      </c>
+      <c r="H64" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="I64" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>8</v>
+      </c>
+      <c r="C65" s="35" t="s">
+        <v>442</v>
+      </c>
+      <c r="D65" s="20" t="s">
+        <v>440</v>
+      </c>
+      <c r="E65" s="5" t="s">
+        <v>444</v>
+      </c>
+      <c r="F65" s="24" t="s">
+        <v>448</v>
+      </c>
+      <c r="G65" s="20" t="s">
+        <v>126</v>
+      </c>
+      <c r="H65" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="I65" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <v>9</v>
+      </c>
+      <c r="C66" s="35" t="s">
+        <v>443</v>
+      </c>
+      <c r="D66" s="20" t="s">
+        <v>441</v>
+      </c>
+      <c r="E66" s="5" t="s">
+        <v>445</v>
+      </c>
+      <c r="F66" s="24" t="s">
+        <v>448</v>
+      </c>
+      <c r="G66" s="20" t="s">
+        <v>126</v>
+      </c>
+      <c r="H66" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="I66" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A67">
+        <v>10</v>
+      </c>
+      <c r="C67" s="35" t="s">
+        <v>345</v>
+      </c>
+      <c r="D67" s="20" t="s">
+        <v>346</v>
+      </c>
+      <c r="E67" s="5" t="s">
+        <v>344</v>
+      </c>
+      <c r="F67" s="24" t="s">
+        <v>348</v>
+      </c>
+      <c r="G67" s="20" t="s">
+        <v>239</v>
+      </c>
+      <c r="H67" t="s">
+        <v>61</v>
+      </c>
+      <c r="I67" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A68">
+        <v>11</v>
+      </c>
+      <c r="C68" s="35" t="s">
+        <v>351</v>
+      </c>
+      <c r="D68" s="20" t="s">
+        <v>350</v>
+      </c>
+      <c r="E68" t="s">
+        <v>349</v>
+      </c>
+      <c r="F68" s="24" t="s">
+        <v>348</v>
+      </c>
+      <c r="G68" s="20" t="s">
+        <v>239</v>
+      </c>
+      <c r="H68" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="I68" s="36" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A69">
+        <v>12</v>
+      </c>
+      <c r="C69" s="35" t="s">
+        <v>359</v>
+      </c>
+      <c r="D69" s="20" t="s">
+        <v>356</v>
+      </c>
+      <c r="E69" t="s">
+        <v>353</v>
+      </c>
+      <c r="F69" s="24" t="s">
+        <v>354</v>
+      </c>
+      <c r="G69" s="20" t="s">
+        <v>239</v>
+      </c>
+      <c r="H69" t="s">
+        <v>61</v>
+      </c>
+      <c r="I69" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A70">
+        <v>13</v>
+      </c>
+      <c r="C70" s="35" t="s">
+        <v>360</v>
+      </c>
+      <c r="D70" s="20" t="s">
+        <v>401</v>
+      </c>
+      <c r="E70" s="5" t="s">
+        <v>357</v>
+      </c>
+      <c r="F70" s="46" t="s">
+        <v>421</v>
+      </c>
+      <c r="G70" s="20" t="s">
+        <v>239</v>
+      </c>
+      <c r="H70" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="I70" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A71">
+        <v>14</v>
+      </c>
+      <c r="C71" s="35" t="s">
+        <v>400</v>
+      </c>
+      <c r="D71" s="20" t="s">
+        <v>402</v>
+      </c>
+      <c r="E71" s="5" t="s">
+        <v>422</v>
+      </c>
+      <c r="F71" s="46" t="s">
+        <v>403</v>
+      </c>
+      <c r="G71" s="20" t="s">
+        <v>239</v>
+      </c>
+      <c r="H71" t="s">
+        <v>61</v>
+      </c>
+      <c r="I71" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A72">
+        <v>15</v>
+      </c>
+      <c r="C72" s="35" t="s">
+        <v>361</v>
+      </c>
+      <c r="D72" s="20" t="s">
+        <v>363</v>
+      </c>
+      <c r="E72" t="s">
+        <v>358</v>
+      </c>
+      <c r="F72" s="24" t="s">
+        <v>364</v>
+      </c>
+      <c r="G72" s="20" t="s">
+        <v>239</v>
+      </c>
+      <c r="H72" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="I72" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A73">
+        <v>16</v>
+      </c>
+      <c r="C73" s="35" t="s">
+        <v>366</v>
+      </c>
+      <c r="D73" s="20" t="s">
+        <v>367</v>
+      </c>
+      <c r="E73" t="s">
+        <v>365</v>
+      </c>
+      <c r="F73" s="24" t="s">
+        <v>430</v>
+      </c>
+      <c r="G73" s="20" t="s">
+        <v>376</v>
+      </c>
+      <c r="H73" t="s">
+        <v>61</v>
+      </c>
+      <c r="I73" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A74">
+        <v>17</v>
+      </c>
+      <c r="C74" s="35" t="s">
+        <v>370</v>
+      </c>
+      <c r="D74" s="20" t="s">
+        <v>371</v>
+      </c>
+      <c r="E74" t="s">
+        <v>369</v>
+      </c>
+      <c r="F74" s="24" t="s">
+        <v>375</v>
+      </c>
+      <c r="G74" s="20" t="s">
+        <v>376</v>
+      </c>
+      <c r="H74" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="I74" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A75">
+        <v>18</v>
+      </c>
+      <c r="C75" s="35" t="s">
+        <v>383</v>
+      </c>
+      <c r="D75" s="20" t="s">
+        <v>380</v>
+      </c>
+      <c r="E75" t="s">
+        <v>377</v>
+      </c>
+      <c r="F75" s="24" t="s">
+        <v>364</v>
+      </c>
+      <c r="G75" s="20" t="s">
+        <v>239</v>
+      </c>
+      <c r="H75" t="s">
+        <v>61</v>
+      </c>
+      <c r="I75" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A76">
+        <v>19</v>
+      </c>
+      <c r="C76" s="35" t="s">
+        <v>384</v>
+      </c>
+      <c r="D76" s="20" t="s">
+        <v>381</v>
+      </c>
+      <c r="E76" t="s">
+        <v>379</v>
+      </c>
+      <c r="F76" s="24" t="s">
+        <v>232</v>
+      </c>
+      <c r="G76" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="H76" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="I76" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A77">
+        <v>20</v>
+      </c>
+      <c r="C77" s="35" t="s">
+        <v>388</v>
+      </c>
+      <c r="D77" s="20" t="s">
+        <v>387</v>
+      </c>
+      <c r="E77" t="s">
+        <v>386</v>
+      </c>
+      <c r="F77" s="24" t="s">
+        <v>232</v>
+      </c>
+      <c r="G77" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="H77" t="s">
+        <v>61</v>
+      </c>
+      <c r="I77" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A78">
+        <v>21</v>
+      </c>
+      <c r="C78" s="35" t="s">
+        <v>390</v>
+      </c>
+      <c r="D78" s="20" t="s">
+        <v>391</v>
+      </c>
+      <c r="E78" t="s">
+        <v>389</v>
+      </c>
+      <c r="F78" s="24" t="s">
+        <v>232</v>
+      </c>
+      <c r="G78" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="H78" t="s">
+        <v>61</v>
+      </c>
+      <c r="I78" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A79">
+        <v>22</v>
+      </c>
+      <c r="C79" s="35" t="s">
+        <v>395</v>
+      </c>
+      <c r="D79" s="20" t="s">
+        <v>393</v>
+      </c>
+      <c r="E79" t="s">
+        <v>394</v>
+      </c>
+      <c r="F79" s="24" t="s">
+        <v>396</v>
+      </c>
+      <c r="G79" s="20" t="s">
+        <v>239</v>
+      </c>
+      <c r="H79" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="I79" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A80">
+        <v>23</v>
+      </c>
+      <c r="C80" s="35" t="s">
+        <v>398</v>
+      </c>
+      <c r="D80" s="20" t="s">
+        <v>399</v>
+      </c>
+      <c r="E80" t="s">
+        <v>397</v>
+      </c>
+      <c r="F80" s="24" t="s">
+        <v>232</v>
+      </c>
+      <c r="G80" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="H80" t="s">
+        <v>61</v>
+      </c>
+      <c r="I80" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A81">
+        <v>24</v>
+      </c>
+      <c r="C81" s="35" t="s">
+        <v>433</v>
+      </c>
+      <c r="D81" s="20" t="s">
+        <v>434</v>
+      </c>
+      <c r="E81" s="5" t="s">
+        <v>435</v>
+      </c>
+      <c r="F81" s="24" t="s">
+        <v>436</v>
+      </c>
+      <c r="G81" s="20" t="s">
+        <v>126</v>
+      </c>
+      <c r="H81" t="s">
+        <v>61</v>
+      </c>
+      <c r="I81" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C82" s="5"/>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B83" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="C83" s="27"/>
+      <c r="D83" s="27"/>
+      <c r="E83" s="27"/>
+      <c r="F83" s="27"/>
+      <c r="G83" s="27"/>
+      <c r="H83" s="28"/>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C84" s="24" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C85" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="D85" s="42" t="s">
+        <v>84</v>
+      </c>
+      <c r="E85" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C86" t="s">
+        <v>423</v>
+      </c>
+      <c r="D86" s="42" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C87" t="s">
+        <v>424</v>
+      </c>
+      <c r="D87" s="47" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C88" t="s">
+        <v>425</v>
+      </c>
+      <c r="D88" s="47" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C89" t="s">
+        <v>426</v>
+      </c>
+      <c r="D89" s="47" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C90" t="s">
+        <v>427</v>
+      </c>
+      <c r="D90" s="47" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C91" t="s">
+        <v>428</v>
+      </c>
+      <c r="D91" s="47" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B93" s="26" t="s">
+        <v>104</v>
+      </c>
+      <c r="C93" s="27"/>
+      <c r="D93" s="27"/>
+      <c r="E93" s="27"/>
+      <c r="F93" s="27"/>
+      <c r="G93" s="27"/>
+      <c r="H93" s="28"/>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C94" s="24" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C95" t="s">
+        <v>277</v>
+      </c>
+      <c r="D95" s="42" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C96" t="s">
+        <v>278</v>
+      </c>
+      <c r="D96" s="42" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="97" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C97" t="s">
+        <v>279</v>
+      </c>
+      <c r="D97" s="42" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="98" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C98" s="5"/>
+      <c r="D98" s="5"/>
+    </row>
+    <row r="99" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C99" s="5"/>
+      <c r="D99" s="5"/>
+    </row>
+    <row r="100" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B100" s="26" t="s">
+        <v>417</v>
+      </c>
+      <c r="C100" s="27"/>
+      <c r="D100" s="27"/>
+      <c r="E100" s="27"/>
+      <c r="F100" s="27"/>
+      <c r="G100" s="27"/>
+      <c r="H100" s="28"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:K87"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="E4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30:I30"/>
+    <sheetView showGridLines="0" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2821,11 +5042,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:K52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
@@ -2950,7 +5171,7 @@
       <c r="C11" t="s">
         <v>267</v>
       </c>
-      <c r="D11" s="51" t="s">
+      <c r="D11" s="50" t="s">
         <v>266</v>
       </c>
       <c r="I11" s="20"/>
@@ -2961,7 +5182,7 @@
       <c r="C12" t="s">
         <v>268</v>
       </c>
-      <c r="D12" s="51" t="s">
+      <c r="D12" s="50" t="s">
         <v>266</v>
       </c>
       <c r="I12" s="20"/>
@@ -3460,12 +5681,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:K69"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Created TestCase USA V2 for use with proper data.
</commit_message>
<xml_diff>
--- a/RECC_Config.xlsx
+++ b/RECC_Config.xlsx
@@ -9,21 +9,22 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="8652" windowHeight="4896" tabRatio="844" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8652" windowHeight="4896" tabRatio="844"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="5" r:id="rId1"/>
     <sheet name="RECC_USA_TestCase_V1.0" sheetId="9" r:id="rId2"/>
-    <sheet name="RECC_Main_Development_1" sheetId="7" r:id="rId3"/>
-    <sheet name="GDP_Test" sheetId="8" r:id="rId4"/>
-    <sheet name="Setting_TestRun_1" sheetId="6" r:id="rId5"/>
+    <sheet name="RECC_USA_TestCase_V2.0" sheetId="10" r:id="rId3"/>
+    <sheet name="RECC_Main_Development_1" sheetId="7" r:id="rId4"/>
+    <sheet name="GDP_Test" sheetId="8" r:id="rId5"/>
+    <sheet name="Setting_TestRun_1" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1010" uniqueCount="458">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1417" uniqueCount="460">
   <si>
     <t>Description</t>
   </si>
@@ -1397,6 +1398,12 @@
   </si>
   <si>
     <t>[21:42)</t>
+  </si>
+  <si>
+    <t>USA_TestCase_V2.0</t>
+  </si>
+  <si>
+    <t>RECC_USA_TestCase_V2.0</t>
   </si>
 </sst>
 </file>
@@ -1984,8 +1991,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2028,7 +2035,7 @@
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="6" t="s">
-        <v>311</v>
+        <v>459</v>
       </c>
       <c r="G4" s="48"/>
     </row>
@@ -2181,8 +2188,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:K100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView topLeftCell="A52" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A52" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3843,6 +3850,1670 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:K100"/>
+  <sheetViews>
+    <sheetView topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="17.77734375" customWidth="1"/>
+    <col min="3" max="3" width="41.88671875" customWidth="1"/>
+    <col min="4" max="4" width="65.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="50.6640625" customWidth="1"/>
+    <col min="6" max="6" width="27.44140625" customWidth="1"/>
+    <col min="7" max="7" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="43.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B2" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="28"/>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C3" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" s="41" t="s">
+        <v>56</v>
+      </c>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="42" t="s">
+        <v>458</v>
+      </c>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="20"/>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="42" t="s">
+        <v>282</v>
+      </c>
+      <c r="I5" s="20"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="20"/>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="43" t="s">
+        <v>459</v>
+      </c>
+      <c r="I6" s="20"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="20"/>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="D7" s="11"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="20"/>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B8" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="28"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="20"/>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C9" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="D9" s="41" t="s">
+        <v>207</v>
+      </c>
+      <c r="E9" s="31"/>
+      <c r="F9" s="39"/>
+      <c r="G9" s="39"/>
+      <c r="H9" s="39"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="19"/>
+      <c r="K9" s="20"/>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="42" t="s">
+        <v>309</v>
+      </c>
+      <c r="I10" s="20"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="20"/>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C11" t="s">
+        <v>267</v>
+      </c>
+      <c r="D11" s="50" t="s">
+        <v>312</v>
+      </c>
+      <c r="I11" s="20"/>
+      <c r="J11" s="19"/>
+      <c r="K11" s="20"/>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C12" t="s">
+        <v>268</v>
+      </c>
+      <c r="D12" s="50" t="s">
+        <v>312</v>
+      </c>
+      <c r="I12" s="20"/>
+      <c r="J12" s="19"/>
+      <c r="K12" s="20"/>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="I13" s="20"/>
+      <c r="J13" s="25"/>
+      <c r="K13" s="20"/>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B14" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="C14" s="27"/>
+      <c r="D14" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="E14" s="27"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="27"/>
+      <c r="H14" s="28"/>
+      <c r="I14" s="36" t="s">
+        <v>439</v>
+      </c>
+      <c r="J14" s="20"/>
+      <c r="K14" s="20"/>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C15" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="E15" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15" s="31" t="s">
+        <v>438</v>
+      </c>
+      <c r="H15" s="30" t="s">
+        <v>186</v>
+      </c>
+      <c r="I15" s="52" t="s">
+        <v>187</v>
+      </c>
+      <c r="K15" s="20"/>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C16" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" t="s">
+        <v>28</v>
+      </c>
+      <c r="E16" t="s">
+        <v>16</v>
+      </c>
+      <c r="F16" t="s">
+        <v>16</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="H16" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="I16" s="20" t="s">
+        <v>188</v>
+      </c>
+      <c r="J16" s="20"/>
+      <c r="K16" s="20"/>
+    </row>
+    <row r="17" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C17" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" t="s">
+        <v>29</v>
+      </c>
+      <c r="E17" t="s">
+        <v>16</v>
+      </c>
+      <c r="F17" t="s">
+        <v>16</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>429</v>
+      </c>
+      <c r="H17" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="I17" s="20" t="s">
+        <v>189</v>
+      </c>
+      <c r="J17" s="20"/>
+      <c r="K17" s="20"/>
+    </row>
+    <row r="18" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C18" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" t="s">
+        <v>37</v>
+      </c>
+      <c r="E18" t="s">
+        <v>23</v>
+      </c>
+      <c r="F18" t="s">
+        <v>42</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>449</v>
+      </c>
+      <c r="H18" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="I18" s="20" t="s">
+        <v>190</v>
+      </c>
+      <c r="J18" s="20"/>
+      <c r="K18" s="20"/>
+    </row>
+    <row r="19" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C19" s="33" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" t="s">
+        <v>38</v>
+      </c>
+      <c r="E19" t="s">
+        <v>24</v>
+      </c>
+      <c r="F19" t="s">
+        <v>24</v>
+      </c>
+      <c r="G19" t="s">
+        <v>418</v>
+      </c>
+      <c r="H19" s="29">
+        <v>1</v>
+      </c>
+      <c r="I19" s="20" t="s">
+        <v>192</v>
+      </c>
+      <c r="J19" s="20"/>
+      <c r="K19" s="20"/>
+    </row>
+    <row r="20" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C20" s="33" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" t="s">
+        <v>31</v>
+      </c>
+      <c r="E20" t="s">
+        <v>39</v>
+      </c>
+      <c r="F20" t="s">
+        <v>40</v>
+      </c>
+      <c r="G20" t="s">
+        <v>276</v>
+      </c>
+      <c r="H20" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="I20" s="20" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="21" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C21" s="45" t="s">
+        <v>142</v>
+      </c>
+      <c r="D21" t="s">
+        <v>150</v>
+      </c>
+      <c r="E21" t="s">
+        <v>26</v>
+      </c>
+      <c r="F21" t="s">
+        <v>155</v>
+      </c>
+      <c r="G21" t="s">
+        <v>457</v>
+      </c>
+      <c r="H21" s="29" t="s">
+        <v>184</v>
+      </c>
+      <c r="I21" s="20" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="22" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C22" s="45" t="s">
+        <v>143</v>
+      </c>
+      <c r="D22" t="s">
+        <v>151</v>
+      </c>
+      <c r="E22" t="s">
+        <v>26</v>
+      </c>
+      <c r="F22" t="s">
+        <v>156</v>
+      </c>
+      <c r="G22" t="s">
+        <v>420</v>
+      </c>
+      <c r="H22" s="29" t="s">
+        <v>179</v>
+      </c>
+      <c r="I22" s="20" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="23" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C23" s="45" t="s">
+        <v>144</v>
+      </c>
+      <c r="D23" t="s">
+        <v>152</v>
+      </c>
+      <c r="E23" t="s">
+        <v>26</v>
+      </c>
+      <c r="F23" t="s">
+        <v>157</v>
+      </c>
+      <c r="G23" t="s">
+        <v>420</v>
+      </c>
+      <c r="H23" s="29" t="s">
+        <v>178</v>
+      </c>
+      <c r="I23" s="20" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C24" s="45" t="s">
+        <v>145</v>
+      </c>
+      <c r="D24" t="s">
+        <v>148</v>
+      </c>
+      <c r="E24" t="s">
+        <v>26</v>
+      </c>
+      <c r="F24" t="s">
+        <v>106</v>
+      </c>
+      <c r="G24" t="s">
+        <v>290</v>
+      </c>
+      <c r="H24" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="I24" s="20" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="25" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C25" s="45" t="s">
+        <v>163</v>
+      </c>
+      <c r="D25" t="s">
+        <v>159</v>
+      </c>
+      <c r="E25" t="s">
+        <v>21</v>
+      </c>
+      <c r="F25" t="s">
+        <v>134</v>
+      </c>
+      <c r="G25" t="s">
+        <v>454</v>
+      </c>
+      <c r="H25" s="29" t="s">
+        <v>337</v>
+      </c>
+      <c r="I25" s="20" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="26" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C26" s="45" t="s">
+        <v>20</v>
+      </c>
+      <c r="D26" t="s">
+        <v>32</v>
+      </c>
+      <c r="E26" t="s">
+        <v>21</v>
+      </c>
+      <c r="F26" t="s">
+        <v>105</v>
+      </c>
+      <c r="G26" t="s">
+        <v>420</v>
+      </c>
+      <c r="H26" s="29" t="s">
+        <v>181</v>
+      </c>
+      <c r="I26" s="20" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="27" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C27" s="45" t="s">
+        <v>331</v>
+      </c>
+      <c r="D27" t="s">
+        <v>332</v>
+      </c>
+      <c r="E27" t="s">
+        <v>21</v>
+      </c>
+      <c r="F27" t="s">
+        <v>333</v>
+      </c>
+      <c r="G27" t="s">
+        <v>334</v>
+      </c>
+      <c r="H27" s="29" t="s">
+        <v>335</v>
+      </c>
+      <c r="I27" s="20" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="28" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C28" s="45" t="s">
+        <v>164</v>
+      </c>
+      <c r="D28" t="s">
+        <v>165</v>
+      </c>
+      <c r="E28" t="s">
+        <v>21</v>
+      </c>
+      <c r="F28" t="s">
+        <v>166</v>
+      </c>
+      <c r="G28" t="s">
+        <v>420</v>
+      </c>
+      <c r="H28" s="29" t="s">
+        <v>205</v>
+      </c>
+      <c r="I28" s="20" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="29" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C29" s="45" t="s">
+        <v>22</v>
+      </c>
+      <c r="D29" t="s">
+        <v>34</v>
+      </c>
+      <c r="E29" t="s">
+        <v>21</v>
+      </c>
+      <c r="F29" t="s">
+        <v>117</v>
+      </c>
+      <c r="G29" t="s">
+        <v>289</v>
+      </c>
+      <c r="H29" s="29" t="s">
+        <v>182</v>
+      </c>
+      <c r="I29" s="20" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="30" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C30" s="45" t="s">
+        <v>167</v>
+      </c>
+      <c r="D30" t="s">
+        <v>170</v>
+      </c>
+      <c r="E30" t="s">
+        <v>169</v>
+      </c>
+      <c r="F30" t="s">
+        <v>168</v>
+      </c>
+      <c r="G30" t="s">
+        <v>287</v>
+      </c>
+      <c r="H30" s="29" t="s">
+        <v>185</v>
+      </c>
+      <c r="I30" s="20" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="31" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C31" s="45" t="s">
+        <v>25</v>
+      </c>
+      <c r="D31" t="s">
+        <v>171</v>
+      </c>
+      <c r="E31" t="s">
+        <v>25</v>
+      </c>
+      <c r="F31" t="s">
+        <v>41</v>
+      </c>
+      <c r="G31" t="s">
+        <v>418</v>
+      </c>
+      <c r="H31" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="I31" s="20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="32" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C32" s="45" t="s">
+        <v>173</v>
+      </c>
+      <c r="D32" t="s">
+        <v>174</v>
+      </c>
+      <c r="E32" t="s">
+        <v>173</v>
+      </c>
+      <c r="F32" t="s">
+        <v>172</v>
+      </c>
+      <c r="G32" s="5" t="s">
+        <v>419</v>
+      </c>
+      <c r="H32" s="29" t="s">
+        <v>183</v>
+      </c>
+      <c r="I32" s="20" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C33" s="33" t="s">
+        <v>283</v>
+      </c>
+      <c r="D33" t="s">
+        <v>284</v>
+      </c>
+      <c r="E33" t="s">
+        <v>25</v>
+      </c>
+      <c r="F33" t="s">
+        <v>285</v>
+      </c>
+      <c r="G33" s="20" t="s">
+        <v>418</v>
+      </c>
+      <c r="H33" s="29" t="s">
+        <v>286</v>
+      </c>
+      <c r="I33" s="20" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C34" s="45" t="s">
+        <v>294</v>
+      </c>
+      <c r="D34" t="s">
+        <v>295</v>
+      </c>
+      <c r="E34" t="s">
+        <v>25</v>
+      </c>
+      <c r="F34" t="s">
+        <v>251</v>
+      </c>
+      <c r="G34" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="H34" s="29" t="s">
+        <v>254</v>
+      </c>
+      <c r="I34" s="20" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B37" s="26" t="s">
+        <v>101</v>
+      </c>
+      <c r="C37" s="27"/>
+      <c r="D37" s="27"/>
+      <c r="E37" s="27"/>
+      <c r="F37" s="27"/>
+      <c r="G37" s="27"/>
+      <c r="H37" s="28"/>
+    </row>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C38" s="34" t="s">
+        <v>102</v>
+      </c>
+      <c r="D38" s="31" t="s">
+        <v>103</v>
+      </c>
+      <c r="E38" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="F38" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="G38" s="39"/>
+      <c r="H38" s="39"/>
+    </row>
+    <row r="39" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C39" s="53">
+        <v>1</v>
+      </c>
+      <c r="D39" t="s">
+        <v>455</v>
+      </c>
+      <c r="E39" t="s">
+        <v>405</v>
+      </c>
+      <c r="F39" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C40" s="53">
+        <v>2</v>
+      </c>
+      <c r="D40" t="s">
+        <v>456</v>
+      </c>
+      <c r="E40" t="s">
+        <v>404</v>
+      </c>
+      <c r="F40" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="41" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C41" s="53">
+        <v>3</v>
+      </c>
+      <c r="D41" t="s">
+        <v>450</v>
+      </c>
+      <c r="E41" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="42" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C42" s="53">
+        <v>4</v>
+      </c>
+      <c r="D42" t="s">
+        <v>452</v>
+      </c>
+      <c r="E42" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="43" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C43" s="53">
+        <v>5</v>
+      </c>
+      <c r="D43" t="s">
+        <v>451</v>
+      </c>
+      <c r="E43" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="44" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C44" s="53">
+        <v>6</v>
+      </c>
+      <c r="D44" t="s">
+        <v>453</v>
+      </c>
+      <c r="E44" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="45" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C45" s="53">
+        <v>7</v>
+      </c>
+      <c r="D45" t="s">
+        <v>407</v>
+      </c>
+      <c r="E45" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="46" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C46" s="53">
+        <v>8</v>
+      </c>
+      <c r="D46" t="s">
+        <v>408</v>
+      </c>
+      <c r="E46" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="47" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C47" s="53">
+        <v>9</v>
+      </c>
+      <c r="D47" t="s">
+        <v>409</v>
+      </c>
+      <c r="E47" t="s">
+        <v>405</v>
+      </c>
+      <c r="F47" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="48" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C48" s="53">
+        <v>10</v>
+      </c>
+      <c r="D48" t="s">
+        <v>410</v>
+      </c>
+      <c r="E48" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C49" s="53">
+        <v>11</v>
+      </c>
+      <c r="D49" t="s">
+        <v>411</v>
+      </c>
+      <c r="E49" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C50" s="53">
+        <v>12</v>
+      </c>
+      <c r="D50" t="s">
+        <v>412</v>
+      </c>
+      <c r="E50" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C51" s="53">
+        <v>13</v>
+      </c>
+      <c r="D51" t="s">
+        <v>415</v>
+      </c>
+      <c r="E51" t="s">
+        <v>405</v>
+      </c>
+      <c r="F51" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C52" s="53">
+        <v>14</v>
+      </c>
+      <c r="D52" t="s">
+        <v>416</v>
+      </c>
+      <c r="E52" t="s">
+        <v>404</v>
+      </c>
+      <c r="F52" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C53" s="5"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B55" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="C55" s="27"/>
+      <c r="D55" s="27"/>
+      <c r="E55" s="27"/>
+      <c r="F55" s="27"/>
+      <c r="G55" s="27"/>
+      <c r="H55" s="28"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C56" s="34" t="s">
+        <v>58</v>
+      </c>
+      <c r="D56" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="E56" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="F56" s="31" t="s">
+        <v>59</v>
+      </c>
+      <c r="G56" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="H56" s="31" t="s">
+        <v>60</v>
+      </c>
+      <c r="I56" s="51" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>0</v>
+      </c>
+      <c r="C57" s="35" t="s">
+        <v>292</v>
+      </c>
+      <c r="D57" t="s">
+        <v>293</v>
+      </c>
+      <c r="E57" s="20" t="s">
+        <v>291</v>
+      </c>
+      <c r="F57" s="24" t="s">
+        <v>263</v>
+      </c>
+      <c r="G57" t="s">
+        <v>239</v>
+      </c>
+      <c r="H57" t="s">
+        <v>61</v>
+      </c>
+      <c r="I57" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>1</v>
+      </c>
+      <c r="C58" s="35" t="s">
+        <v>300</v>
+      </c>
+      <c r="D58" t="s">
+        <v>301</v>
+      </c>
+      <c r="E58" s="20" t="s">
+        <v>299</v>
+      </c>
+      <c r="F58" s="46" t="s">
+        <v>303</v>
+      </c>
+      <c r="G58" s="20" t="s">
+        <v>239</v>
+      </c>
+      <c r="H58" t="s">
+        <v>61</v>
+      </c>
+      <c r="I58" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>2</v>
+      </c>
+      <c r="C59" s="35" t="s">
+        <v>305</v>
+      </c>
+      <c r="D59" t="s">
+        <v>306</v>
+      </c>
+      <c r="E59" s="20" t="s">
+        <v>304</v>
+      </c>
+      <c r="F59" s="46" t="s">
+        <v>308</v>
+      </c>
+      <c r="G59" s="20" t="s">
+        <v>239</v>
+      </c>
+      <c r="H59" t="s">
+        <v>61</v>
+      </c>
+      <c r="I59" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>3</v>
+      </c>
+      <c r="C60" s="35" t="s">
+        <v>315</v>
+      </c>
+      <c r="D60" s="20" t="s">
+        <v>317</v>
+      </c>
+      <c r="E60" t="s">
+        <v>313</v>
+      </c>
+      <c r="F60" s="46" t="s">
+        <v>432</v>
+      </c>
+      <c r="G60" s="20" t="s">
+        <v>321</v>
+      </c>
+      <c r="H60" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="I60" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>4</v>
+      </c>
+      <c r="C61" s="35" t="s">
+        <v>316</v>
+      </c>
+      <c r="D61" s="20" t="s">
+        <v>318</v>
+      </c>
+      <c r="E61" t="s">
+        <v>314</v>
+      </c>
+      <c r="F61" s="24" t="s">
+        <v>320</v>
+      </c>
+      <c r="G61" s="20" t="s">
+        <v>239</v>
+      </c>
+      <c r="H61" t="s">
+        <v>61</v>
+      </c>
+      <c r="I61" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>5</v>
+      </c>
+      <c r="C62" s="35" t="s">
+        <v>329</v>
+      </c>
+      <c r="D62" s="20" t="s">
+        <v>325</v>
+      </c>
+      <c r="E62" t="s">
+        <v>323</v>
+      </c>
+      <c r="F62" s="24" t="s">
+        <v>275</v>
+      </c>
+      <c r="G62" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="H62" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="I62" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>6</v>
+      </c>
+      <c r="C63" s="35" t="s">
+        <v>330</v>
+      </c>
+      <c r="D63" s="20" t="s">
+        <v>328</v>
+      </c>
+      <c r="E63" t="s">
+        <v>326</v>
+      </c>
+      <c r="F63" s="24" t="s">
+        <v>339</v>
+      </c>
+      <c r="G63" s="20" t="s">
+        <v>321</v>
+      </c>
+      <c r="H63" t="s">
+        <v>61</v>
+      </c>
+      <c r="I63" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <v>7</v>
+      </c>
+      <c r="C64" s="35" t="s">
+        <v>343</v>
+      </c>
+      <c r="D64" s="20" t="s">
+        <v>342</v>
+      </c>
+      <c r="E64" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="F64" s="24" t="s">
+        <v>339</v>
+      </c>
+      <c r="G64" s="20" t="s">
+        <v>321</v>
+      </c>
+      <c r="H64" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="I64" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>8</v>
+      </c>
+      <c r="C65" s="35" t="s">
+        <v>442</v>
+      </c>
+      <c r="D65" s="20" t="s">
+        <v>440</v>
+      </c>
+      <c r="E65" s="5" t="s">
+        <v>444</v>
+      </c>
+      <c r="F65" s="24" t="s">
+        <v>448</v>
+      </c>
+      <c r="G65" s="20" t="s">
+        <v>126</v>
+      </c>
+      <c r="H65" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="I65" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <v>9</v>
+      </c>
+      <c r="C66" s="35" t="s">
+        <v>443</v>
+      </c>
+      <c r="D66" s="20" t="s">
+        <v>441</v>
+      </c>
+      <c r="E66" s="5" t="s">
+        <v>445</v>
+      </c>
+      <c r="F66" s="24" t="s">
+        <v>448</v>
+      </c>
+      <c r="G66" s="20" t="s">
+        <v>126</v>
+      </c>
+      <c r="H66" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="I66" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A67">
+        <v>10</v>
+      </c>
+      <c r="C67" s="35" t="s">
+        <v>345</v>
+      </c>
+      <c r="D67" s="20" t="s">
+        <v>346</v>
+      </c>
+      <c r="E67" s="5" t="s">
+        <v>344</v>
+      </c>
+      <c r="F67" s="24" t="s">
+        <v>348</v>
+      </c>
+      <c r="G67" s="20" t="s">
+        <v>239</v>
+      </c>
+      <c r="H67" t="s">
+        <v>61</v>
+      </c>
+      <c r="I67" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A68">
+        <v>11</v>
+      </c>
+      <c r="C68" s="35" t="s">
+        <v>351</v>
+      </c>
+      <c r="D68" s="20" t="s">
+        <v>350</v>
+      </c>
+      <c r="E68" t="s">
+        <v>349</v>
+      </c>
+      <c r="F68" s="24" t="s">
+        <v>348</v>
+      </c>
+      <c r="G68" s="20" t="s">
+        <v>239</v>
+      </c>
+      <c r="H68" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="I68" s="36" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A69">
+        <v>12</v>
+      </c>
+      <c r="C69" s="35" t="s">
+        <v>359</v>
+      </c>
+      <c r="D69" s="20" t="s">
+        <v>356</v>
+      </c>
+      <c r="E69" t="s">
+        <v>353</v>
+      </c>
+      <c r="F69" s="24" t="s">
+        <v>354</v>
+      </c>
+      <c r="G69" s="20" t="s">
+        <v>239</v>
+      </c>
+      <c r="H69" t="s">
+        <v>61</v>
+      </c>
+      <c r="I69" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A70">
+        <v>13</v>
+      </c>
+      <c r="C70" s="35" t="s">
+        <v>360</v>
+      </c>
+      <c r="D70" s="20" t="s">
+        <v>401</v>
+      </c>
+      <c r="E70" s="5" t="s">
+        <v>357</v>
+      </c>
+      <c r="F70" s="46" t="s">
+        <v>421</v>
+      </c>
+      <c r="G70" s="20" t="s">
+        <v>239</v>
+      </c>
+      <c r="H70" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="I70" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A71">
+        <v>14</v>
+      </c>
+      <c r="C71" s="35" t="s">
+        <v>400</v>
+      </c>
+      <c r="D71" s="20" t="s">
+        <v>402</v>
+      </c>
+      <c r="E71" s="5" t="s">
+        <v>422</v>
+      </c>
+      <c r="F71" s="46" t="s">
+        <v>403</v>
+      </c>
+      <c r="G71" s="20" t="s">
+        <v>239</v>
+      </c>
+      <c r="H71" t="s">
+        <v>61</v>
+      </c>
+      <c r="I71" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A72">
+        <v>15</v>
+      </c>
+      <c r="C72" s="35" t="s">
+        <v>361</v>
+      </c>
+      <c r="D72" s="20" t="s">
+        <v>363</v>
+      </c>
+      <c r="E72" t="s">
+        <v>358</v>
+      </c>
+      <c r="F72" s="24" t="s">
+        <v>364</v>
+      </c>
+      <c r="G72" s="20" t="s">
+        <v>239</v>
+      </c>
+      <c r="H72" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="I72" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A73">
+        <v>16</v>
+      </c>
+      <c r="C73" s="35" t="s">
+        <v>366</v>
+      </c>
+      <c r="D73" s="20" t="s">
+        <v>367</v>
+      </c>
+      <c r="E73" t="s">
+        <v>365</v>
+      </c>
+      <c r="F73" s="24" t="s">
+        <v>430</v>
+      </c>
+      <c r="G73" s="20" t="s">
+        <v>376</v>
+      </c>
+      <c r="H73" t="s">
+        <v>61</v>
+      </c>
+      <c r="I73" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A74">
+        <v>17</v>
+      </c>
+      <c r="C74" s="35" t="s">
+        <v>370</v>
+      </c>
+      <c r="D74" s="20" t="s">
+        <v>371</v>
+      </c>
+      <c r="E74" t="s">
+        <v>369</v>
+      </c>
+      <c r="F74" s="24" t="s">
+        <v>375</v>
+      </c>
+      <c r="G74" s="20" t="s">
+        <v>376</v>
+      </c>
+      <c r="H74" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="I74" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A75">
+        <v>18</v>
+      </c>
+      <c r="C75" s="35" t="s">
+        <v>383</v>
+      </c>
+      <c r="D75" s="20" t="s">
+        <v>380</v>
+      </c>
+      <c r="E75" t="s">
+        <v>377</v>
+      </c>
+      <c r="F75" s="24" t="s">
+        <v>364</v>
+      </c>
+      <c r="G75" s="20" t="s">
+        <v>239</v>
+      </c>
+      <c r="H75" t="s">
+        <v>61</v>
+      </c>
+      <c r="I75" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A76">
+        <v>19</v>
+      </c>
+      <c r="C76" s="35" t="s">
+        <v>384</v>
+      </c>
+      <c r="D76" s="20" t="s">
+        <v>381</v>
+      </c>
+      <c r="E76" t="s">
+        <v>379</v>
+      </c>
+      <c r="F76" s="24" t="s">
+        <v>232</v>
+      </c>
+      <c r="G76" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="H76" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="I76" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A77">
+        <v>20</v>
+      </c>
+      <c r="C77" s="35" t="s">
+        <v>388</v>
+      </c>
+      <c r="D77" s="20" t="s">
+        <v>387</v>
+      </c>
+      <c r="E77" t="s">
+        <v>386</v>
+      </c>
+      <c r="F77" s="24" t="s">
+        <v>232</v>
+      </c>
+      <c r="G77" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="H77" t="s">
+        <v>61</v>
+      </c>
+      <c r="I77" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A78">
+        <v>21</v>
+      </c>
+      <c r="C78" s="35" t="s">
+        <v>390</v>
+      </c>
+      <c r="D78" s="20" t="s">
+        <v>391</v>
+      </c>
+      <c r="E78" t="s">
+        <v>389</v>
+      </c>
+      <c r="F78" s="24" t="s">
+        <v>232</v>
+      </c>
+      <c r="G78" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="H78" t="s">
+        <v>61</v>
+      </c>
+      <c r="I78" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A79">
+        <v>22</v>
+      </c>
+      <c r="C79" s="35" t="s">
+        <v>395</v>
+      </c>
+      <c r="D79" s="20" t="s">
+        <v>393</v>
+      </c>
+      <c r="E79" t="s">
+        <v>394</v>
+      </c>
+      <c r="F79" s="24" t="s">
+        <v>396</v>
+      </c>
+      <c r="G79" s="20" t="s">
+        <v>239</v>
+      </c>
+      <c r="H79" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="I79" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A80">
+        <v>23</v>
+      </c>
+      <c r="C80" s="35" t="s">
+        <v>398</v>
+      </c>
+      <c r="D80" s="20" t="s">
+        <v>399</v>
+      </c>
+      <c r="E80" t="s">
+        <v>397</v>
+      </c>
+      <c r="F80" s="24" t="s">
+        <v>232</v>
+      </c>
+      <c r="G80" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="H80" t="s">
+        <v>61</v>
+      </c>
+      <c r="I80" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A81">
+        <v>24</v>
+      </c>
+      <c r="C81" s="35" t="s">
+        <v>433</v>
+      </c>
+      <c r="D81" s="20" t="s">
+        <v>434</v>
+      </c>
+      <c r="E81" s="5" t="s">
+        <v>435</v>
+      </c>
+      <c r="F81" s="24" t="s">
+        <v>436</v>
+      </c>
+      <c r="G81" s="20" t="s">
+        <v>126</v>
+      </c>
+      <c r="H81" t="s">
+        <v>61</v>
+      </c>
+      <c r="I81" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C82" s="5"/>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B83" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="C83" s="27"/>
+      <c r="D83" s="27"/>
+      <c r="E83" s="27"/>
+      <c r="F83" s="27"/>
+      <c r="G83" s="27"/>
+      <c r="H83" s="28"/>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C84" s="24" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C85" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="D85" s="42" t="s">
+        <v>84</v>
+      </c>
+      <c r="E85" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C86" t="s">
+        <v>423</v>
+      </c>
+      <c r="D86" s="42" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C87" t="s">
+        <v>424</v>
+      </c>
+      <c r="D87" s="47" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C88" t="s">
+        <v>425</v>
+      </c>
+      <c r="D88" s="47" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C89" t="s">
+        <v>426</v>
+      </c>
+      <c r="D89" s="47" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C90" t="s">
+        <v>427</v>
+      </c>
+      <c r="D90" s="47" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C91" t="s">
+        <v>428</v>
+      </c>
+      <c r="D91" s="47" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B93" s="26" t="s">
+        <v>104</v>
+      </c>
+      <c r="C93" s="27"/>
+      <c r="D93" s="27"/>
+      <c r="E93" s="27"/>
+      <c r="F93" s="27"/>
+      <c r="G93" s="27"/>
+      <c r="H93" s="28"/>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C94" s="24" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C95" t="s">
+        <v>277</v>
+      </c>
+      <c r="D95" s="42" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C96" t="s">
+        <v>278</v>
+      </c>
+      <c r="D96" s="42" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="97" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C97" t="s">
+        <v>279</v>
+      </c>
+      <c r="D97" s="42" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="98" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C98" s="5"/>
+      <c r="D98" s="5"/>
+    </row>
+    <row r="99" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C99" s="5"/>
+      <c r="D99" s="5"/>
+    </row>
+    <row r="100" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B100" s="26" t="s">
+        <v>417</v>
+      </c>
+      <c r="C100" s="27"/>
+      <c r="D100" s="27"/>
+      <c r="E100" s="27"/>
+      <c r="F100" s="27"/>
+      <c r="G100" s="27"/>
+      <c r="H100" s="28"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:K87"/>
   <sheetViews>
@@ -5042,7 +6713,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:K52"/>
   <sheetViews>
@@ -5681,7 +7352,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:K69"/>
   <sheetViews>

</xml_diff>

<commit_message>
USA test case with proper data running.
</commit_message>
<xml_diff>
--- a/RECC_Config.xlsx
+++ b/RECC_Config.xlsx
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="8652" windowHeight="4896" tabRatio="844"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8652" windowHeight="4896" tabRatio="844" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="5" r:id="rId1"/>
-    <sheet name="RECC_USA_TestCase_V1.0" sheetId="9" r:id="rId2"/>
-    <sheet name="RECC_USA_TestCase_V2.0" sheetId="10" r:id="rId3"/>
+    <sheet name="RECC_USA_TestCase_V2.0" sheetId="10" r:id="rId2"/>
+    <sheet name="RECC_USA_TestCase_V1.0" sheetId="9" r:id="rId3"/>
     <sheet name="RECC_Main_Development_1" sheetId="7" r:id="rId4"/>
     <sheet name="GDP_Test" sheetId="8" r:id="rId5"/>
     <sheet name="Setting_TestRun_1" sheetId="6" r:id="rId6"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1417" uniqueCount="460">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1627" uniqueCount="611">
   <si>
     <t>Description</t>
   </si>
@@ -1404,13 +1404,466 @@
   </si>
   <si>
     <t>RECC_USA_TestCase_V2.0</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>RECC db status for US</t>
+  </si>
+  <si>
+    <t>SSP</t>
+  </si>
+  <si>
+    <t>downloaded from SSP database, 32 SSP regions, US included</t>
+  </si>
+  <si>
+    <t>Hist/fixed</t>
+  </si>
+  <si>
+    <t>RE</t>
+  </si>
+  <si>
+    <t>SSP/RCP</t>
+  </si>
+  <si>
+    <t>stoichiometric relations, present</t>
+  </si>
+  <si>
+    <t>Color</t>
+  </si>
+  <si>
+    <t>no data</t>
+  </si>
+  <si>
+    <t>Groups</t>
+  </si>
+  <si>
+    <t>SSP-specific data</t>
+  </si>
+  <si>
+    <t>SSP-RCP-combination-specific data</t>
+  </si>
+  <si>
+    <t>Historic data or fixed values</t>
+  </si>
+  <si>
+    <t>Resource-efficiency-strategy data</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>ready</t>
+  </si>
+  <si>
+    <t>2_S_RECC_FinalProducts_2015_USA_V2.0</t>
+  </si>
+  <si>
+    <t>2_S_RECC_FinalProducts_Future_USA_V2.0</t>
+  </si>
+  <si>
+    <t>3_EI_Products_UsePhase_USA_V2.0</t>
+  </si>
+  <si>
+    <t>3_IU_Products_UsePhase_USA_V2.0</t>
+  </si>
+  <si>
+    <t>3_LT_RECC_ProductLifetime_V2.0</t>
+  </si>
+  <si>
+    <t>3_MC_RECC_FinalProducts_Buildings_USA_V2.0</t>
+  </si>
+  <si>
+    <t>3_MC_RECC_FinalProducts_Vehicles_USA_V2.0</t>
+  </si>
+  <si>
+    <t>3_MC_Elements_Materials_ExistingStock_V2.0</t>
+  </si>
+  <si>
+    <t>3_MC_Elements_Materials_Primary_V2.0</t>
+  </si>
+  <si>
+    <t>3_SHA_RECC_REStrategyScaleUp_SSP_32R_V2.0</t>
+  </si>
+  <si>
+    <t>4_PE_GHGIntensityEnergySupply_V2.0</t>
+  </si>
+  <si>
+    <t>4_PE_ProcessExtensions_USA_V2.0</t>
+  </si>
+  <si>
+    <t>4_EI_ProcessEnergyIntensity_USA_V2.0</t>
+  </si>
+  <si>
+    <t>4_PY_EoL_RR_USA_V2.0</t>
+  </si>
+  <si>
+    <t>4_PY_Manufacturing_USA_V2.0</t>
+  </si>
+  <si>
+    <t>4_PY_MaterialProductionRemelting_V2.0</t>
+  </si>
+  <si>
+    <t>6_PR_EoL_RR_Improvement_USA_V2.0</t>
+  </si>
+  <si>
+    <t>6_PR_MoreIntenseUse_USA_V2.0</t>
+  </si>
+  <si>
+    <t>6_PR_LightWeighting_USA_V2.0</t>
+  </si>
+  <si>
+    <t>6_PR_LifeTimeExtension_USA_V2.0</t>
+  </si>
+  <si>
+    <t>6_PR_FabricationYieldImprovement_USA_V2.0</t>
+  </si>
+  <si>
+    <t>6_PR_ReUse_USA_V2.0</t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t>vehicles: million units. buildings: billion m2</t>
+  </si>
+  <si>
+    <t>Million</t>
+  </si>
+  <si>
+    <t>vehicles: cars per person, buildings: m2 per person</t>
+  </si>
+  <si>
+    <t>contains some simple scenario calculations, must be linked to SSP storylines</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>US$2005/ton</t>
+  </si>
+  <si>
+    <t>kg/unit</t>
+  </si>
+  <si>
+    <t>kg/m2</t>
+  </si>
+  <si>
+    <t>Mechanism/use in ODYM-RECC model</t>
+  </si>
+  <si>
+    <t>1 (kg/kg)</t>
+  </si>
+  <si>
+    <t>3_SHA_RECC_Urbanisation_SSP_32R_V1.0</t>
+  </si>
+  <si>
+    <t>3_SHA_RECC_Urbanisation_SSP_32R</t>
+  </si>
+  <si>
+    <t>Urbanisation rate in % by region and SSP scenario</t>
+  </si>
+  <si>
+    <t>58dc2274-f746-491c-adc5-3ce091a43f36</t>
+  </si>
+  <si>
+    <t>1_F_RECC_PPP_GDP_SSP_32R_V1.0</t>
+  </si>
+  <si>
+    <t>1_F_RECC_PPP_GDP_SSP_32R</t>
+  </si>
+  <si>
+    <t>GDP data for SSP scenarios. PPP GDP in billion US$2005/yr.</t>
+  </si>
+  <si>
+    <t>c44683c0-76d0-40c3-a4dd-3c94bf8ee104</t>
+  </si>
+  <si>
+    <t>billion US$2005/yr</t>
+  </si>
+  <si>
+    <t>Not used by ODYM-RECC, can be used for exogenous scenario modelling</t>
+  </si>
+  <si>
+    <t>yr</t>
+  </si>
+  <si>
+    <t>vehicles: km/yr. buildings: 1</t>
+  </si>
+  <si>
+    <t>Vehicles: MJ/km. Buildings: MJ/m2/yr</t>
+  </si>
+  <si>
+    <t>Needs refinement. Not SSP-dependent at the moment</t>
+  </si>
+  <si>
+    <t>kg of CO2-eq/MJ</t>
+  </si>
+  <si>
+    <t>kg/kg</t>
+  </si>
+  <si>
+    <t>MJ/kg</t>
+  </si>
+  <si>
+    <t>percentage points</t>
+  </si>
+  <si>
+    <t>increase of EoL RR (EoL product to scrap) in percentage points from base value</t>
+  </si>
+  <si>
+    <t>NewStock = 1/(1+ MoreIntenseUsePotential * ImplementationCurve) * OldStock</t>
+  </si>
+  <si>
+    <t>NewLifeTime = (1+ LifetimeExtensionPotential * ImplementationCurve) * OldLifetime. (For future age-cohorts only, for existing cohorts no extension has been implemented yet.)</t>
+  </si>
+  <si>
+    <t>contains potential estimates from previous work, must be linked to SSP storylines</t>
+  </si>
+  <si>
+    <t>Scales up per capita stocks</t>
+  </si>
+  <si>
+    <t>2015 in-use stock, starting value</t>
+  </si>
+  <si>
+    <t>Future stock trajectories, drive inflow and outflow.</t>
+  </si>
+  <si>
+    <t>NewMaterialContent = (1- LightWeightingPotential * ImplementationCurve) * OldMaterialContent.</t>
+  </si>
+  <si>
+    <t>NewFabricationYield = OldFabricationYield - FabricationYieldImprovementPotential * ImplementationCurve</t>
+  </si>
+  <si>
+    <t>ReUseFlow = ReUsePotential * ImplementationCurve * Obsolete Products (Outflow use phase)</t>
+  </si>
+  <si>
+    <t>Translates service output from stock into energy consumption (use phase)</t>
+  </si>
+  <si>
+    <t>Translates stock into service output from stock (use phase)</t>
+  </si>
+  <si>
+    <t>translates product stock/flow into material stock/flow</t>
+  </si>
+  <si>
+    <t>Breakdown of materials in existing stock into chemical elements</t>
+  </si>
+  <si>
+    <t>Breakdown of materials in primary production into chemical elements</t>
+  </si>
+  <si>
+    <t>CO2 price/tax per SSP-RCP scenario</t>
+  </si>
+  <si>
+    <t>% of RE strategy potential implemented, dependent on scenario, time, and region</t>
+  </si>
+  <si>
+    <t>Translates stock into flows (stock-driven model)</t>
+  </si>
+  <si>
+    <t>Translates energy consumption into GHG emissions from energy use (scope 1)</t>
+  </si>
+  <si>
+    <t>Translates energy consumption into GHG emissions from energy supply (scope 2)</t>
+  </si>
+  <si>
+    <t>Translates manufacturing and waste mgt. process output into extensions such as CO2 emissions</t>
+  </si>
+  <si>
+    <t>Translates manufacturing and waste mgt. process output into energy demand</t>
+  </si>
+  <si>
+    <t>Translates EoL product output into scrap (End-of-life recovery rate), material-specific</t>
+  </si>
+  <si>
+    <t>Translates scrap into secondary materials, element-specific</t>
+  </si>
+  <si>
+    <t>Translates manufacturing process output into fabrication scrap</t>
+  </si>
+  <si>
+    <t>4_EI_ManufacturingEnergyIntensity_USA</t>
+  </si>
+  <si>
+    <t>specific energy consumption of material production processes</t>
+  </si>
+  <si>
+    <t>specific energy consumption of manufacturing processes</t>
+  </si>
+  <si>
+    <t>4_EI_ManufacturingEnergyIntensity_USA_V1.0</t>
+  </si>
+  <si>
+    <t>Fncr</t>
+  </si>
+  <si>
+    <t>5cc66f0a-35fb-4c24-a46a-7c93f94866ae</t>
+  </si>
+  <si>
+    <t>40c2fa93-17a7-4190-9925-a32b040b4bb0</t>
+  </si>
+  <si>
+    <t>bfc8d8e2-6f5a-4bb3-8654-3cd30420c177</t>
+  </si>
+  <si>
+    <t>2ca77a36-e533-46ca-9100-00943c565a0c</t>
+  </si>
+  <si>
+    <t>64925b9f-8752-4de7-96cf-30c798436d25</t>
+  </si>
+  <si>
+    <t>36894dc1-28f6-4035-889a-8b49d1e6fbf6</t>
+  </si>
+  <si>
+    <t>2d812575-7f69-40e2-8439-8f0b91fde862</t>
+  </si>
+  <si>
+    <t>64b87156-5c97-4fb7-89ec-51e357a261fd</t>
+  </si>
+  <si>
+    <t>e796bb77-83ce-4376-b9fe-9ff054597ad6</t>
+  </si>
+  <si>
+    <t>4cd676b2-2111-4fec-965a-46e2a620d812</t>
+  </si>
+  <si>
+    <t>db13f4ef-f950-4dc1-a9be-542eb1d3e350</t>
+  </si>
+  <si>
+    <t>91cfa29c-04bf-48fb-ae85-05c5437ab108</t>
+  </si>
+  <si>
+    <t>467e0480-8732-48f3-a733-fcbc0ba930b2</t>
+  </si>
+  <si>
+    <t>ad3b9910-bde2-4078-bd19-f2b675ba3a4e</t>
+  </si>
+  <si>
+    <t>01258323-be23-4ceb-a9c4-c9c13e4ff648</t>
+  </si>
+  <si>
+    <t>3041b7f0-3348-490d-88e3-1504242fb7b3</t>
+  </si>
+  <si>
+    <t>affd2976-8d97-4e7e-b56c-f55292581f65</t>
+  </si>
+  <si>
+    <t>0d593bb9-f575-4452-bc2c-ee5674e2f70c</t>
+  </si>
+  <si>
+    <t>a4007b31-eeca-4718-a995-2a2f7d5e638b</t>
+  </si>
+  <si>
+    <t>f37c6a72-3122-4b06-8747-9ecb310834ae</t>
+  </si>
+  <si>
+    <t>6badcb78-869f-48b1-bc70-309e4da64323</t>
+  </si>
+  <si>
+    <t>320ffb83-c4f0-4109-9b9f-c2dbdf0a034d</t>
+  </si>
+  <si>
+    <t>8b77fecc-703f-4d50-8c53-c629b217e123</t>
+  </si>
+  <si>
+    <t>available historic data were transferred, dataset file contains original data and ancillary calculations</t>
+  </si>
+  <si>
+    <t>Aggregated product groups such as buildings, vehicles, …</t>
+  </si>
+  <si>
+    <t>Product Groups</t>
+  </si>
+  <si>
+    <t>3_SHA_TypeSplit_NewProducts_USA</t>
+  </si>
+  <si>
+    <t>Split product groups into different types, at point of final consumption</t>
+  </si>
+  <si>
+    <t>3_SHA_TypeSplit_NewProducts_USA_V1.0</t>
+  </si>
+  <si>
+    <t>Used to divided total new buildings (m2/yr) and vehicles (#) into different types.</t>
+  </si>
+  <si>
+    <t>2d195d97-f04b-4286-9be6-9901cfe75ef8</t>
+  </si>
+  <si>
+    <t>GgtrS</t>
+  </si>
+  <si>
+    <t>StGr</t>
+  </si>
+  <si>
+    <t>Vehicle km/yr: No recent data, use 20000 km/yr from old source</t>
+  </si>
+  <si>
+    <t>At the moment, only ‘standard’ building type is used</t>
+  </si>
+  <si>
+    <t>buildings: only standard energy consumption is covered.</t>
+  </si>
+  <si>
+    <t>3_SHA_EnergyCarrierSplit_Buildings_USA</t>
+  </si>
+  <si>
+    <t>Split total building energy consumption into different energy carriers</t>
+  </si>
+  <si>
+    <t>3_SHA_EnergyCarrierSplit_Buildings_USA_V1.0</t>
+  </si>
+  <si>
+    <t>Used to split total building energy consumption into different energy carriers</t>
+  </si>
+  <si>
+    <t>0df23fd6-4cc9-4b3a-ae70-f8ed0751c1e3</t>
+  </si>
+  <si>
+    <t>[0,2,6,8,9,10,11,13]</t>
+  </si>
+  <si>
+    <t>tGrnS</t>
+  </si>
+  <si>
+    <t>Data from SSP scenario group could directly be used, some energy carriers relabelled.</t>
+  </si>
+  <si>
+    <t>all relevant scenario values transferred from scenario working group</t>
+  </si>
+  <si>
+    <t>data lacking, contains typical figures for element composition of materials</t>
+  </si>
+  <si>
+    <t>contains IEA ETP proxies: BAU for SSP3 and 5, BLUE MAP for SSP 1 and 4, (BAU + BLUE MAP)/2 for SSP2</t>
+  </si>
+  <si>
+    <t>No data at the moment. Fix later.</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>Product_groups_m3</t>
+  </si>
+  <si>
+    <t>[2,3,1,0,4]</t>
+  </si>
+  <si>
+    <t>good data but not SSP-consistent yet</t>
+  </si>
+  <si>
+    <t>workable but needs substantial refinement, not SSP-consistent yet</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1488,8 +1941,24 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1505,6 +1974,30 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1600,7 +2093,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1709,6 +2202,29 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1991,8 +2507,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D11:D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2186,10 +2702,2400 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:O105"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D96" sqref="D96"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="17.77734375" customWidth="1"/>
+    <col min="3" max="3" width="41.88671875" customWidth="1"/>
+    <col min="4" max="4" width="65.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="50.6640625" customWidth="1"/>
+    <col min="6" max="6" width="27.44140625" customWidth="1"/>
+    <col min="7" max="7" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="43.77734375" customWidth="1"/>
+    <col min="12" max="12" width="73.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="46.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="90" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B2" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="28"/>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C3" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" s="41" t="s">
+        <v>56</v>
+      </c>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="42" t="s">
+        <v>458</v>
+      </c>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="20"/>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="42" t="s">
+        <v>282</v>
+      </c>
+      <c r="I5" s="20"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="20"/>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="43" t="s">
+        <v>459</v>
+      </c>
+      <c r="I6" s="20"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="20"/>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="D7" s="11"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="20"/>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B8" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="28"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="20"/>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C9" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="D9" s="41" t="s">
+        <v>207</v>
+      </c>
+      <c r="E9" s="31"/>
+      <c r="F9" s="39"/>
+      <c r="G9" s="39"/>
+      <c r="H9" s="39"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="19"/>
+      <c r="K9" s="20"/>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="42" t="s">
+        <v>309</v>
+      </c>
+      <c r="I10" s="20"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="20"/>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C11" t="s">
+        <v>267</v>
+      </c>
+      <c r="D11" s="50" t="s">
+        <v>312</v>
+      </c>
+      <c r="I11" s="20"/>
+      <c r="J11" s="19"/>
+      <c r="K11" s="20"/>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C12" t="s">
+        <v>268</v>
+      </c>
+      <c r="D12" s="50" t="s">
+        <v>312</v>
+      </c>
+      <c r="I12" s="20"/>
+      <c r="J12" s="19"/>
+      <c r="K12" s="20"/>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="I13" s="20"/>
+      <c r="J13" s="25"/>
+      <c r="K13" s="20"/>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B14" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="C14" s="27"/>
+      <c r="D14" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="E14" s="27"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="27"/>
+      <c r="H14" s="28"/>
+      <c r="I14" s="36" t="s">
+        <v>439</v>
+      </c>
+      <c r="J14" s="20"/>
+      <c r="K14" s="20"/>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C15" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="E15" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15" s="31" t="s">
+        <v>438</v>
+      </c>
+      <c r="H15" s="30" t="s">
+        <v>186</v>
+      </c>
+      <c r="I15" s="52" t="s">
+        <v>187</v>
+      </c>
+      <c r="K15" s="20"/>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C16" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" t="s">
+        <v>28</v>
+      </c>
+      <c r="E16" t="s">
+        <v>16</v>
+      </c>
+      <c r="F16" t="s">
+        <v>16</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="H16" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="I16" s="20" t="s">
+        <v>188</v>
+      </c>
+      <c r="J16" s="20"/>
+      <c r="K16" s="20"/>
+    </row>
+    <row r="17" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C17" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" t="s">
+        <v>29</v>
+      </c>
+      <c r="E17" t="s">
+        <v>16</v>
+      </c>
+      <c r="F17" t="s">
+        <v>16</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>429</v>
+      </c>
+      <c r="H17" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="I17" s="20" t="s">
+        <v>189</v>
+      </c>
+      <c r="J17" s="20"/>
+      <c r="K17" s="20"/>
+    </row>
+    <row r="18" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C18" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" t="s">
+        <v>37</v>
+      </c>
+      <c r="E18" t="s">
+        <v>23</v>
+      </c>
+      <c r="F18" t="s">
+        <v>42</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>449</v>
+      </c>
+      <c r="H18" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="I18" s="20" t="s">
+        <v>190</v>
+      </c>
+      <c r="J18" s="20"/>
+      <c r="K18" s="20"/>
+    </row>
+    <row r="19" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C19" s="33" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" t="s">
+        <v>38</v>
+      </c>
+      <c r="E19" t="s">
+        <v>24</v>
+      </c>
+      <c r="F19" t="s">
+        <v>24</v>
+      </c>
+      <c r="G19" t="s">
+        <v>418</v>
+      </c>
+      <c r="H19" s="29">
+        <v>1</v>
+      </c>
+      <c r="I19" s="20" t="s">
+        <v>192</v>
+      </c>
+      <c r="J19" s="20"/>
+      <c r="K19" s="20"/>
+    </row>
+    <row r="20" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C20" s="33" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" t="s">
+        <v>31</v>
+      </c>
+      <c r="E20" t="s">
+        <v>39</v>
+      </c>
+      <c r="F20" t="s">
+        <v>40</v>
+      </c>
+      <c r="G20" t="s">
+        <v>276</v>
+      </c>
+      <c r="H20" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="I20" s="20" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="21" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C21" s="45" t="s">
+        <v>142</v>
+      </c>
+      <c r="D21" t="s">
+        <v>150</v>
+      </c>
+      <c r="E21" t="s">
+        <v>26</v>
+      </c>
+      <c r="F21" t="s">
+        <v>155</v>
+      </c>
+      <c r="G21" t="s">
+        <v>457</v>
+      </c>
+      <c r="H21" s="29" t="s">
+        <v>184</v>
+      </c>
+      <c r="I21" s="20" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="22" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C22" s="45" t="s">
+        <v>143</v>
+      </c>
+      <c r="D22" t="s">
+        <v>151</v>
+      </c>
+      <c r="E22" t="s">
+        <v>26</v>
+      </c>
+      <c r="F22" t="s">
+        <v>156</v>
+      </c>
+      <c r="G22" t="s">
+        <v>420</v>
+      </c>
+      <c r="H22" s="29" t="s">
+        <v>179</v>
+      </c>
+      <c r="I22" s="20" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="23" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C23" s="45" t="s">
+        <v>144</v>
+      </c>
+      <c r="D23" t="s">
+        <v>152</v>
+      </c>
+      <c r="E23" t="s">
+        <v>26</v>
+      </c>
+      <c r="F23" t="s">
+        <v>157</v>
+      </c>
+      <c r="G23" t="s">
+        <v>420</v>
+      </c>
+      <c r="H23" s="29" t="s">
+        <v>178</v>
+      </c>
+      <c r="I23" s="20" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C24" s="45" t="s">
+        <v>145</v>
+      </c>
+      <c r="D24" t="s">
+        <v>148</v>
+      </c>
+      <c r="E24" t="s">
+        <v>26</v>
+      </c>
+      <c r="F24" t="s">
+        <v>106</v>
+      </c>
+      <c r="G24" t="s">
+        <v>290</v>
+      </c>
+      <c r="H24" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="I24" s="20" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="25" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C25" s="45" t="s">
+        <v>163</v>
+      </c>
+      <c r="D25" t="s">
+        <v>159</v>
+      </c>
+      <c r="E25" t="s">
+        <v>21</v>
+      </c>
+      <c r="F25" t="s">
+        <v>134</v>
+      </c>
+      <c r="G25" t="s">
+        <v>454</v>
+      </c>
+      <c r="H25" s="29" t="s">
+        <v>337</v>
+      </c>
+      <c r="I25" s="20" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="26" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C26" s="45" t="s">
+        <v>20</v>
+      </c>
+      <c r="D26" t="s">
+        <v>32</v>
+      </c>
+      <c r="E26" t="s">
+        <v>21</v>
+      </c>
+      <c r="F26" t="s">
+        <v>105</v>
+      </c>
+      <c r="G26" t="s">
+        <v>420</v>
+      </c>
+      <c r="H26" s="29" t="s">
+        <v>181</v>
+      </c>
+      <c r="I26" s="20" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="27" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C27" s="45" t="s">
+        <v>331</v>
+      </c>
+      <c r="D27" t="s">
+        <v>332</v>
+      </c>
+      <c r="E27" t="s">
+        <v>21</v>
+      </c>
+      <c r="F27" t="s">
+        <v>333</v>
+      </c>
+      <c r="G27" t="s">
+        <v>334</v>
+      </c>
+      <c r="H27" s="29" t="s">
+        <v>335</v>
+      </c>
+      <c r="I27" s="20" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="28" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C28" s="45" t="s">
+        <v>164</v>
+      </c>
+      <c r="D28" t="s">
+        <v>165</v>
+      </c>
+      <c r="E28" t="s">
+        <v>21</v>
+      </c>
+      <c r="F28" t="s">
+        <v>166</v>
+      </c>
+      <c r="G28" t="s">
+        <v>420</v>
+      </c>
+      <c r="H28" s="29" t="s">
+        <v>205</v>
+      </c>
+      <c r="I28" s="20" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="29" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C29" s="45" t="s">
+        <v>22</v>
+      </c>
+      <c r="D29" t="s">
+        <v>34</v>
+      </c>
+      <c r="E29" t="s">
+        <v>21</v>
+      </c>
+      <c r="F29" t="s">
+        <v>117</v>
+      </c>
+      <c r="G29" t="s">
+        <v>289</v>
+      </c>
+      <c r="H29" s="29" t="s">
+        <v>182</v>
+      </c>
+      <c r="I29" s="20" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="30" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C30" s="45" t="s">
+        <v>167</v>
+      </c>
+      <c r="D30" t="s">
+        <v>170</v>
+      </c>
+      <c r="E30" t="s">
+        <v>169</v>
+      </c>
+      <c r="F30" t="s">
+        <v>168</v>
+      </c>
+      <c r="G30" t="s">
+        <v>599</v>
+      </c>
+      <c r="H30" s="29" t="s">
+        <v>185</v>
+      </c>
+      <c r="I30" s="20" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="31" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C31" s="45" t="s">
+        <v>25</v>
+      </c>
+      <c r="D31" t="s">
+        <v>171</v>
+      </c>
+      <c r="E31" t="s">
+        <v>25</v>
+      </c>
+      <c r="F31" t="s">
+        <v>41</v>
+      </c>
+      <c r="G31" t="s">
+        <v>418</v>
+      </c>
+      <c r="H31" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="I31" s="20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="32" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C32" s="45" t="s">
+        <v>173</v>
+      </c>
+      <c r="D32" t="s">
+        <v>174</v>
+      </c>
+      <c r="E32" t="s">
+        <v>173</v>
+      </c>
+      <c r="F32" t="s">
+        <v>172</v>
+      </c>
+      <c r="G32" s="5" t="s">
+        <v>419</v>
+      </c>
+      <c r="H32" s="29" t="s">
+        <v>183</v>
+      </c>
+      <c r="I32" s="20" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C33" s="33" t="s">
+        <v>283</v>
+      </c>
+      <c r="D33" t="s">
+        <v>284</v>
+      </c>
+      <c r="E33" t="s">
+        <v>25</v>
+      </c>
+      <c r="F33" t="s">
+        <v>285</v>
+      </c>
+      <c r="G33" s="20" t="s">
+        <v>418</v>
+      </c>
+      <c r="H33" s="29" t="s">
+        <v>286</v>
+      </c>
+      <c r="I33" s="20" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C34" s="45" t="s">
+        <v>294</v>
+      </c>
+      <c r="D34" t="s">
+        <v>295</v>
+      </c>
+      <c r="E34" t="s">
+        <v>25</v>
+      </c>
+      <c r="F34" t="s">
+        <v>251</v>
+      </c>
+      <c r="G34" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="H34" s="29" t="s">
+        <v>254</v>
+      </c>
+      <c r="I34" s="20" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C35" s="45" t="s">
+        <v>583</v>
+      </c>
+      <c r="D35" t="s">
+        <v>582</v>
+      </c>
+      <c r="E35" t="s">
+        <v>21</v>
+      </c>
+      <c r="F35" t="s">
+        <v>607</v>
+      </c>
+      <c r="G35" s="20" t="s">
+        <v>418</v>
+      </c>
+      <c r="H35" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="I35" s="20" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B37" s="26" t="s">
+        <v>101</v>
+      </c>
+      <c r="C37" s="27"/>
+      <c r="D37" s="27"/>
+      <c r="E37" s="27"/>
+      <c r="F37" s="27"/>
+      <c r="G37" s="27"/>
+      <c r="H37" s="28"/>
+    </row>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C38" s="34" t="s">
+        <v>102</v>
+      </c>
+      <c r="D38" s="31" t="s">
+        <v>103</v>
+      </c>
+      <c r="E38" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="F38" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="G38" s="39"/>
+      <c r="H38" s="39"/>
+    </row>
+    <row r="39" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C39" s="53">
+        <v>1</v>
+      </c>
+      <c r="D39" t="s">
+        <v>455</v>
+      </c>
+      <c r="E39" t="s">
+        <v>405</v>
+      </c>
+      <c r="F39" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C40" s="53">
+        <v>2</v>
+      </c>
+      <c r="D40" t="s">
+        <v>456</v>
+      </c>
+      <c r="E40" t="s">
+        <v>404</v>
+      </c>
+      <c r="F40" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="41" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C41" s="53">
+        <v>3</v>
+      </c>
+      <c r="D41" t="s">
+        <v>450</v>
+      </c>
+      <c r="E41" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="42" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C42" s="53">
+        <v>4</v>
+      </c>
+      <c r="D42" t="s">
+        <v>452</v>
+      </c>
+      <c r="E42" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="43" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C43" s="53">
+        <v>5</v>
+      </c>
+      <c r="D43" t="s">
+        <v>451</v>
+      </c>
+      <c r="E43" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="44" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C44" s="53">
+        <v>6</v>
+      </c>
+      <c r="D44" t="s">
+        <v>453</v>
+      </c>
+      <c r="E44" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="45" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C45" s="53">
+        <v>7</v>
+      </c>
+      <c r="D45" t="s">
+        <v>407</v>
+      </c>
+      <c r="E45" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="46" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C46" s="53">
+        <v>8</v>
+      </c>
+      <c r="D46" t="s">
+        <v>408</v>
+      </c>
+      <c r="E46" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="47" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C47" s="53">
+        <v>9</v>
+      </c>
+      <c r="D47" t="s">
+        <v>409</v>
+      </c>
+      <c r="E47" t="s">
+        <v>405</v>
+      </c>
+      <c r="F47" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="48" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C48" s="53">
+        <v>10</v>
+      </c>
+      <c r="D48" t="s">
+        <v>410</v>
+      </c>
+      <c r="E48" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="C49" s="53">
+        <v>11</v>
+      </c>
+      <c r="D49" t="s">
+        <v>411</v>
+      </c>
+      <c r="E49" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="C50" s="53">
+        <v>12</v>
+      </c>
+      <c r="D50" t="s">
+        <v>412</v>
+      </c>
+      <c r="E50" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="C51" s="53">
+        <v>13</v>
+      </c>
+      <c r="D51" t="s">
+        <v>415</v>
+      </c>
+      <c r="E51" t="s">
+        <v>405</v>
+      </c>
+      <c r="F51" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="C52" s="53">
+        <v>14</v>
+      </c>
+      <c r="D52" t="s">
+        <v>416</v>
+      </c>
+      <c r="E52" t="s">
+        <v>404</v>
+      </c>
+      <c r="F52" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="C53" s="5"/>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B55" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="C55" s="27"/>
+      <c r="D55" s="27"/>
+      <c r="E55" s="27"/>
+      <c r="F55" s="27"/>
+      <c r="G55" s="27"/>
+      <c r="H55" s="28"/>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="C56" s="34" t="s">
+        <v>58</v>
+      </c>
+      <c r="D56" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="E56" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="F56" s="31" t="s">
+        <v>59</v>
+      </c>
+      <c r="G56" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="H56" s="31" t="s">
+        <v>60</v>
+      </c>
+      <c r="I56" s="31" t="s">
+        <v>297</v>
+      </c>
+      <c r="J56" s="54" t="s">
+        <v>460</v>
+      </c>
+      <c r="K56" s="54" t="s">
+        <v>475</v>
+      </c>
+      <c r="L56" s="54" t="s">
+        <v>461</v>
+      </c>
+      <c r="M56" s="55" t="s">
+        <v>59</v>
+      </c>
+      <c r="N56" s="55" t="s">
+        <v>499</v>
+      </c>
+      <c r="O56" s="55" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>0</v>
+      </c>
+      <c r="C57" s="35" t="s">
+        <v>292</v>
+      </c>
+      <c r="D57" t="s">
+        <v>293</v>
+      </c>
+      <c r="E57" s="20" t="s">
+        <v>291</v>
+      </c>
+      <c r="F57" s="24" t="s">
+        <v>263</v>
+      </c>
+      <c r="G57" t="s">
+        <v>239</v>
+      </c>
+      <c r="H57" t="s">
+        <v>61</v>
+      </c>
+      <c r="I57" t="s">
+        <v>298</v>
+      </c>
+      <c r="J57" s="5" t="s">
+        <v>462</v>
+      </c>
+      <c r="K57" s="56"/>
+      <c r="L57" s="20" t="s">
+        <v>463</v>
+      </c>
+      <c r="M57" s="23" t="s">
+        <v>263</v>
+      </c>
+      <c r="N57" s="20" t="s">
+        <v>501</v>
+      </c>
+      <c r="O57" s="20" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>1</v>
+      </c>
+      <c r="C58" s="35" t="s">
+        <v>300</v>
+      </c>
+      <c r="D58" t="s">
+        <v>301</v>
+      </c>
+      <c r="E58" s="20" t="s">
+        <v>477</v>
+      </c>
+      <c r="F58" s="46" t="s">
+        <v>303</v>
+      </c>
+      <c r="G58" s="20" t="s">
+        <v>239</v>
+      </c>
+      <c r="H58" t="s">
+        <v>61</v>
+      </c>
+      <c r="I58" t="s">
+        <v>558</v>
+      </c>
+      <c r="J58" s="5" t="s">
+        <v>464</v>
+      </c>
+      <c r="K58" s="56"/>
+      <c r="L58" s="20" t="s">
+        <v>581</v>
+      </c>
+      <c r="M58" s="23" t="s">
+        <v>303</v>
+      </c>
+      <c r="N58" t="s">
+        <v>500</v>
+      </c>
+      <c r="O58" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>2</v>
+      </c>
+      <c r="C59" s="35" t="s">
+        <v>305</v>
+      </c>
+      <c r="D59" t="s">
+        <v>306</v>
+      </c>
+      <c r="E59" s="20" t="s">
+        <v>478</v>
+      </c>
+      <c r="F59" s="46" t="s">
+        <v>590</v>
+      </c>
+      <c r="G59" s="20" t="s">
+        <v>239</v>
+      </c>
+      <c r="H59" t="s">
+        <v>61</v>
+      </c>
+      <c r="I59" t="s">
+        <v>559</v>
+      </c>
+      <c r="J59" s="5" t="s">
+        <v>462</v>
+      </c>
+      <c r="K59" s="56"/>
+      <c r="L59" s="20" t="s">
+        <v>602</v>
+      </c>
+      <c r="M59" t="s">
+        <v>590</v>
+      </c>
+      <c r="N59" t="s">
+        <v>502</v>
+      </c>
+      <c r="O59" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>3</v>
+      </c>
+      <c r="C60" s="35" t="s">
+        <v>315</v>
+      </c>
+      <c r="D60" s="20" t="s">
+        <v>317</v>
+      </c>
+      <c r="E60" t="s">
+        <v>479</v>
+      </c>
+      <c r="F60" s="46" t="s">
+        <v>432</v>
+      </c>
+      <c r="G60" s="20" t="s">
+        <v>321</v>
+      </c>
+      <c r="H60" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="I60" t="s">
+        <v>560</v>
+      </c>
+      <c r="J60" s="5" t="s">
+        <v>462</v>
+      </c>
+      <c r="K60" s="69"/>
+      <c r="L60" s="20" t="s">
+        <v>593</v>
+      </c>
+      <c r="M60" t="s">
+        <v>432</v>
+      </c>
+      <c r="N60" t="s">
+        <v>522</v>
+      </c>
+      <c r="O60" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>4</v>
+      </c>
+      <c r="B61" s="68"/>
+      <c r="C61" s="35" t="s">
+        <v>316</v>
+      </c>
+      <c r="D61" s="20" t="s">
+        <v>318</v>
+      </c>
+      <c r="E61" t="s">
+        <v>480</v>
+      </c>
+      <c r="F61" s="24" t="s">
+        <v>320</v>
+      </c>
+      <c r="G61" s="20" t="s">
+        <v>239</v>
+      </c>
+      <c r="H61" t="s">
+        <v>61</v>
+      </c>
+      <c r="I61" t="s">
+        <v>561</v>
+      </c>
+      <c r="J61" s="5" t="s">
+        <v>462</v>
+      </c>
+      <c r="K61" s="69"/>
+      <c r="L61" s="20" t="s">
+        <v>591</v>
+      </c>
+      <c r="M61" t="s">
+        <v>320</v>
+      </c>
+      <c r="N61" t="s">
+        <v>521</v>
+      </c>
+      <c r="O61" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>5</v>
+      </c>
+      <c r="C62" s="67" t="s">
+        <v>329</v>
+      </c>
+      <c r="D62" s="20" t="s">
+        <v>325</v>
+      </c>
+      <c r="E62" t="s">
+        <v>481</v>
+      </c>
+      <c r="F62" s="24" t="s">
+        <v>275</v>
+      </c>
+      <c r="G62" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="H62" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="I62" t="s">
+        <v>562</v>
+      </c>
+      <c r="J62" s="5" t="s">
+        <v>464</v>
+      </c>
+      <c r="K62" s="69"/>
+      <c r="L62" s="20" t="s">
+        <v>523</v>
+      </c>
+      <c r="M62" s="20" t="s">
+        <v>275</v>
+      </c>
+      <c r="N62" s="20" t="s">
+        <v>520</v>
+      </c>
+      <c r="O62" s="20" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>6</v>
+      </c>
+      <c r="C63" s="67" t="s">
+        <v>330</v>
+      </c>
+      <c r="D63" s="20" t="s">
+        <v>328</v>
+      </c>
+      <c r="E63" t="s">
+        <v>482</v>
+      </c>
+      <c r="F63" s="24" t="s">
+        <v>339</v>
+      </c>
+      <c r="G63" s="20" t="s">
+        <v>321</v>
+      </c>
+      <c r="H63" t="s">
+        <v>61</v>
+      </c>
+      <c r="I63" t="s">
+        <v>563</v>
+      </c>
+      <c r="J63" s="5" t="s">
+        <v>464</v>
+      </c>
+      <c r="K63" s="69"/>
+      <c r="L63" s="20" t="s">
+        <v>523</v>
+      </c>
+      <c r="M63" s="20" t="s">
+        <v>339</v>
+      </c>
+      <c r="N63" s="20" t="s">
+        <v>507</v>
+      </c>
+      <c r="O63" s="20" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <v>7</v>
+      </c>
+      <c r="C64" s="67" t="s">
+        <v>343</v>
+      </c>
+      <c r="D64" s="20" t="s">
+        <v>342</v>
+      </c>
+      <c r="E64" s="5" t="s">
+        <v>483</v>
+      </c>
+      <c r="F64" s="24" t="s">
+        <v>339</v>
+      </c>
+      <c r="G64" s="20" t="s">
+        <v>321</v>
+      </c>
+      <c r="H64" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="I64" t="s">
+        <v>564</v>
+      </c>
+      <c r="J64" s="5" t="s">
+        <v>464</v>
+      </c>
+      <c r="K64" s="69"/>
+      <c r="L64" s="20" t="s">
+        <v>523</v>
+      </c>
+      <c r="M64" s="20" t="s">
+        <v>339</v>
+      </c>
+      <c r="N64" s="20" t="s">
+        <v>506</v>
+      </c>
+      <c r="O64" s="20" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="65" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>8</v>
+      </c>
+      <c r="C65" s="67" t="s">
+        <v>442</v>
+      </c>
+      <c r="D65" s="20" t="s">
+        <v>440</v>
+      </c>
+      <c r="E65" s="5" t="s">
+        <v>484</v>
+      </c>
+      <c r="F65" s="24" t="s">
+        <v>448</v>
+      </c>
+      <c r="G65" s="20" t="s">
+        <v>126</v>
+      </c>
+      <c r="H65" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="I65" t="s">
+        <v>565</v>
+      </c>
+      <c r="J65" s="5" t="s">
+        <v>464</v>
+      </c>
+      <c r="K65" s="56"/>
+      <c r="L65" s="20" t="s">
+        <v>603</v>
+      </c>
+      <c r="M65" s="20" t="s">
+        <v>448</v>
+      </c>
+      <c r="N65" s="20" t="s">
+        <v>509</v>
+      </c>
+      <c r="O65" s="20" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="66" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <v>9</v>
+      </c>
+      <c r="C66" s="67" t="s">
+        <v>443</v>
+      </c>
+      <c r="D66" s="20" t="s">
+        <v>441</v>
+      </c>
+      <c r="E66" s="5" t="s">
+        <v>485</v>
+      </c>
+      <c r="F66" s="24" t="s">
+        <v>448</v>
+      </c>
+      <c r="G66" s="20" t="s">
+        <v>126</v>
+      </c>
+      <c r="H66" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="I66" t="s">
+        <v>566</v>
+      </c>
+      <c r="J66" s="5" t="s">
+        <v>464</v>
+      </c>
+      <c r="K66" s="56"/>
+      <c r="L66" s="20" t="s">
+        <v>603</v>
+      </c>
+      <c r="M66" s="20" t="s">
+        <v>448</v>
+      </c>
+      <c r="N66" s="20" t="s">
+        <v>509</v>
+      </c>
+      <c r="O66" s="20" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="67" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A67">
+        <v>10</v>
+      </c>
+      <c r="C67" s="67" t="s">
+        <v>345</v>
+      </c>
+      <c r="D67" s="20" t="s">
+        <v>346</v>
+      </c>
+      <c r="E67" s="5" t="s">
+        <v>344</v>
+      </c>
+      <c r="F67" s="24" t="s">
+        <v>348</v>
+      </c>
+      <c r="G67" s="20" t="s">
+        <v>239</v>
+      </c>
+      <c r="H67" t="s">
+        <v>61</v>
+      </c>
+      <c r="I67" t="s">
+        <v>347</v>
+      </c>
+      <c r="J67" s="5" t="s">
+        <v>466</v>
+      </c>
+      <c r="K67" s="56"/>
+      <c r="L67" s="20" t="s">
+        <v>463</v>
+      </c>
+      <c r="M67" s="23" t="s">
+        <v>348</v>
+      </c>
+      <c r="N67" t="s">
+        <v>505</v>
+      </c>
+      <c r="O67" s="20" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="68" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A68">
+        <v>11</v>
+      </c>
+      <c r="C68" s="67" t="s">
+        <v>351</v>
+      </c>
+      <c r="D68" s="20" t="s">
+        <v>350</v>
+      </c>
+      <c r="E68" t="s">
+        <v>486</v>
+      </c>
+      <c r="F68" s="24" t="s">
+        <v>348</v>
+      </c>
+      <c r="G68" s="20" t="s">
+        <v>239</v>
+      </c>
+      <c r="H68" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="I68" s="36" t="s">
+        <v>567</v>
+      </c>
+      <c r="J68" s="5" t="s">
+        <v>466</v>
+      </c>
+      <c r="K68" s="57"/>
+      <c r="L68" s="20" t="s">
+        <v>503</v>
+      </c>
+      <c r="M68" t="s">
+        <v>348</v>
+      </c>
+      <c r="N68" t="s">
+        <v>504</v>
+      </c>
+      <c r="O68" s="20" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A69">
+        <v>12</v>
+      </c>
+      <c r="C69" s="67" t="s">
+        <v>359</v>
+      </c>
+      <c r="D69" s="20" t="s">
+        <v>356</v>
+      </c>
+      <c r="E69" t="s">
+        <v>487</v>
+      </c>
+      <c r="F69" s="24" t="s">
+        <v>354</v>
+      </c>
+      <c r="G69" s="20" t="s">
+        <v>239</v>
+      </c>
+      <c r="H69" t="s">
+        <v>61</v>
+      </c>
+      <c r="I69" t="s">
+        <v>568</v>
+      </c>
+      <c r="J69" s="5" t="s">
+        <v>466</v>
+      </c>
+      <c r="K69" s="56"/>
+      <c r="L69" s="20" t="s">
+        <v>604</v>
+      </c>
+      <c r="M69" t="s">
+        <v>354</v>
+      </c>
+      <c r="N69" t="s">
+        <v>524</v>
+      </c>
+      <c r="O69" s="20" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="70" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A70">
+        <v>13</v>
+      </c>
+      <c r="C70" s="67" t="s">
+        <v>360</v>
+      </c>
+      <c r="D70" s="20" t="s">
+        <v>401</v>
+      </c>
+      <c r="E70" s="5" t="s">
+        <v>488</v>
+      </c>
+      <c r="F70" s="46" t="s">
+        <v>421</v>
+      </c>
+      <c r="G70" s="20" t="s">
+        <v>239</v>
+      </c>
+      <c r="H70" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="I70" t="s">
+        <v>569</v>
+      </c>
+      <c r="J70" s="5" t="s">
+        <v>464</v>
+      </c>
+      <c r="K70" s="69"/>
+      <c r="L70" s="20" t="s">
+        <v>523</v>
+      </c>
+      <c r="M70" t="s">
+        <v>421</v>
+      </c>
+      <c r="N70" t="s">
+        <v>525</v>
+      </c>
+      <c r="O70" s="20" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="71" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A71">
+        <v>14</v>
+      </c>
+      <c r="C71" s="67" t="s">
+        <v>400</v>
+      </c>
+      <c r="D71" s="20" t="s">
+        <v>554</v>
+      </c>
+      <c r="E71" s="5" t="s">
+        <v>489</v>
+      </c>
+      <c r="F71" s="46" t="s">
+        <v>403</v>
+      </c>
+      <c r="G71" s="20" t="s">
+        <v>239</v>
+      </c>
+      <c r="H71" t="s">
+        <v>61</v>
+      </c>
+      <c r="I71" s="65" t="s">
+        <v>570</v>
+      </c>
+      <c r="J71" s="5" t="s">
+        <v>464</v>
+      </c>
+      <c r="K71" s="69"/>
+      <c r="L71" s="20" t="s">
+        <v>523</v>
+      </c>
+      <c r="M71" t="s">
+        <v>403</v>
+      </c>
+      <c r="N71" t="s">
+        <v>526</v>
+      </c>
+      <c r="O71" s="20" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="72" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A72">
+        <v>15</v>
+      </c>
+      <c r="C72" s="67" t="s">
+        <v>553</v>
+      </c>
+      <c r="D72" s="20" t="s">
+        <v>555</v>
+      </c>
+      <c r="E72" s="5" t="s">
+        <v>556</v>
+      </c>
+      <c r="F72" s="46" t="s">
+        <v>557</v>
+      </c>
+      <c r="G72" s="20" t="s">
+        <v>239</v>
+      </c>
+      <c r="H72" t="s">
+        <v>61</v>
+      </c>
+      <c r="I72" t="s">
+        <v>571</v>
+      </c>
+      <c r="J72" s="5" t="s">
+        <v>464</v>
+      </c>
+      <c r="K72" s="57"/>
+      <c r="L72" s="20" t="s">
+        <v>605</v>
+      </c>
+      <c r="M72" t="s">
+        <v>557</v>
+      </c>
+      <c r="N72" t="s">
+        <v>526</v>
+      </c>
+      <c r="O72" s="20" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="73" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A73">
+        <v>16</v>
+      </c>
+      <c r="C73" s="67" t="s">
+        <v>361</v>
+      </c>
+      <c r="D73" s="20" t="s">
+        <v>363</v>
+      </c>
+      <c r="E73" t="s">
+        <v>490</v>
+      </c>
+      <c r="F73" s="24" t="s">
+        <v>364</v>
+      </c>
+      <c r="G73" s="20" t="s">
+        <v>239</v>
+      </c>
+      <c r="H73" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="I73" t="s">
+        <v>572</v>
+      </c>
+      <c r="J73" s="5" t="s">
+        <v>464</v>
+      </c>
+      <c r="K73" s="56"/>
+      <c r="L73" s="20" t="s">
+        <v>606</v>
+      </c>
+      <c r="M73" s="20" t="s">
+        <v>364</v>
+      </c>
+      <c r="N73" s="20" t="s">
+        <v>504</v>
+      </c>
+      <c r="O73" s="20" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="74" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A74">
+        <v>17</v>
+      </c>
+      <c r="C74" s="67" t="s">
+        <v>366</v>
+      </c>
+      <c r="D74" s="20" t="s">
+        <v>367</v>
+      </c>
+      <c r="E74" t="s">
+        <v>491</v>
+      </c>
+      <c r="F74" s="24" t="s">
+        <v>430</v>
+      </c>
+      <c r="G74" s="20" t="s">
+        <v>376</v>
+      </c>
+      <c r="H74" t="s">
+        <v>61</v>
+      </c>
+      <c r="I74" t="s">
+        <v>573</v>
+      </c>
+      <c r="J74" s="5" t="s">
+        <v>464</v>
+      </c>
+      <c r="K74" s="56"/>
+      <c r="L74" s="20" t="s">
+        <v>606</v>
+      </c>
+      <c r="M74" s="20" t="s">
+        <v>430</v>
+      </c>
+      <c r="N74" s="63">
+        <v>1</v>
+      </c>
+      <c r="O74" s="20" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="75" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A75">
+        <v>18</v>
+      </c>
+      <c r="C75" s="67" t="s">
+        <v>370</v>
+      </c>
+      <c r="D75" s="20" t="s">
+        <v>371</v>
+      </c>
+      <c r="E75" t="s">
+        <v>492</v>
+      </c>
+      <c r="F75" s="24" t="s">
+        <v>375</v>
+      </c>
+      <c r="G75" s="20" t="s">
+        <v>376</v>
+      </c>
+      <c r="H75" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="I75" t="s">
+        <v>574</v>
+      </c>
+      <c r="J75" s="5" t="s">
+        <v>464</v>
+      </c>
+      <c r="K75" s="56"/>
+      <c r="L75" s="20" t="s">
+        <v>606</v>
+      </c>
+      <c r="M75" s="20" t="s">
+        <v>375</v>
+      </c>
+      <c r="N75" s="63">
+        <v>1</v>
+      </c>
+      <c r="O75" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="76" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A76">
+        <v>19</v>
+      </c>
+      <c r="C76" s="67" t="s">
+        <v>383</v>
+      </c>
+      <c r="D76" s="20" t="s">
+        <v>380</v>
+      </c>
+      <c r="E76" t="s">
+        <v>493</v>
+      </c>
+      <c r="F76" s="24" t="s">
+        <v>364</v>
+      </c>
+      <c r="G76" s="20" t="s">
+        <v>239</v>
+      </c>
+      <c r="H76" t="s">
+        <v>61</v>
+      </c>
+      <c r="I76" t="s">
+        <v>575</v>
+      </c>
+      <c r="J76" s="5" t="s">
+        <v>464</v>
+      </c>
+      <c r="K76" s="57"/>
+      <c r="L76" s="20" t="s">
+        <v>531</v>
+      </c>
+      <c r="M76" s="20" t="s">
+        <v>364</v>
+      </c>
+      <c r="N76" s="20" t="s">
+        <v>527</v>
+      </c>
+      <c r="O76" s="20" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="77" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A77">
+        <v>20</v>
+      </c>
+      <c r="C77" s="67" t="s">
+        <v>384</v>
+      </c>
+      <c r="D77" s="20" t="s">
+        <v>381</v>
+      </c>
+      <c r="E77" t="s">
+        <v>494</v>
+      </c>
+      <c r="F77" s="24" t="s">
+        <v>112</v>
+      </c>
+      <c r="G77" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="H77" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="I77" t="s">
+        <v>576</v>
+      </c>
+      <c r="J77" s="5" t="s">
+        <v>465</v>
+      </c>
+      <c r="K77" s="57"/>
+      <c r="L77" s="20" t="s">
+        <v>531</v>
+      </c>
+      <c r="M77" s="20" t="s">
+        <v>232</v>
+      </c>
+      <c r="N77" s="63">
+        <v>1</v>
+      </c>
+      <c r="O77" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="78" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A78">
+        <v>21</v>
+      </c>
+      <c r="C78" s="67" t="s">
+        <v>388</v>
+      </c>
+      <c r="D78" s="20" t="s">
+        <v>387</v>
+      </c>
+      <c r="E78" t="s">
+        <v>495</v>
+      </c>
+      <c r="F78" s="24" t="s">
+        <v>232</v>
+      </c>
+      <c r="G78" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="H78" t="s">
+        <v>61</v>
+      </c>
+      <c r="I78" t="s">
+        <v>577</v>
+      </c>
+      <c r="J78" s="5" t="s">
+        <v>465</v>
+      </c>
+      <c r="K78" s="57"/>
+      <c r="L78" s="20" t="s">
+        <v>531</v>
+      </c>
+      <c r="M78" s="20" t="s">
+        <v>232</v>
+      </c>
+      <c r="N78" s="63">
+        <v>1</v>
+      </c>
+      <c r="O78" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="79" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A79">
+        <v>22</v>
+      </c>
+      <c r="C79" s="67" t="s">
+        <v>390</v>
+      </c>
+      <c r="D79" s="20" t="s">
+        <v>391</v>
+      </c>
+      <c r="E79" t="s">
+        <v>496</v>
+      </c>
+      <c r="F79" s="24" t="s">
+        <v>232</v>
+      </c>
+      <c r="G79" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="H79" t="s">
+        <v>61</v>
+      </c>
+      <c r="I79" t="s">
+        <v>578</v>
+      </c>
+      <c r="J79" s="5" t="s">
+        <v>465</v>
+      </c>
+      <c r="K79" s="57"/>
+      <c r="L79" s="20" t="s">
+        <v>531</v>
+      </c>
+      <c r="M79" s="20" t="s">
+        <v>232</v>
+      </c>
+      <c r="N79" s="63">
+        <v>1</v>
+      </c>
+      <c r="O79" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="80" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A80">
+        <v>23</v>
+      </c>
+      <c r="C80" s="67" t="s">
+        <v>395</v>
+      </c>
+      <c r="D80" s="20" t="s">
+        <v>393</v>
+      </c>
+      <c r="E80" t="s">
+        <v>497</v>
+      </c>
+      <c r="F80" s="24" t="s">
+        <v>396</v>
+      </c>
+      <c r="G80" s="20" t="s">
+        <v>239</v>
+      </c>
+      <c r="H80" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="I80" t="s">
+        <v>579</v>
+      </c>
+      <c r="J80" s="5" t="s">
+        <v>465</v>
+      </c>
+      <c r="K80" s="57"/>
+      <c r="L80" s="20" t="s">
+        <v>531</v>
+      </c>
+      <c r="M80" s="20" t="s">
+        <v>396</v>
+      </c>
+      <c r="N80" s="64">
+        <v>1</v>
+      </c>
+      <c r="O80" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="81" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A81">
+        <v>24</v>
+      </c>
+      <c r="C81" s="67" t="s">
+        <v>398</v>
+      </c>
+      <c r="D81" s="20" t="s">
+        <v>399</v>
+      </c>
+      <c r="E81" t="s">
+        <v>498</v>
+      </c>
+      <c r="F81" s="24" t="s">
+        <v>232</v>
+      </c>
+      <c r="G81" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="H81" t="s">
+        <v>61</v>
+      </c>
+      <c r="I81" t="s">
+        <v>580</v>
+      </c>
+      <c r="J81" s="5" t="s">
+        <v>465</v>
+      </c>
+      <c r="K81" s="57"/>
+      <c r="L81" s="20" t="s">
+        <v>531</v>
+      </c>
+      <c r="M81" s="20" t="s">
+        <v>232</v>
+      </c>
+      <c r="N81" s="64">
+        <v>1</v>
+      </c>
+      <c r="O81" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="82" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A82">
+        <v>25</v>
+      </c>
+      <c r="C82" s="67" t="s">
+        <v>433</v>
+      </c>
+      <c r="D82" s="20" t="s">
+        <v>434</v>
+      </c>
+      <c r="E82" s="5" t="s">
+        <v>435</v>
+      </c>
+      <c r="F82" s="24" t="s">
+        <v>436</v>
+      </c>
+      <c r="G82" s="20" t="s">
+        <v>126</v>
+      </c>
+      <c r="H82" t="s">
+        <v>61</v>
+      </c>
+      <c r="I82" t="s">
+        <v>437</v>
+      </c>
+      <c r="J82" s="5" t="s">
+        <v>464</v>
+      </c>
+      <c r="K82" s="56"/>
+      <c r="L82" s="20" t="s">
+        <v>467</v>
+      </c>
+      <c r="M82" s="23" t="s">
+        <v>436</v>
+      </c>
+      <c r="N82" t="s">
+        <v>524</v>
+      </c>
+      <c r="O82" s="20" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="83" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A83">
+        <v>26</v>
+      </c>
+      <c r="C83" s="8" t="s">
+        <v>511</v>
+      </c>
+      <c r="D83" s="20" t="s">
+        <v>512</v>
+      </c>
+      <c r="E83" s="5" t="s">
+        <v>510</v>
+      </c>
+      <c r="F83" s="24" t="s">
+        <v>263</v>
+      </c>
+      <c r="G83" s="20" t="s">
+        <v>239</v>
+      </c>
+      <c r="H83" t="s">
+        <v>61</v>
+      </c>
+      <c r="I83" t="s">
+        <v>513</v>
+      </c>
+      <c r="J83" s="5" t="s">
+        <v>466</v>
+      </c>
+      <c r="K83" s="56"/>
+      <c r="L83" s="20" t="s">
+        <v>463</v>
+      </c>
+      <c r="M83" s="23" t="s">
+        <v>263</v>
+      </c>
+      <c r="N83" s="20" t="s">
+        <v>504</v>
+      </c>
+      <c r="O83" s="20" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="84" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A84">
+        <v>27</v>
+      </c>
+      <c r="C84" s="8" t="s">
+        <v>515</v>
+      </c>
+      <c r="D84" s="20" t="s">
+        <v>516</v>
+      </c>
+      <c r="E84" s="5" t="s">
+        <v>514</v>
+      </c>
+      <c r="F84" s="24" t="s">
+        <v>263</v>
+      </c>
+      <c r="G84" s="20" t="s">
+        <v>239</v>
+      </c>
+      <c r="H84" t="s">
+        <v>61</v>
+      </c>
+      <c r="I84" t="s">
+        <v>517</v>
+      </c>
+      <c r="J84" s="5" t="s">
+        <v>466</v>
+      </c>
+      <c r="K84" s="56"/>
+      <c r="L84" s="20" t="s">
+        <v>463</v>
+      </c>
+      <c r="M84" s="23" t="s">
+        <v>263</v>
+      </c>
+      <c r="N84" s="20" t="s">
+        <v>518</v>
+      </c>
+      <c r="O84" s="20" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="85" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A85">
+        <v>28</v>
+      </c>
+      <c r="C85" s="66" t="s">
+        <v>584</v>
+      </c>
+      <c r="D85" s="20" t="s">
+        <v>585</v>
+      </c>
+      <c r="E85" s="20" t="s">
+        <v>586</v>
+      </c>
+      <c r="F85" s="24" t="s">
+        <v>589</v>
+      </c>
+      <c r="G85" s="20" t="s">
+        <v>608</v>
+      </c>
+      <c r="H85" t="s">
+        <v>61</v>
+      </c>
+      <c r="I85" t="s">
+        <v>588</v>
+      </c>
+      <c r="J85" s="5" t="s">
+        <v>466</v>
+      </c>
+      <c r="K85" s="57"/>
+      <c r="L85" s="20" t="s">
+        <v>592</v>
+      </c>
+      <c r="M85" s="23" t="s">
+        <v>589</v>
+      </c>
+      <c r="N85" s="20" t="s">
+        <v>504</v>
+      </c>
+      <c r="O85" s="20" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="86" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A86">
+        <v>29</v>
+      </c>
+      <c r="C86" s="66" t="s">
+        <v>594</v>
+      </c>
+      <c r="D86" s="20" t="s">
+        <v>595</v>
+      </c>
+      <c r="E86" s="20" t="s">
+        <v>596</v>
+      </c>
+      <c r="F86" s="24" t="s">
+        <v>600</v>
+      </c>
+      <c r="G86" s="20" t="s">
+        <v>321</v>
+      </c>
+      <c r="H86" t="s">
+        <v>61</v>
+      </c>
+      <c r="I86" t="s">
+        <v>598</v>
+      </c>
+      <c r="J86" s="5" t="s">
+        <v>466</v>
+      </c>
+      <c r="K86" s="56"/>
+      <c r="L86" s="20" t="s">
+        <v>601</v>
+      </c>
+      <c r="M86" s="23" t="s">
+        <v>600</v>
+      </c>
+      <c r="N86" s="20" t="s">
+        <v>504</v>
+      </c>
+      <c r="O86" s="20" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="87" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="C87" s="5"/>
+      <c r="J87" s="5"/>
+      <c r="K87" s="5"/>
+      <c r="L87" s="5"/>
+      <c r="M87" s="5"/>
+      <c r="N87" s="5"/>
+    </row>
+    <row r="88" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B88" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="C88" s="27"/>
+      <c r="D88" s="27"/>
+      <c r="E88" s="27"/>
+      <c r="F88" s="27"/>
+      <c r="G88" s="27"/>
+      <c r="H88" s="28"/>
+      <c r="K88" s="58" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="89" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="C89" s="24" t="s">
+        <v>82</v>
+      </c>
+      <c r="K89" s="59"/>
+      <c r="L89" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="90" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="C90" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="D90" s="42" t="s">
+        <v>84</v>
+      </c>
+      <c r="E90" t="s">
+        <v>85</v>
+      </c>
+      <c r="K90" s="60"/>
+      <c r="L90" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="91" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="C91" t="s">
+        <v>423</v>
+      </c>
+      <c r="D91" s="42" t="s">
+        <v>431</v>
+      </c>
+      <c r="K91" s="70"/>
+      <c r="L91" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="92" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="C92" t="s">
+        <v>424</v>
+      </c>
+      <c r="D92" s="42" t="s">
+        <v>431</v>
+      </c>
+      <c r="E92" s="47" t="s">
+        <v>280</v>
+      </c>
+      <c r="K92" s="61"/>
+      <c r="L92" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="93" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C93" t="s">
+        <v>425</v>
+      </c>
+      <c r="D93" s="42" t="s">
+        <v>431</v>
+      </c>
+      <c r="E93" s="47" t="s">
+        <v>280</v>
+      </c>
+      <c r="J93" s="62" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="94" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="C94" t="s">
+        <v>426</v>
+      </c>
+      <c r="D94" s="42" t="s">
+        <v>431</v>
+      </c>
+      <c r="E94" s="47" t="s">
+        <v>280</v>
+      </c>
+      <c r="J94" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="K94" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="95" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="C95" t="s">
+        <v>427</v>
+      </c>
+      <c r="D95" s="42" t="s">
+        <v>431</v>
+      </c>
+      <c r="E95" s="47" t="s">
+        <v>280</v>
+      </c>
+      <c r="J95" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="K95" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="96" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="C96" t="s">
+        <v>428</v>
+      </c>
+      <c r="D96" s="42" t="s">
+        <v>431</v>
+      </c>
+      <c r="E96" s="47" t="s">
+        <v>280</v>
+      </c>
+      <c r="J96" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="K96" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="97" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="J97" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="K97" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="98" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B98" s="26" t="s">
+        <v>104</v>
+      </c>
+      <c r="C98" s="27"/>
+      <c r="D98" s="27"/>
+      <c r="E98" s="27"/>
+      <c r="F98" s="27"/>
+      <c r="G98" s="27"/>
+      <c r="H98" s="28"/>
+    </row>
+    <row r="99" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C99" s="24" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="100" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C100" t="s">
+        <v>277</v>
+      </c>
+      <c r="D100" s="42" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="101" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C101" t="s">
+        <v>278</v>
+      </c>
+      <c r="D101" s="42" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="102" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C102" t="s">
+        <v>279</v>
+      </c>
+      <c r="D102" s="42" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="103" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C103" s="5"/>
+      <c r="D103" s="5"/>
+    </row>
+    <row r="104" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C104" s="5"/>
+      <c r="D104" s="5"/>
+    </row>
+    <row r="105" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B105" s="26" t="s">
+        <v>417</v>
+      </c>
+      <c r="C105" s="27"/>
+      <c r="D105" s="27"/>
+      <c r="E105" s="27"/>
+      <c r="F105" s="27"/>
+      <c r="G105" s="27"/>
+      <c r="H105" s="28"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:K100"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A52" sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="E49" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C74" sqref="C74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3846,1670 +6752,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:K100"/>
-  <sheetViews>
-    <sheetView topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="17.77734375" customWidth="1"/>
-    <col min="3" max="3" width="41.88671875" customWidth="1"/>
-    <col min="4" max="4" width="65.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="50.6640625" customWidth="1"/>
-    <col min="6" max="6" width="27.44140625" customWidth="1"/>
-    <col min="7" max="7" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="43.77734375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B2" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="28"/>
-    </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="C3" s="31" t="s">
-        <v>57</v>
-      </c>
-      <c r="D3" s="41" t="s">
-        <v>56</v>
-      </c>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-    </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="42" t="s">
-        <v>458</v>
-      </c>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
-      <c r="K4" s="20"/>
-    </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="C5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D5" s="42" t="s">
-        <v>282</v>
-      </c>
-      <c r="I5" s="20"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="20"/>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="C6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="43" t="s">
-        <v>459</v>
-      </c>
-      <c r="I6" s="20"/>
-      <c r="J6" s="20"/>
-      <c r="K6" s="20"/>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="D7" s="11"/>
-      <c r="I7" s="20"/>
-      <c r="J7" s="19"/>
-      <c r="K7" s="20"/>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B8" s="26" t="s">
-        <v>80</v>
-      </c>
-      <c r="C8" s="27"/>
-      <c r="D8" s="27"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="27"/>
-      <c r="G8" s="27"/>
-      <c r="H8" s="28"/>
-      <c r="I8" s="20"/>
-      <c r="J8" s="19"/>
-      <c r="K8" s="20"/>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="C9" s="31" t="s">
-        <v>57</v>
-      </c>
-      <c r="D9" s="41" t="s">
-        <v>207</v>
-      </c>
-      <c r="E9" s="31"/>
-      <c r="F9" s="39"/>
-      <c r="G9" s="39"/>
-      <c r="H9" s="39"/>
-      <c r="I9" s="20"/>
-      <c r="J9" s="19"/>
-      <c r="K9" s="20"/>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="C10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="42" t="s">
-        <v>309</v>
-      </c>
-      <c r="I10" s="20"/>
-      <c r="J10" s="19"/>
-      <c r="K10" s="20"/>
-    </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="C11" t="s">
-        <v>267</v>
-      </c>
-      <c r="D11" s="50" t="s">
-        <v>312</v>
-      </c>
-      <c r="I11" s="20"/>
-      <c r="J11" s="19"/>
-      <c r="K11" s="20"/>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="C12" t="s">
-        <v>268</v>
-      </c>
-      <c r="D12" s="50" t="s">
-        <v>312</v>
-      </c>
-      <c r="I12" s="20"/>
-      <c r="J12" s="19"/>
-      <c r="K12" s="20"/>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="I13" s="20"/>
-      <c r="J13" s="25"/>
-      <c r="K13" s="20"/>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B14" s="26" t="s">
-        <v>115</v>
-      </c>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27" t="s">
-        <v>116</v>
-      </c>
-      <c r="E14" s="27"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="27"/>
-      <c r="H14" s="28"/>
-      <c r="I14" s="36" t="s">
-        <v>439</v>
-      </c>
-      <c r="J14" s="20"/>
-      <c r="K14" s="20"/>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="C15" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="D15" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="E15" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="F15" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="G15" s="31" t="s">
-        <v>438</v>
-      </c>
-      <c r="H15" s="30" t="s">
-        <v>186</v>
-      </c>
-      <c r="I15" s="52" t="s">
-        <v>187</v>
-      </c>
-      <c r="K15" s="20"/>
-    </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="C16" s="33" t="s">
-        <v>16</v>
-      </c>
-      <c r="D16" t="s">
-        <v>28</v>
-      </c>
-      <c r="E16" t="s">
-        <v>16</v>
-      </c>
-      <c r="F16" t="s">
-        <v>16</v>
-      </c>
-      <c r="G16" s="5" t="s">
-        <v>281</v>
-      </c>
-      <c r="H16" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="I16" s="20" t="s">
-        <v>188</v>
-      </c>
-      <c r="J16" s="20"/>
-      <c r="K16" s="20"/>
-    </row>
-    <row r="17" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="C17" s="33" t="s">
-        <v>17</v>
-      </c>
-      <c r="D17" t="s">
-        <v>29</v>
-      </c>
-      <c r="E17" t="s">
-        <v>16</v>
-      </c>
-      <c r="F17" t="s">
-        <v>16</v>
-      </c>
-      <c r="G17" s="5" t="s">
-        <v>429</v>
-      </c>
-      <c r="H17" s="29" t="s">
-        <v>52</v>
-      </c>
-      <c r="I17" s="20" t="s">
-        <v>189</v>
-      </c>
-      <c r="J17" s="20"/>
-      <c r="K17" s="20"/>
-    </row>
-    <row r="18" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="C18" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="D18" t="s">
-        <v>37</v>
-      </c>
-      <c r="E18" t="s">
-        <v>23</v>
-      </c>
-      <c r="F18" t="s">
-        <v>42</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>449</v>
-      </c>
-      <c r="H18" s="29" t="s">
-        <v>51</v>
-      </c>
-      <c r="I18" s="20" t="s">
-        <v>190</v>
-      </c>
-      <c r="J18" s="20"/>
-      <c r="K18" s="20"/>
-    </row>
-    <row r="19" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="C19" s="33" t="s">
-        <v>24</v>
-      </c>
-      <c r="D19" t="s">
-        <v>38</v>
-      </c>
-      <c r="E19" t="s">
-        <v>24</v>
-      </c>
-      <c r="F19" t="s">
-        <v>24</v>
-      </c>
-      <c r="G19" t="s">
-        <v>418</v>
-      </c>
-      <c r="H19" s="29">
-        <v>1</v>
-      </c>
-      <c r="I19" s="20" t="s">
-        <v>192</v>
-      </c>
-      <c r="J19" s="20"/>
-      <c r="K19" s="20"/>
-    </row>
-    <row r="20" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="C20" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="D20" t="s">
-        <v>31</v>
-      </c>
-      <c r="E20" t="s">
-        <v>39</v>
-      </c>
-      <c r="F20" t="s">
-        <v>40</v>
-      </c>
-      <c r="G20" t="s">
-        <v>276</v>
-      </c>
-      <c r="H20" s="29" t="s">
-        <v>45</v>
-      </c>
-      <c r="I20" s="20" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="21" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="C21" s="45" t="s">
-        <v>142</v>
-      </c>
-      <c r="D21" t="s">
-        <v>150</v>
-      </c>
-      <c r="E21" t="s">
-        <v>26</v>
-      </c>
-      <c r="F21" t="s">
-        <v>155</v>
-      </c>
-      <c r="G21" t="s">
-        <v>457</v>
-      </c>
-      <c r="H21" s="29" t="s">
-        <v>184</v>
-      </c>
-      <c r="I21" s="20" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="22" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="C22" s="45" t="s">
-        <v>143</v>
-      </c>
-      <c r="D22" t="s">
-        <v>151</v>
-      </c>
-      <c r="E22" t="s">
-        <v>26</v>
-      </c>
-      <c r="F22" t="s">
-        <v>156</v>
-      </c>
-      <c r="G22" t="s">
-        <v>420</v>
-      </c>
-      <c r="H22" s="29" t="s">
-        <v>179</v>
-      </c>
-      <c r="I22" s="20" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="23" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="C23" s="45" t="s">
-        <v>144</v>
-      </c>
-      <c r="D23" t="s">
-        <v>152</v>
-      </c>
-      <c r="E23" t="s">
-        <v>26</v>
-      </c>
-      <c r="F23" t="s">
-        <v>157</v>
-      </c>
-      <c r="G23" t="s">
-        <v>420</v>
-      </c>
-      <c r="H23" s="29" t="s">
-        <v>178</v>
-      </c>
-      <c r="I23" s="20" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="24" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="C24" s="45" t="s">
-        <v>145</v>
-      </c>
-      <c r="D24" t="s">
-        <v>148</v>
-      </c>
-      <c r="E24" t="s">
-        <v>26</v>
-      </c>
-      <c r="F24" t="s">
-        <v>106</v>
-      </c>
-      <c r="G24" t="s">
-        <v>290</v>
-      </c>
-      <c r="H24" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="I24" s="20" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="25" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="C25" s="45" t="s">
-        <v>163</v>
-      </c>
-      <c r="D25" t="s">
-        <v>159</v>
-      </c>
-      <c r="E25" t="s">
-        <v>21</v>
-      </c>
-      <c r="F25" t="s">
-        <v>134</v>
-      </c>
-      <c r="G25" t="s">
-        <v>454</v>
-      </c>
-      <c r="H25" s="29" t="s">
-        <v>337</v>
-      </c>
-      <c r="I25" s="20" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="26" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="C26" s="45" t="s">
-        <v>20</v>
-      </c>
-      <c r="D26" t="s">
-        <v>32</v>
-      </c>
-      <c r="E26" t="s">
-        <v>21</v>
-      </c>
-      <c r="F26" t="s">
-        <v>105</v>
-      </c>
-      <c r="G26" t="s">
-        <v>420</v>
-      </c>
-      <c r="H26" s="29" t="s">
-        <v>181</v>
-      </c>
-      <c r="I26" s="20" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="27" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="C27" s="45" t="s">
-        <v>331</v>
-      </c>
-      <c r="D27" t="s">
-        <v>332</v>
-      </c>
-      <c r="E27" t="s">
-        <v>21</v>
-      </c>
-      <c r="F27" t="s">
-        <v>333</v>
-      </c>
-      <c r="G27" t="s">
-        <v>334</v>
-      </c>
-      <c r="H27" s="29" t="s">
-        <v>335</v>
-      </c>
-      <c r="I27" s="20" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="28" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="C28" s="45" t="s">
-        <v>164</v>
-      </c>
-      <c r="D28" t="s">
-        <v>165</v>
-      </c>
-      <c r="E28" t="s">
-        <v>21</v>
-      </c>
-      <c r="F28" t="s">
-        <v>166</v>
-      </c>
-      <c r="G28" t="s">
-        <v>420</v>
-      </c>
-      <c r="H28" s="29" t="s">
-        <v>205</v>
-      </c>
-      <c r="I28" s="20" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="29" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="C29" s="45" t="s">
-        <v>22</v>
-      </c>
-      <c r="D29" t="s">
-        <v>34</v>
-      </c>
-      <c r="E29" t="s">
-        <v>21</v>
-      </c>
-      <c r="F29" t="s">
-        <v>117</v>
-      </c>
-      <c r="G29" t="s">
-        <v>289</v>
-      </c>
-      <c r="H29" s="29" t="s">
-        <v>182</v>
-      </c>
-      <c r="I29" s="20" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="30" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="C30" s="45" t="s">
-        <v>167</v>
-      </c>
-      <c r="D30" t="s">
-        <v>170</v>
-      </c>
-      <c r="E30" t="s">
-        <v>169</v>
-      </c>
-      <c r="F30" t="s">
-        <v>168</v>
-      </c>
-      <c r="G30" t="s">
-        <v>287</v>
-      </c>
-      <c r="H30" s="29" t="s">
-        <v>185</v>
-      </c>
-      <c r="I30" s="20" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="31" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="C31" s="45" t="s">
-        <v>25</v>
-      </c>
-      <c r="D31" t="s">
-        <v>171</v>
-      </c>
-      <c r="E31" t="s">
-        <v>25</v>
-      </c>
-      <c r="F31" t="s">
-        <v>41</v>
-      </c>
-      <c r="G31" t="s">
-        <v>418</v>
-      </c>
-      <c r="H31" s="29" t="s">
-        <v>44</v>
-      </c>
-      <c r="I31" s="20" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="32" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="C32" s="45" t="s">
-        <v>173</v>
-      </c>
-      <c r="D32" t="s">
-        <v>174</v>
-      </c>
-      <c r="E32" t="s">
-        <v>173</v>
-      </c>
-      <c r="F32" t="s">
-        <v>172</v>
-      </c>
-      <c r="G32" s="5" t="s">
-        <v>419</v>
-      </c>
-      <c r="H32" s="29" t="s">
-        <v>183</v>
-      </c>
-      <c r="I32" s="20" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="C33" s="33" t="s">
-        <v>283</v>
-      </c>
-      <c r="D33" t="s">
-        <v>284</v>
-      </c>
-      <c r="E33" t="s">
-        <v>25</v>
-      </c>
-      <c r="F33" t="s">
-        <v>285</v>
-      </c>
-      <c r="G33" s="20" t="s">
-        <v>418</v>
-      </c>
-      <c r="H33" s="29" t="s">
-        <v>286</v>
-      </c>
-      <c r="I33" s="20" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="C34" s="45" t="s">
-        <v>294</v>
-      </c>
-      <c r="D34" t="s">
-        <v>295</v>
-      </c>
-      <c r="E34" t="s">
-        <v>25</v>
-      </c>
-      <c r="F34" t="s">
-        <v>251</v>
-      </c>
-      <c r="G34" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="H34" s="29" t="s">
-        <v>254</v>
-      </c>
-      <c r="I34" s="20" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B37" s="26" t="s">
-        <v>101</v>
-      </c>
-      <c r="C37" s="27"/>
-      <c r="D37" s="27"/>
-      <c r="E37" s="27"/>
-      <c r="F37" s="27"/>
-      <c r="G37" s="27"/>
-      <c r="H37" s="28"/>
-    </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="C38" s="34" t="s">
-        <v>102</v>
-      </c>
-      <c r="D38" s="31" t="s">
-        <v>103</v>
-      </c>
-      <c r="E38" s="31" t="s">
-        <v>65</v>
-      </c>
-      <c r="F38" s="31" t="s">
-        <v>66</v>
-      </c>
-      <c r="G38" s="39"/>
-      <c r="H38" s="39"/>
-    </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="C39" s="53">
-        <v>1</v>
-      </c>
-      <c r="D39" t="s">
-        <v>455</v>
-      </c>
-      <c r="E39" t="s">
-        <v>405</v>
-      </c>
-      <c r="F39" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="C40" s="53">
-        <v>2</v>
-      </c>
-      <c r="D40" t="s">
-        <v>456</v>
-      </c>
-      <c r="E40" t="s">
-        <v>404</v>
-      </c>
-      <c r="F40" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="C41" s="53">
-        <v>3</v>
-      </c>
-      <c r="D41" t="s">
-        <v>450</v>
-      </c>
-      <c r="E41" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="C42" s="53">
-        <v>4</v>
-      </c>
-      <c r="D42" t="s">
-        <v>452</v>
-      </c>
-      <c r="E42" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="C43" s="53">
-        <v>5</v>
-      </c>
-      <c r="D43" t="s">
-        <v>451</v>
-      </c>
-      <c r="E43" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="C44" s="53">
-        <v>6</v>
-      </c>
-      <c r="D44" t="s">
-        <v>453</v>
-      </c>
-      <c r="E44" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="C45" s="53">
-        <v>7</v>
-      </c>
-      <c r="D45" t="s">
-        <v>407</v>
-      </c>
-      <c r="E45" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="46" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="C46" s="53">
-        <v>8</v>
-      </c>
-      <c r="D46" t="s">
-        <v>408</v>
-      </c>
-      <c r="E46" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="47" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="C47" s="53">
-        <v>9</v>
-      </c>
-      <c r="D47" t="s">
-        <v>409</v>
-      </c>
-      <c r="E47" t="s">
-        <v>405</v>
-      </c>
-      <c r="F47" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="48" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="C48" s="53">
-        <v>10</v>
-      </c>
-      <c r="D48" t="s">
-        <v>410</v>
-      </c>
-      <c r="E48" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C49" s="53">
-        <v>11</v>
-      </c>
-      <c r="D49" t="s">
-        <v>411</v>
-      </c>
-      <c r="E49" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C50" s="53">
-        <v>12</v>
-      </c>
-      <c r="D50" t="s">
-        <v>412</v>
-      </c>
-      <c r="E50" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C51" s="53">
-        <v>13</v>
-      </c>
-      <c r="D51" t="s">
-        <v>415</v>
-      </c>
-      <c r="E51" t="s">
-        <v>405</v>
-      </c>
-      <c r="F51" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C52" s="53">
-        <v>14</v>
-      </c>
-      <c r="D52" t="s">
-        <v>416</v>
-      </c>
-      <c r="E52" t="s">
-        <v>404</v>
-      </c>
-      <c r="F52" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C53" s="5"/>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B55" s="26" t="s">
-        <v>55</v>
-      </c>
-      <c r="C55" s="27"/>
-      <c r="D55" s="27"/>
-      <c r="E55" s="27"/>
-      <c r="F55" s="27"/>
-      <c r="G55" s="27"/>
-      <c r="H55" s="28"/>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C56" s="34" t="s">
-        <v>58</v>
-      </c>
-      <c r="D56" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="E56" s="31" t="s">
-        <v>107</v>
-      </c>
-      <c r="F56" s="31" t="s">
-        <v>59</v>
-      </c>
-      <c r="G56" s="31" t="s">
-        <v>71</v>
-      </c>
-      <c r="H56" s="31" t="s">
-        <v>60</v>
-      </c>
-      <c r="I56" s="51" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A57">
-        <v>0</v>
-      </c>
-      <c r="C57" s="35" t="s">
-        <v>292</v>
-      </c>
-      <c r="D57" t="s">
-        <v>293</v>
-      </c>
-      <c r="E57" s="20" t="s">
-        <v>291</v>
-      </c>
-      <c r="F57" s="24" t="s">
-        <v>263</v>
-      </c>
-      <c r="G57" t="s">
-        <v>239</v>
-      </c>
-      <c r="H57" t="s">
-        <v>61</v>
-      </c>
-      <c r="I57" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A58">
-        <v>1</v>
-      </c>
-      <c r="C58" s="35" t="s">
-        <v>300</v>
-      </c>
-      <c r="D58" t="s">
-        <v>301</v>
-      </c>
-      <c r="E58" s="20" t="s">
-        <v>299</v>
-      </c>
-      <c r="F58" s="46" t="s">
-        <v>303</v>
-      </c>
-      <c r="G58" s="20" t="s">
-        <v>239</v>
-      </c>
-      <c r="H58" t="s">
-        <v>61</v>
-      </c>
-      <c r="I58" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A59">
-        <v>2</v>
-      </c>
-      <c r="C59" s="35" t="s">
-        <v>305</v>
-      </c>
-      <c r="D59" t="s">
-        <v>306</v>
-      </c>
-      <c r="E59" s="20" t="s">
-        <v>304</v>
-      </c>
-      <c r="F59" s="46" t="s">
-        <v>308</v>
-      </c>
-      <c r="G59" s="20" t="s">
-        <v>239</v>
-      </c>
-      <c r="H59" t="s">
-        <v>61</v>
-      </c>
-      <c r="I59" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A60">
-        <v>3</v>
-      </c>
-      <c r="C60" s="35" t="s">
-        <v>315</v>
-      </c>
-      <c r="D60" s="20" t="s">
-        <v>317</v>
-      </c>
-      <c r="E60" t="s">
-        <v>313</v>
-      </c>
-      <c r="F60" s="46" t="s">
-        <v>432</v>
-      </c>
-      <c r="G60" s="20" t="s">
-        <v>321</v>
-      </c>
-      <c r="H60" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="I60" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A61">
-        <v>4</v>
-      </c>
-      <c r="C61" s="35" t="s">
-        <v>316</v>
-      </c>
-      <c r="D61" s="20" t="s">
-        <v>318</v>
-      </c>
-      <c r="E61" t="s">
-        <v>314</v>
-      </c>
-      <c r="F61" s="24" t="s">
-        <v>320</v>
-      </c>
-      <c r="G61" s="20" t="s">
-        <v>239</v>
-      </c>
-      <c r="H61" t="s">
-        <v>61</v>
-      </c>
-      <c r="I61" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A62">
-        <v>5</v>
-      </c>
-      <c r="C62" s="35" t="s">
-        <v>329</v>
-      </c>
-      <c r="D62" s="20" t="s">
-        <v>325</v>
-      </c>
-      <c r="E62" t="s">
-        <v>323</v>
-      </c>
-      <c r="F62" s="24" t="s">
-        <v>275</v>
-      </c>
-      <c r="G62" s="20" t="s">
-        <v>113</v>
-      </c>
-      <c r="H62" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="I62" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A63">
-        <v>6</v>
-      </c>
-      <c r="C63" s="35" t="s">
-        <v>330</v>
-      </c>
-      <c r="D63" s="20" t="s">
-        <v>328</v>
-      </c>
-      <c r="E63" t="s">
-        <v>326</v>
-      </c>
-      <c r="F63" s="24" t="s">
-        <v>339</v>
-      </c>
-      <c r="G63" s="20" t="s">
-        <v>321</v>
-      </c>
-      <c r="H63" t="s">
-        <v>61</v>
-      </c>
-      <c r="I63" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A64">
-        <v>7</v>
-      </c>
-      <c r="C64" s="35" t="s">
-        <v>343</v>
-      </c>
-      <c r="D64" s="20" t="s">
-        <v>342</v>
-      </c>
-      <c r="E64" s="5" t="s">
-        <v>341</v>
-      </c>
-      <c r="F64" s="24" t="s">
-        <v>339</v>
-      </c>
-      <c r="G64" s="20" t="s">
-        <v>321</v>
-      </c>
-      <c r="H64" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="I64" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A65">
-        <v>8</v>
-      </c>
-      <c r="C65" s="35" t="s">
-        <v>442</v>
-      </c>
-      <c r="D65" s="20" t="s">
-        <v>440</v>
-      </c>
-      <c r="E65" s="5" t="s">
-        <v>444</v>
-      </c>
-      <c r="F65" s="24" t="s">
-        <v>448</v>
-      </c>
-      <c r="G65" s="20" t="s">
-        <v>126</v>
-      </c>
-      <c r="H65" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="I65" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A66">
-        <v>9</v>
-      </c>
-      <c r="C66" s="35" t="s">
-        <v>443</v>
-      </c>
-      <c r="D66" s="20" t="s">
-        <v>441</v>
-      </c>
-      <c r="E66" s="5" t="s">
-        <v>445</v>
-      </c>
-      <c r="F66" s="24" t="s">
-        <v>448</v>
-      </c>
-      <c r="G66" s="20" t="s">
-        <v>126</v>
-      </c>
-      <c r="H66" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="I66" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A67">
-        <v>10</v>
-      </c>
-      <c r="C67" s="35" t="s">
-        <v>345</v>
-      </c>
-      <c r="D67" s="20" t="s">
-        <v>346</v>
-      </c>
-      <c r="E67" s="5" t="s">
-        <v>344</v>
-      </c>
-      <c r="F67" s="24" t="s">
-        <v>348</v>
-      </c>
-      <c r="G67" s="20" t="s">
-        <v>239</v>
-      </c>
-      <c r="H67" t="s">
-        <v>61</v>
-      </c>
-      <c r="I67" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A68">
-        <v>11</v>
-      </c>
-      <c r="C68" s="35" t="s">
-        <v>351</v>
-      </c>
-      <c r="D68" s="20" t="s">
-        <v>350</v>
-      </c>
-      <c r="E68" t="s">
-        <v>349</v>
-      </c>
-      <c r="F68" s="24" t="s">
-        <v>348</v>
-      </c>
-      <c r="G68" s="20" t="s">
-        <v>239</v>
-      </c>
-      <c r="H68" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="I68" s="36" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A69">
-        <v>12</v>
-      </c>
-      <c r="C69" s="35" t="s">
-        <v>359</v>
-      </c>
-      <c r="D69" s="20" t="s">
-        <v>356</v>
-      </c>
-      <c r="E69" t="s">
-        <v>353</v>
-      </c>
-      <c r="F69" s="24" t="s">
-        <v>354</v>
-      </c>
-      <c r="G69" s="20" t="s">
-        <v>239</v>
-      </c>
-      <c r="H69" t="s">
-        <v>61</v>
-      </c>
-      <c r="I69" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A70">
-        <v>13</v>
-      </c>
-      <c r="C70" s="35" t="s">
-        <v>360</v>
-      </c>
-      <c r="D70" s="20" t="s">
-        <v>401</v>
-      </c>
-      <c r="E70" s="5" t="s">
-        <v>357</v>
-      </c>
-      <c r="F70" s="46" t="s">
-        <v>421</v>
-      </c>
-      <c r="G70" s="20" t="s">
-        <v>239</v>
-      </c>
-      <c r="H70" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="I70" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A71">
-        <v>14</v>
-      </c>
-      <c r="C71" s="35" t="s">
-        <v>400</v>
-      </c>
-      <c r="D71" s="20" t="s">
-        <v>402</v>
-      </c>
-      <c r="E71" s="5" t="s">
-        <v>422</v>
-      </c>
-      <c r="F71" s="46" t="s">
-        <v>403</v>
-      </c>
-      <c r="G71" s="20" t="s">
-        <v>239</v>
-      </c>
-      <c r="H71" t="s">
-        <v>61</v>
-      </c>
-      <c r="I71" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A72">
-        <v>15</v>
-      </c>
-      <c r="C72" s="35" t="s">
-        <v>361</v>
-      </c>
-      <c r="D72" s="20" t="s">
-        <v>363</v>
-      </c>
-      <c r="E72" t="s">
-        <v>358</v>
-      </c>
-      <c r="F72" s="24" t="s">
-        <v>364</v>
-      </c>
-      <c r="G72" s="20" t="s">
-        <v>239</v>
-      </c>
-      <c r="H72" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="I72" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A73">
-        <v>16</v>
-      </c>
-      <c r="C73" s="35" t="s">
-        <v>366</v>
-      </c>
-      <c r="D73" s="20" t="s">
-        <v>367</v>
-      </c>
-      <c r="E73" t="s">
-        <v>365</v>
-      </c>
-      <c r="F73" s="24" t="s">
-        <v>430</v>
-      </c>
-      <c r="G73" s="20" t="s">
-        <v>376</v>
-      </c>
-      <c r="H73" t="s">
-        <v>61</v>
-      </c>
-      <c r="I73" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A74">
-        <v>17</v>
-      </c>
-      <c r="C74" s="35" t="s">
-        <v>370</v>
-      </c>
-      <c r="D74" s="20" t="s">
-        <v>371</v>
-      </c>
-      <c r="E74" t="s">
-        <v>369</v>
-      </c>
-      <c r="F74" s="24" t="s">
-        <v>375</v>
-      </c>
-      <c r="G74" s="20" t="s">
-        <v>376</v>
-      </c>
-      <c r="H74" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="I74" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A75">
-        <v>18</v>
-      </c>
-      <c r="C75" s="35" t="s">
-        <v>383</v>
-      </c>
-      <c r="D75" s="20" t="s">
-        <v>380</v>
-      </c>
-      <c r="E75" t="s">
-        <v>377</v>
-      </c>
-      <c r="F75" s="24" t="s">
-        <v>364</v>
-      </c>
-      <c r="G75" s="20" t="s">
-        <v>239</v>
-      </c>
-      <c r="H75" t="s">
-        <v>61</v>
-      </c>
-      <c r="I75" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A76">
-        <v>19</v>
-      </c>
-      <c r="C76" s="35" t="s">
-        <v>384</v>
-      </c>
-      <c r="D76" s="20" t="s">
-        <v>381</v>
-      </c>
-      <c r="E76" t="s">
-        <v>379</v>
-      </c>
-      <c r="F76" s="24" t="s">
-        <v>232</v>
-      </c>
-      <c r="G76" s="20" t="s">
-        <v>113</v>
-      </c>
-      <c r="H76" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="I76" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A77">
-        <v>20</v>
-      </c>
-      <c r="C77" s="35" t="s">
-        <v>388</v>
-      </c>
-      <c r="D77" s="20" t="s">
-        <v>387</v>
-      </c>
-      <c r="E77" t="s">
-        <v>386</v>
-      </c>
-      <c r="F77" s="24" t="s">
-        <v>232</v>
-      </c>
-      <c r="G77" s="20" t="s">
-        <v>113</v>
-      </c>
-      <c r="H77" t="s">
-        <v>61</v>
-      </c>
-      <c r="I77" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A78">
-        <v>21</v>
-      </c>
-      <c r="C78" s="35" t="s">
-        <v>390</v>
-      </c>
-      <c r="D78" s="20" t="s">
-        <v>391</v>
-      </c>
-      <c r="E78" t="s">
-        <v>389</v>
-      </c>
-      <c r="F78" s="24" t="s">
-        <v>232</v>
-      </c>
-      <c r="G78" s="20" t="s">
-        <v>113</v>
-      </c>
-      <c r="H78" t="s">
-        <v>61</v>
-      </c>
-      <c r="I78" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A79">
-        <v>22</v>
-      </c>
-      <c r="C79" s="35" t="s">
-        <v>395</v>
-      </c>
-      <c r="D79" s="20" t="s">
-        <v>393</v>
-      </c>
-      <c r="E79" t="s">
-        <v>394</v>
-      </c>
-      <c r="F79" s="24" t="s">
-        <v>396</v>
-      </c>
-      <c r="G79" s="20" t="s">
-        <v>239</v>
-      </c>
-      <c r="H79" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="I79" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A80">
-        <v>23</v>
-      </c>
-      <c r="C80" s="35" t="s">
-        <v>398</v>
-      </c>
-      <c r="D80" s="20" t="s">
-        <v>399</v>
-      </c>
-      <c r="E80" t="s">
-        <v>397</v>
-      </c>
-      <c r="F80" s="24" t="s">
-        <v>232</v>
-      </c>
-      <c r="G80" s="20" t="s">
-        <v>113</v>
-      </c>
-      <c r="H80" t="s">
-        <v>61</v>
-      </c>
-      <c r="I80" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A81">
-        <v>24</v>
-      </c>
-      <c r="C81" s="35" t="s">
-        <v>433</v>
-      </c>
-      <c r="D81" s="20" t="s">
-        <v>434</v>
-      </c>
-      <c r="E81" s="5" t="s">
-        <v>435</v>
-      </c>
-      <c r="F81" s="24" t="s">
-        <v>436</v>
-      </c>
-      <c r="G81" s="20" t="s">
-        <v>126</v>
-      </c>
-      <c r="H81" t="s">
-        <v>61</v>
-      </c>
-      <c r="I81" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C82" s="5"/>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B83" s="26" t="s">
-        <v>81</v>
-      </c>
-      <c r="C83" s="27"/>
-      <c r="D83" s="27"/>
-      <c r="E83" s="27"/>
-      <c r="F83" s="27"/>
-      <c r="G83" s="27"/>
-      <c r="H83" s="28"/>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C84" s="24" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C85" s="35" t="s">
-        <v>83</v>
-      </c>
-      <c r="D85" s="42" t="s">
-        <v>84</v>
-      </c>
-      <c r="E85" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C86" t="s">
-        <v>423</v>
-      </c>
-      <c r="D86" s="42" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C87" t="s">
-        <v>424</v>
-      </c>
-      <c r="D87" s="47" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C88" t="s">
-        <v>425</v>
-      </c>
-      <c r="D88" s="47" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C89" t="s">
-        <v>426</v>
-      </c>
-      <c r="D89" s="47" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C90" t="s">
-        <v>427</v>
-      </c>
-      <c r="D90" s="47" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C91" t="s">
-        <v>428</v>
-      </c>
-      <c r="D91" s="47" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B93" s="26" t="s">
-        <v>104</v>
-      </c>
-      <c r="C93" s="27"/>
-      <c r="D93" s="27"/>
-      <c r="E93" s="27"/>
-      <c r="F93" s="27"/>
-      <c r="G93" s="27"/>
-      <c r="H93" s="28"/>
-    </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C94" s="24" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C95" t="s">
-        <v>277</v>
-      </c>
-      <c r="D95" s="42" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C96" t="s">
-        <v>278</v>
-      </c>
-      <c r="D96" s="42" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="97" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C97" t="s">
-        <v>279</v>
-      </c>
-      <c r="D97" s="42" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="98" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C98" s="5"/>
-      <c r="D98" s="5"/>
-    </row>
-    <row r="99" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C99" s="5"/>
-      <c r="D99" s="5"/>
-    </row>
-    <row r="100" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B100" s="26" t="s">
-        <v>417</v>
-      </c>
-      <c r="C100" s="27"/>
-      <c r="D100" s="27"/>
-      <c r="E100" s="27"/>
-      <c r="F100" s="27"/>
-      <c r="G100" s="27"/>
-      <c r="H100" s="28"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
USA 2.0 Test Run for Yokohama meeting is finished.
</commit_message>
<xml_diff>
--- a/RECC_Config.xlsx
+++ b/RECC_Config.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1627" uniqueCount="611">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1636" uniqueCount="614">
   <si>
     <t>Description</t>
   </si>
@@ -1857,6 +1857,15 @@
   </si>
   <si>
     <t>workable but needs substantial refinement, not SSP-consistent yet</t>
+  </si>
+  <si>
+    <t>SectorSelect</t>
+  </si>
+  <si>
+    <t>residential buildings, passenger vehicles, all</t>
+  </si>
+  <si>
+    <t>passenger vehicles</t>
   </si>
 </sst>
 </file>
@@ -2702,11 +2711,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:O105"/>
+  <dimension ref="A2:O107"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D96" sqref="D96"/>
+      <selection pane="topRight" activeCell="D99" sqref="D99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4880,209 +4889,252 @@
       </c>
     </row>
     <row r="87" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="C87" s="5"/>
+      <c r="C87" s="66"/>
+      <c r="D87" s="20"/>
+      <c r="E87" s="20"/>
+      <c r="F87" s="24"/>
+      <c r="G87" s="20"/>
       <c r="J87" s="5"/>
-      <c r="K87" s="5"/>
-      <c r="L87" s="5"/>
-      <c r="M87" s="5"/>
-      <c r="N87" s="5"/>
-    </row>
-    <row r="88" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B88" s="26" t="s">
+      <c r="K87" s="56"/>
+      <c r="L87" s="20"/>
+      <c r="M87" s="23"/>
+      <c r="N87" s="20"/>
+      <c r="O87" s="20"/>
+    </row>
+    <row r="88" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="C88" s="5"/>
+      <c r="J88" s="5"/>
+      <c r="K88" s="5"/>
+      <c r="L88" s="5"/>
+      <c r="M88" s="5"/>
+      <c r="N88" s="5"/>
+    </row>
+    <row r="89" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B89" s="26" t="s">
         <v>81</v>
       </c>
-      <c r="C88" s="27"/>
-      <c r="D88" s="27"/>
-      <c r="E88" s="27"/>
-      <c r="F88" s="27"/>
-      <c r="G88" s="27"/>
-      <c r="H88" s="28"/>
-      <c r="K88" s="58" t="s">
+      <c r="C89" s="27"/>
+      <c r="D89" s="27"/>
+      <c r="E89" s="27"/>
+      <c r="F89" s="27"/>
+      <c r="G89" s="27"/>
+      <c r="H89" s="28"/>
+      <c r="K89" s="58" t="s">
         <v>468</v>
       </c>
     </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="C89" s="24" t="s">
+    <row r="90" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="C90" s="24" t="s">
         <v>82</v>
       </c>
-      <c r="K89" s="59"/>
-      <c r="L89" t="s">
+      <c r="K90" s="59"/>
+      <c r="L90" t="s">
         <v>469</v>
       </c>
     </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="C90" s="35" t="s">
+    <row r="91" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="C91" s="35" t="s">
         <v>83</v>
       </c>
-      <c r="D90" s="42" t="s">
+      <c r="D91" s="42" t="s">
         <v>84</v>
       </c>
-      <c r="E90" t="s">
+      <c r="E91" t="s">
         <v>85</v>
       </c>
-      <c r="K90" s="60"/>
-      <c r="L90" t="s">
+      <c r="K91" s="60"/>
+      <c r="L91" t="s">
         <v>610</v>
-      </c>
-    </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="C91" t="s">
-        <v>423</v>
-      </c>
-      <c r="D91" s="42" t="s">
-        <v>431</v>
-      </c>
-      <c r="K91" s="70"/>
-      <c r="L91" t="s">
-        <v>609</v>
       </c>
     </row>
     <row r="92" spans="1:15" x14ac:dyDescent="0.3">
       <c r="C92" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D92" s="42" t="s">
         <v>431</v>
       </c>
-      <c r="E92" s="47" t="s">
+      <c r="K92" s="70"/>
+      <c r="L92" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="93" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="C93" t="s">
+        <v>424</v>
+      </c>
+      <c r="D93" s="47" t="s">
         <v>280</v>
-      </c>
-      <c r="K92" s="61"/>
-      <c r="L92" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="93" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C93" t="s">
-        <v>425</v>
-      </c>
-      <c r="D93" s="42" t="s">
-        <v>431</v>
       </c>
       <c r="E93" s="47" t="s">
         <v>280</v>
       </c>
-      <c r="J93" s="62" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="F93" s="42" t="s">
+        <v>431</v>
+      </c>
+      <c r="K93" s="61"/>
+      <c r="L93" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="94" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C94" t="s">
-        <v>426</v>
-      </c>
-      <c r="D94" s="42" t="s">
-        <v>431</v>
+        <v>425</v>
+      </c>
+      <c r="D94" s="47" t="s">
+        <v>280</v>
       </c>
       <c r="E94" s="47" t="s">
         <v>280</v>
       </c>
-      <c r="J94" s="1" t="s">
-        <v>462</v>
-      </c>
-      <c r="K94" t="s">
-        <v>471</v>
+      <c r="F94" s="42" t="s">
+        <v>431</v>
+      </c>
+      <c r="J94" s="62" t="s">
+        <v>470</v>
       </c>
     </row>
     <row r="95" spans="1:15" x14ac:dyDescent="0.3">
       <c r="C95" t="s">
-        <v>427</v>
-      </c>
-      <c r="D95" s="42" t="s">
-        <v>431</v>
+        <v>426</v>
+      </c>
+      <c r="D95" s="47" t="s">
+        <v>280</v>
       </c>
       <c r="E95" s="47" t="s">
         <v>280</v>
       </c>
+      <c r="F95" s="42" t="s">
+        <v>431</v>
+      </c>
       <c r="J95" s="1" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="K95" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="96" spans="1:15" x14ac:dyDescent="0.3">
       <c r="C96" t="s">
-        <v>428</v>
-      </c>
-      <c r="D96" s="42" t="s">
-        <v>431</v>
+        <v>427</v>
+      </c>
+      <c r="D96" s="47" t="s">
+        <v>280</v>
       </c>
       <c r="E96" s="47" t="s">
         <v>280</v>
       </c>
+      <c r="F96" s="42" t="s">
+        <v>431</v>
+      </c>
       <c r="J96" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="K96" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="97" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C97" t="s">
+        <v>428</v>
+      </c>
+      <c r="D97" s="47" t="s">
+        <v>280</v>
+      </c>
+      <c r="E97" s="47" t="s">
+        <v>280</v>
+      </c>
+      <c r="F97" s="42" t="s">
+        <v>431</v>
+      </c>
+      <c r="J97" s="1" t="s">
         <v>464</v>
       </c>
-      <c r="K96" t="s">
+      <c r="K97" t="s">
         <v>473</v>
       </c>
     </row>
-    <row r="97" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="J97" s="1" t="s">
+    <row r="98" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C98" t="s">
+        <v>611</v>
+      </c>
+      <c r="D98" s="64" t="s">
+        <v>418</v>
+      </c>
+      <c r="E98" s="64" t="s">
+        <v>612</v>
+      </c>
+      <c r="F98" s="64" t="s">
+        <v>613</v>
+      </c>
+      <c r="J98" s="1"/>
+    </row>
+    <row r="99" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="J99" s="1" t="s">
         <v>465</v>
       </c>
-      <c r="K97" t="s">
+      <c r="K99" t="s">
         <v>474</v>
       </c>
     </row>
-    <row r="98" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B98" s="26" t="s">
+    <row r="100" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B100" s="26" t="s">
         <v>104</v>
       </c>
-      <c r="C98" s="27"/>
-      <c r="D98" s="27"/>
-      <c r="E98" s="27"/>
-      <c r="F98" s="27"/>
-      <c r="G98" s="27"/>
-      <c r="H98" s="28"/>
-    </row>
-    <row r="99" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="C99" s="24" t="s">
+      <c r="C100" s="27"/>
+      <c r="D100" s="27"/>
+      <c r="E100" s="27"/>
+      <c r="F100" s="27"/>
+      <c r="G100" s="27"/>
+      <c r="H100" s="28"/>
+    </row>
+    <row r="101" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C101" s="24" t="s">
         <v>70</v>
-      </c>
-    </row>
-    <row r="100" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="C100" t="s">
-        <v>277</v>
-      </c>
-      <c r="D100" s="42" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="101" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="C101" t="s">
-        <v>278</v>
-      </c>
-      <c r="D101" s="42" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="102" spans="2:11" x14ac:dyDescent="0.3">
       <c r="C102" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D102" s="42" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="103" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="C103" s="5"/>
-      <c r="D103" s="5"/>
+      <c r="C103" t="s">
+        <v>278</v>
+      </c>
+      <c r="D103" s="42" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="104" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="C104" s="5"/>
-      <c r="D104" s="5"/>
+      <c r="C104" t="s">
+        <v>279</v>
+      </c>
+      <c r="D104" s="42" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="105" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B105" s="26" t="s">
+      <c r="C105" s="5"/>
+      <c r="D105" s="5"/>
+    </row>
+    <row r="106" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C106" s="5"/>
+      <c r="D106" s="5"/>
+    </row>
+    <row r="107" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B107" s="26" t="s">
         <v>417</v>
       </c>
-      <c r="C105" s="27"/>
-      <c r="D105" s="27"/>
-      <c r="E105" s="27"/>
-      <c r="F105" s="27"/>
-      <c r="G105" s="27"/>
-      <c r="H105" s="28"/>
+      <c r="C107" s="27"/>
+      <c r="D107" s="27"/>
+      <c r="E107" s="27"/>
+      <c r="F107" s="27"/>
+      <c r="G107" s="27"/>
+      <c r="H107" s="28"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update RECC model to G7+IC countries, loop over scenarios.
</commit_message>
<xml_diff>
--- a/RECC_Config.xlsx
+++ b/RECC_Config.xlsx
@@ -13,18 +13,19 @@
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="5" r:id="rId1"/>
-    <sheet name="RECC_USA_TestCase_V2.0" sheetId="10" r:id="rId2"/>
-    <sheet name="RECC_USA_TestCase_V1.0" sheetId="9" r:id="rId3"/>
-    <sheet name="RECC_Main_Development_1" sheetId="7" r:id="rId4"/>
-    <sheet name="GDP_Test" sheetId="8" r:id="rId5"/>
-    <sheet name="Setting_TestRun_1" sheetId="6" r:id="rId6"/>
+    <sheet name="RECC_G7IC_V1" sheetId="11" r:id="rId2"/>
+    <sheet name="RECC_USA_TestCase_V2.0" sheetId="10" r:id="rId3"/>
+    <sheet name="RECC_USA_TestCase_V1.0" sheetId="9" r:id="rId4"/>
+    <sheet name="RECC_Main_Development_1" sheetId="7" r:id="rId5"/>
+    <sheet name="GDP_Test" sheetId="8" r:id="rId6"/>
+    <sheet name="Setting_TestRun_1" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1636" uniqueCount="614">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2310" uniqueCount="713">
   <si>
     <t>Description</t>
   </si>
@@ -1866,6 +1867,303 @@
   </si>
   <si>
     <t>passenger vehicles</t>
+  </si>
+  <si>
+    <t>Evaluate six RE strategies for US, pilot case study, results presented at IRP Yokohama meeting</t>
+  </si>
+  <si>
+    <t>f8d101d4-f0b9-42e4-8b79-6ec0933c8135</t>
+  </si>
+  <si>
+    <t>2_P_RECC_Population_SSP_32R_V2.0</t>
+  </si>
+  <si>
+    <t>Evaluate six RE strategies for G7, first version with complete historic data but insystematic scenarios.</t>
+  </si>
+  <si>
+    <t>Used to split the total constructed building area into heated, cooled, and DHW-reference area</t>
+  </si>
+  <si>
+    <t>3f0e82a8-60a8-493a-aea6-73a6c93a75ca</t>
+  </si>
+  <si>
+    <t>[0,1,2,5]</t>
+  </si>
+  <si>
+    <t>[0,1,5]</t>
+  </si>
+  <si>
+    <t>[0,6,13,24,26,29,30,101]</t>
+  </si>
+  <si>
+    <t>ServiceTypes</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>SerVice types</t>
+  </si>
+  <si>
+    <t>ServiceType</t>
+  </si>
+  <si>
+    <t>Different uses of building energy: heating, cooling, …</t>
+  </si>
+  <si>
+    <t>remanufacturing_reuse</t>
+  </si>
+  <si>
+    <t>downloaded from SSP database, 32 SSP regions, six largest EU countries disaggregated</t>
+  </si>
+  <si>
+    <t>7910f0c7-c7dc-4b54-a35e-961771d9d23a</t>
+  </si>
+  <si>
+    <t>[2,4,9,12,13,31,32,33,34,35,36,37,38,39]</t>
+  </si>
+  <si>
+    <t>2_S_RECC_FinalProducts_2015_G7IC</t>
+  </si>
+  <si>
+    <t>2_S_RECC_FinalProducts_2015_G7IC_V1.0</t>
+  </si>
+  <si>
+    <t>2_S_RECC_FinalProducts_Future_G7IC</t>
+  </si>
+  <si>
+    <t>2_S_RECC_FinalProducts_Future_G7IC_V1.0</t>
+  </si>
+  <si>
+    <t>6bd9a417-d36b-44eb-95d4-07d704552c23</t>
+  </si>
+  <si>
+    <t>3_EI_Products_UsePhase_G7IC</t>
+  </si>
+  <si>
+    <t>3_EI_Products_UsePhase_G7IC_V1.0</t>
+  </si>
+  <si>
+    <t>8373c2a3-6e19-4576-88bb-305a2b4ab73a</t>
+  </si>
+  <si>
+    <t>90c4ec9e-2246-41cd-8669-f37bd89e0279</t>
+  </si>
+  <si>
+    <t>3_LT_RECC_ProductLifetime_V3.0</t>
+  </si>
+  <si>
+    <t>19f56f03-9f39-4b3e-a0ca-1bb8a4944ddd</t>
+  </si>
+  <si>
+    <t>cgVrS</t>
+  </si>
+  <si>
+    <t>tgVrS</t>
+  </si>
+  <si>
+    <t>3_IO_Vehicles_UsePhase_G7IC</t>
+  </si>
+  <si>
+    <t>3_IO_Buildings_UsePhase_G7IC</t>
+  </si>
+  <si>
+    <t>intensity of operation of buildings in use phase, by age-cohort</t>
+  </si>
+  <si>
+    <t>intensity of operation of vehicles in use phase, by model year</t>
+  </si>
+  <si>
+    <t>3_IO_Vehicles_UsePhase_G7IC_V1.0</t>
+  </si>
+  <si>
+    <t>3_IO_Buildings_UsePhase_G7IC_V1.0</t>
+  </si>
+  <si>
+    <t>vehicles: km/yr</t>
+  </si>
+  <si>
+    <t>5b25642b-f113-4453-a979-8dda09e2d5f7</t>
+  </si>
+  <si>
+    <t>3_SHA_EnergyCarrierSplit_Vehicles_G7IC</t>
+  </si>
+  <si>
+    <t>3_SHA_EnergyCarrierSplit_Buildings_G7IC</t>
+  </si>
+  <si>
+    <t>Split total energy consumption into different energy carriers, vehicles</t>
+  </si>
+  <si>
+    <t>Split total energy consumption into different energy carriers, buildings</t>
+  </si>
+  <si>
+    <t>3_SHA_EnergyCarrierSplit_Vehicles_G7IC_V1.0</t>
+  </si>
+  <si>
+    <t>3_SHA_EnergyCarrierSplit_Buildings_G7IC_V1.0</t>
+  </si>
+  <si>
+    <t>b75a013e-614f-4f05-9ead-88cf1901d81c</t>
+  </si>
+  <si>
+    <t>3_MC_RECC_Vehicles_G7IC</t>
+  </si>
+  <si>
+    <t>3_MC_RECC_Buildings_G7IC</t>
+  </si>
+  <si>
+    <t>3_MC_RECC_Buildings_G7IC_V1.0</t>
+  </si>
+  <si>
+    <t>3_MC_RECC_Vehicles_G7IC_V1.0</t>
+  </si>
+  <si>
+    <t>material composition scenarios of buildings in the use phase</t>
+  </si>
+  <si>
+    <t>material composition scenarios of vehicles in the use phase</t>
+  </si>
+  <si>
+    <t>ea1b46a1-5c2b-40c6-9ea1-af00cdee7c6c</t>
+  </si>
+  <si>
+    <t>adaab236-f653-4533-ae38-5a958c18e2ea</t>
+  </si>
+  <si>
+    <t>RECC db status for US + 9 EU regions (CAN, JPN, CHN, IND are added later)</t>
+  </si>
+  <si>
+    <t>no data or incomplete data</t>
+  </si>
+  <si>
+    <t>only US scenarios working</t>
+  </si>
+  <si>
+    <t>Scenarios lacking</t>
+  </si>
+  <si>
+    <t>Used to split total vehicle energy consumption into different energy carriers</t>
+  </si>
+  <si>
+    <t>downloaded from SSP database, 32 SSP regions, needs disagg. For 9 EU regions</t>
+  </si>
+  <si>
+    <t>ready for US-EU-CN assesssment</t>
+  </si>
+  <si>
+    <t>Data for JP, CN, IND, CAN lacking</t>
+  </si>
+  <si>
+    <t>buildings: share of area that is relevant for heating, cooling, and DHW generation</t>
+  </si>
+  <si>
+    <t>3_PR_RECC_CO2Price_SSP_32R_V2.0</t>
+  </si>
+  <si>
+    <t>downloaded from SSP database, 32 SSP regions, disagg. To 9 EU regions</t>
+  </si>
+  <si>
+    <t>a27e27df-1d72-4d96-8bc8-e71cc2c39a7a</t>
+  </si>
+  <si>
+    <t>f908b3d7-f106-43ba-a3f1-6d1ddd0db579</t>
+  </si>
+  <si>
+    <t>contains some simple scenario calculations, needs better link to SSP storylines</t>
+  </si>
+  <si>
+    <t>For US only, is applied to all countries by model script. Contains some simple scenario calculations, needs better link to SSP storylines</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For US only, is applied to all countries by model script. </t>
+  </si>
+  <si>
+    <t>4_EI_WasteMgtEnergyIntensity</t>
+  </si>
+  <si>
+    <t>specific energy consumption of waste management and remelting processes</t>
+  </si>
+  <si>
+    <t>4_EI_WasteMgtEnergyIntensity_V1.0</t>
+  </si>
+  <si>
+    <t>Wncr</t>
+  </si>
+  <si>
+    <t>wmeWtr</t>
+  </si>
+  <si>
+    <t>[18:26)</t>
+  </si>
+  <si>
+    <t>[21:36)</t>
+  </si>
+  <si>
+    <t>external</t>
+  </si>
+  <si>
+    <t>primary production</t>
+  </si>
+  <si>
+    <t>energy supply</t>
+  </si>
+  <si>
+    <t>manufacturing</t>
+  </si>
+  <si>
+    <t>waste mgt. and remelting</t>
+  </si>
+  <si>
+    <t>coordinate with Paula and Steffi</t>
+  </si>
+  <si>
+    <t>a7b82038-e3a4-46b2-8453-6aa2a3ff3b76</t>
+  </si>
+  <si>
+    <t>Translates waste mgt. process output into energy demand</t>
+  </si>
+  <si>
+    <t>Translates manufacturing process output into energy demand</t>
+  </si>
+  <si>
+    <t>Translates primary material production process output into energy demand</t>
+  </si>
+  <si>
+    <t>grmwW</t>
+  </si>
+  <si>
+    <t>RECC_G7IC_V1</t>
+  </si>
+  <si>
+    <t>G7IC_V1</t>
+  </si>
+  <si>
+    <t>RECC_G7IC_V1.0</t>
+  </si>
+  <si>
+    <t>contains MESSAGE results for electricity and SSP1, 2, and 3.</t>
+  </si>
+  <si>
+    <t>4_PE_GHGIntensityEnergySupply_CDLINKS_MESSAGEix</t>
+  </si>
+  <si>
+    <t>4_PE_GHGIntensityEnergySupply_CDLINKS_MESSAGEix_V1.0</t>
+  </si>
+  <si>
+    <t>64ddc6aa-6e45-4c4d-bdd1-f654fa02c3fc</t>
+  </si>
+  <si>
+    <t>XnSrt</t>
+  </si>
+  <si>
+    <t>cgVnrS</t>
+  </si>
+  <si>
+    <t>cgrVnS</t>
+  </si>
+  <si>
+    <t>waste management and remelting industries</t>
   </si>
 </sst>
 </file>
@@ -1967,7 +2265,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2007,6 +2305,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2102,7 +2406,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -2234,6 +2538,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -2517,7 +2832,7 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D11:D12"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2560,7 +2875,7 @@
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="6" t="s">
-        <v>459</v>
+        <v>702</v>
       </c>
       <c r="G4" s="48"/>
     </row>
@@ -2713,9 +3028,2582 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:O107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D99" sqref="D99"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F74" sqref="F74"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="25.33203125" customWidth="1"/>
+    <col min="3" max="3" width="41.88671875" customWidth="1"/>
+    <col min="4" max="4" width="65.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="50.6640625" customWidth="1"/>
+    <col min="6" max="6" width="24.6640625" customWidth="1"/>
+    <col min="7" max="7" width="38.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="45.109375" customWidth="1"/>
+    <col min="12" max="12" width="73.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="46.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="90" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B2" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="28"/>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C3" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" s="41" t="s">
+        <v>56</v>
+      </c>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="42" t="s">
+        <v>703</v>
+      </c>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="20"/>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="42" t="s">
+        <v>617</v>
+      </c>
+      <c r="I5" s="20"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="20"/>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="43" t="s">
+        <v>704</v>
+      </c>
+      <c r="I6" s="20"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="20"/>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="D7" s="11"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="20"/>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B8" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="28"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="20"/>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C9" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="D9" s="41" t="s">
+        <v>207</v>
+      </c>
+      <c r="E9" s="31"/>
+      <c r="F9" s="39"/>
+      <c r="G9" s="39"/>
+      <c r="H9" s="39"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="19"/>
+      <c r="K9" s="20"/>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="42" t="s">
+        <v>309</v>
+      </c>
+      <c r="I10" s="20"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="20"/>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C11" t="s">
+        <v>267</v>
+      </c>
+      <c r="D11" s="50" t="s">
+        <v>312</v>
+      </c>
+      <c r="I11" s="20"/>
+      <c r="J11" s="19"/>
+      <c r="K11" s="20"/>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C12" t="s">
+        <v>268</v>
+      </c>
+      <c r="D12" s="50" t="s">
+        <v>312</v>
+      </c>
+      <c r="I12" s="20"/>
+      <c r="J12" s="19"/>
+      <c r="K12" s="20"/>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="I13" s="20"/>
+      <c r="J13" s="25"/>
+      <c r="K13" s="20"/>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B14" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="C14" s="27"/>
+      <c r="D14" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="E14" s="27"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="27"/>
+      <c r="H14" s="28"/>
+      <c r="I14" s="36" t="s">
+        <v>439</v>
+      </c>
+      <c r="J14" s="20"/>
+      <c r="K14" s="20"/>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C15" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="E15" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15" s="31" t="s">
+        <v>438</v>
+      </c>
+      <c r="H15" s="30" t="s">
+        <v>186</v>
+      </c>
+      <c r="I15" s="52" t="s">
+        <v>187</v>
+      </c>
+      <c r="K15" s="20"/>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C16" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" t="s">
+        <v>28</v>
+      </c>
+      <c r="E16" t="s">
+        <v>16</v>
+      </c>
+      <c r="F16" t="s">
+        <v>16</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="H16" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="I16" s="20" t="s">
+        <v>188</v>
+      </c>
+      <c r="J16" s="20"/>
+      <c r="K16" s="20"/>
+    </row>
+    <row r="17" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C17" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" t="s">
+        <v>29</v>
+      </c>
+      <c r="E17" t="s">
+        <v>16</v>
+      </c>
+      <c r="F17" t="s">
+        <v>16</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>429</v>
+      </c>
+      <c r="H17" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="I17" s="20" t="s">
+        <v>189</v>
+      </c>
+      <c r="J17" s="20"/>
+      <c r="K17" s="20"/>
+    </row>
+    <row r="18" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C18" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" t="s">
+        <v>37</v>
+      </c>
+      <c r="E18" t="s">
+        <v>23</v>
+      </c>
+      <c r="F18" t="s">
+        <v>42</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>622</v>
+      </c>
+      <c r="H18" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="I18" s="20" t="s">
+        <v>190</v>
+      </c>
+      <c r="J18" s="20"/>
+      <c r="K18" s="20"/>
+    </row>
+    <row r="19" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C19" s="33" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" t="s">
+        <v>38</v>
+      </c>
+      <c r="E19" t="s">
+        <v>24</v>
+      </c>
+      <c r="F19" t="s">
+        <v>24</v>
+      </c>
+      <c r="G19" t="s">
+        <v>418</v>
+      </c>
+      <c r="H19" s="29">
+        <v>1</v>
+      </c>
+      <c r="I19" s="20" t="s">
+        <v>192</v>
+      </c>
+      <c r="J19" s="20"/>
+      <c r="K19" s="20"/>
+    </row>
+    <row r="20" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C20" s="33" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" t="s">
+        <v>31</v>
+      </c>
+      <c r="E20" t="s">
+        <v>39</v>
+      </c>
+      <c r="F20" t="s">
+        <v>40</v>
+      </c>
+      <c r="G20" t="s">
+        <v>631</v>
+      </c>
+      <c r="H20" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="I20" s="20" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="21" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C21" s="45" t="s">
+        <v>142</v>
+      </c>
+      <c r="D21" t="s">
+        <v>150</v>
+      </c>
+      <c r="E21" t="s">
+        <v>26</v>
+      </c>
+      <c r="F21" t="s">
+        <v>155</v>
+      </c>
+      <c r="G21" t="s">
+        <v>690</v>
+      </c>
+      <c r="H21" s="29" t="s">
+        <v>184</v>
+      </c>
+      <c r="I21" s="20" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="22" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C22" s="45" t="s">
+        <v>143</v>
+      </c>
+      <c r="D22" t="s">
+        <v>151</v>
+      </c>
+      <c r="E22" t="s">
+        <v>26</v>
+      </c>
+      <c r="F22" t="s">
+        <v>156</v>
+      </c>
+      <c r="G22" t="s">
+        <v>420</v>
+      </c>
+      <c r="H22" s="29" t="s">
+        <v>179</v>
+      </c>
+      <c r="I22" s="20" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="23" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C23" s="45" t="s">
+        <v>144</v>
+      </c>
+      <c r="D23" t="s">
+        <v>152</v>
+      </c>
+      <c r="E23" t="s">
+        <v>26</v>
+      </c>
+      <c r="F23" t="s">
+        <v>157</v>
+      </c>
+      <c r="G23" t="s">
+        <v>420</v>
+      </c>
+      <c r="H23" s="29" t="s">
+        <v>178</v>
+      </c>
+      <c r="I23" s="20" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C24" s="45" t="s">
+        <v>145</v>
+      </c>
+      <c r="D24" t="s">
+        <v>148</v>
+      </c>
+      <c r="E24" t="s">
+        <v>26</v>
+      </c>
+      <c r="F24" t="s">
+        <v>106</v>
+      </c>
+      <c r="G24" t="s">
+        <v>689</v>
+      </c>
+      <c r="H24" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="I24" s="20" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="25" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C25" s="45" t="s">
+        <v>163</v>
+      </c>
+      <c r="D25" t="s">
+        <v>159</v>
+      </c>
+      <c r="E25" t="s">
+        <v>21</v>
+      </c>
+      <c r="F25" t="s">
+        <v>134</v>
+      </c>
+      <c r="G25" t="s">
+        <v>420</v>
+      </c>
+      <c r="H25" s="29" t="s">
+        <v>337</v>
+      </c>
+      <c r="I25" s="20" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="26" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C26" s="45" t="s">
+        <v>20</v>
+      </c>
+      <c r="D26" t="s">
+        <v>32</v>
+      </c>
+      <c r="E26" t="s">
+        <v>21</v>
+      </c>
+      <c r="F26" t="s">
+        <v>105</v>
+      </c>
+      <c r="G26" t="s">
+        <v>420</v>
+      </c>
+      <c r="H26" s="29" t="s">
+        <v>181</v>
+      </c>
+      <c r="I26" s="20" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="27" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C27" s="45" t="s">
+        <v>331</v>
+      </c>
+      <c r="D27" t="s">
+        <v>332</v>
+      </c>
+      <c r="E27" t="s">
+        <v>21</v>
+      </c>
+      <c r="F27" t="s">
+        <v>333</v>
+      </c>
+      <c r="G27" t="s">
+        <v>334</v>
+      </c>
+      <c r="H27" s="29" t="s">
+        <v>335</v>
+      </c>
+      <c r="I27" s="20" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="28" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C28" s="45" t="s">
+        <v>22</v>
+      </c>
+      <c r="D28" t="s">
+        <v>34</v>
+      </c>
+      <c r="E28" t="s">
+        <v>21</v>
+      </c>
+      <c r="F28" t="s">
+        <v>117</v>
+      </c>
+      <c r="G28" t="s">
+        <v>289</v>
+      </c>
+      <c r="H28" s="29" t="s">
+        <v>182</v>
+      </c>
+      <c r="I28" s="20" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="29" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C29" s="45" t="s">
+        <v>167</v>
+      </c>
+      <c r="D29" t="s">
+        <v>170</v>
+      </c>
+      <c r="E29" t="s">
+        <v>169</v>
+      </c>
+      <c r="F29" t="s">
+        <v>168</v>
+      </c>
+      <c r="G29" t="s">
+        <v>599</v>
+      </c>
+      <c r="H29" s="29" t="s">
+        <v>185</v>
+      </c>
+      <c r="I29" s="20" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="30" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C30" s="45" t="s">
+        <v>25</v>
+      </c>
+      <c r="D30" t="s">
+        <v>171</v>
+      </c>
+      <c r="E30" t="s">
+        <v>25</v>
+      </c>
+      <c r="F30" t="s">
+        <v>41</v>
+      </c>
+      <c r="G30" t="s">
+        <v>113</v>
+      </c>
+      <c r="H30" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="I30" s="20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="31" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C31" s="45" t="s">
+        <v>173</v>
+      </c>
+      <c r="D31" t="s">
+        <v>174</v>
+      </c>
+      <c r="E31" t="s">
+        <v>173</v>
+      </c>
+      <c r="F31" t="s">
+        <v>172</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>419</v>
+      </c>
+      <c r="H31" s="29" t="s">
+        <v>183</v>
+      </c>
+      <c r="I31" s="20" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="32" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C32" s="33" t="s">
+        <v>283</v>
+      </c>
+      <c r="D32" t="s">
+        <v>284</v>
+      </c>
+      <c r="E32" t="s">
+        <v>25</v>
+      </c>
+      <c r="F32" t="s">
+        <v>285</v>
+      </c>
+      <c r="G32" s="20" t="s">
+        <v>621</v>
+      </c>
+      <c r="H32" s="29" t="s">
+        <v>286</v>
+      </c>
+      <c r="I32" s="20" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C33" s="45" t="s">
+        <v>294</v>
+      </c>
+      <c r="D33" t="s">
+        <v>295</v>
+      </c>
+      <c r="E33" t="s">
+        <v>25</v>
+      </c>
+      <c r="F33" t="s">
+        <v>251</v>
+      </c>
+      <c r="G33" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="H33" s="29" t="s">
+        <v>254</v>
+      </c>
+      <c r="I33" s="20" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C34" s="45" t="s">
+        <v>583</v>
+      </c>
+      <c r="D34" t="s">
+        <v>582</v>
+      </c>
+      <c r="E34" t="s">
+        <v>21</v>
+      </c>
+      <c r="F34" t="s">
+        <v>607</v>
+      </c>
+      <c r="G34" s="20" t="s">
+        <v>418</v>
+      </c>
+      <c r="H34" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="I34" s="20" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C35" s="72" t="s">
+        <v>626</v>
+      </c>
+      <c r="D35" s="42" t="s">
+        <v>627</v>
+      </c>
+      <c r="E35" t="s">
+        <v>173</v>
+      </c>
+      <c r="F35" s="68" t="s">
+        <v>623</v>
+      </c>
+      <c r="G35" s="20" t="s">
+        <v>620</v>
+      </c>
+      <c r="H35" s="29" t="s">
+        <v>624</v>
+      </c>
+      <c r="I35" s="20" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B37" s="26" t="s">
+        <v>101</v>
+      </c>
+      <c r="C37" s="27"/>
+      <c r="D37" s="27"/>
+      <c r="E37" s="27"/>
+      <c r="F37" s="27"/>
+      <c r="G37" s="27"/>
+      <c r="H37" s="28"/>
+    </row>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C38" s="34" t="s">
+        <v>102</v>
+      </c>
+      <c r="D38" s="31" t="s">
+        <v>103</v>
+      </c>
+      <c r="E38" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="F38" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="G38" s="39"/>
+      <c r="H38" s="39"/>
+    </row>
+    <row r="39" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C39" s="53">
+        <v>3</v>
+      </c>
+      <c r="D39" t="s">
+        <v>450</v>
+      </c>
+      <c r="E39" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C40" s="53">
+        <v>4</v>
+      </c>
+      <c r="D40" t="s">
+        <v>452</v>
+      </c>
+      <c r="E40" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="41" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C41" s="53">
+        <v>6</v>
+      </c>
+      <c r="D41" t="s">
+        <v>453</v>
+      </c>
+      <c r="E41" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="42" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C42" s="53">
+        <v>7</v>
+      </c>
+      <c r="D42" t="s">
+        <v>407</v>
+      </c>
+      <c r="E42" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="43" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C43" s="53">
+        <v>8</v>
+      </c>
+      <c r="D43" t="s">
+        <v>408</v>
+      </c>
+      <c r="E43" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="44" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C44" s="53">
+        <v>9</v>
+      </c>
+      <c r="D44" t="s">
+        <v>409</v>
+      </c>
+      <c r="E44" t="s">
+        <v>405</v>
+      </c>
+      <c r="F44" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="45" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C45" s="53">
+        <v>10</v>
+      </c>
+      <c r="D45" t="s">
+        <v>410</v>
+      </c>
+      <c r="E45" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="46" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C46" s="53">
+        <v>11</v>
+      </c>
+      <c r="D46" t="s">
+        <v>712</v>
+      </c>
+      <c r="E46" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="47" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C47" s="53">
+        <v>12</v>
+      </c>
+      <c r="D47" t="s">
+        <v>412</v>
+      </c>
+      <c r="E47" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="48" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C48" s="53">
+        <v>13</v>
+      </c>
+      <c r="D48" t="s">
+        <v>415</v>
+      </c>
+      <c r="E48" t="s">
+        <v>405</v>
+      </c>
+      <c r="F48" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C49" s="53">
+        <v>14</v>
+      </c>
+      <c r="D49" t="s">
+        <v>416</v>
+      </c>
+      <c r="E49" t="s">
+        <v>404</v>
+      </c>
+      <c r="F49" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C50" s="73">
+        <v>15</v>
+      </c>
+      <c r="D50" t="s">
+        <v>628</v>
+      </c>
+      <c r="E50" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B52" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="C52" s="27"/>
+      <c r="D52" s="27"/>
+      <c r="E52" s="27"/>
+      <c r="F52" s="27"/>
+      <c r="G52" s="27"/>
+      <c r="H52" s="28"/>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B53" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="C53" s="34" t="s">
+        <v>58</v>
+      </c>
+      <c r="D53" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="E53" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="F53" s="31" t="s">
+        <v>59</v>
+      </c>
+      <c r="G53" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="H53" s="31" t="s">
+        <v>60</v>
+      </c>
+      <c r="I53" s="31" t="s">
+        <v>297</v>
+      </c>
+      <c r="J53" s="54" t="s">
+        <v>460</v>
+      </c>
+      <c r="K53" s="54" t="s">
+        <v>475</v>
+      </c>
+      <c r="L53" s="54" t="s">
+        <v>668</v>
+      </c>
+      <c r="M53" s="55" t="s">
+        <v>499</v>
+      </c>
+      <c r="N53" s="55" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>0</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>691</v>
+      </c>
+      <c r="C54" s="35" t="s">
+        <v>292</v>
+      </c>
+      <c r="D54" t="s">
+        <v>293</v>
+      </c>
+      <c r="E54" s="20" t="s">
+        <v>616</v>
+      </c>
+      <c r="F54" s="24" t="s">
+        <v>263</v>
+      </c>
+      <c r="G54" t="s">
+        <v>239</v>
+      </c>
+      <c r="H54" t="s">
+        <v>61</v>
+      </c>
+      <c r="I54" t="s">
+        <v>615</v>
+      </c>
+      <c r="J54" s="5" t="s">
+        <v>462</v>
+      </c>
+      <c r="K54" s="56"/>
+      <c r="L54" s="20" t="s">
+        <v>629</v>
+      </c>
+      <c r="M54" s="20" t="s">
+        <v>501</v>
+      </c>
+      <c r="N54" s="20" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>1</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="C55" s="35" t="s">
+        <v>632</v>
+      </c>
+      <c r="D55" t="s">
+        <v>301</v>
+      </c>
+      <c r="E55" s="20" t="s">
+        <v>633</v>
+      </c>
+      <c r="F55" s="46" t="s">
+        <v>303</v>
+      </c>
+      <c r="G55" s="20" t="s">
+        <v>239</v>
+      </c>
+      <c r="H55" t="s">
+        <v>61</v>
+      </c>
+      <c r="I55" t="s">
+        <v>630</v>
+      </c>
+      <c r="J55" s="5" t="s">
+        <v>464</v>
+      </c>
+      <c r="K55" s="69"/>
+      <c r="L55" s="20" t="s">
+        <v>675</v>
+      </c>
+      <c r="M55" t="s">
+        <v>500</v>
+      </c>
+      <c r="N55" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>2</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="C56" s="35" t="s">
+        <v>634</v>
+      </c>
+      <c r="D56" t="s">
+        <v>306</v>
+      </c>
+      <c r="E56" s="20" t="s">
+        <v>635</v>
+      </c>
+      <c r="F56" s="46" t="s">
+        <v>590</v>
+      </c>
+      <c r="G56" s="20" t="s">
+        <v>239</v>
+      </c>
+      <c r="H56" t="s">
+        <v>61</v>
+      </c>
+      <c r="I56" t="s">
+        <v>636</v>
+      </c>
+      <c r="J56" s="5" t="s">
+        <v>462</v>
+      </c>
+      <c r="K56" s="59"/>
+      <c r="L56" s="20" t="s">
+        <v>670</v>
+      </c>
+      <c r="M56" t="s">
+        <v>502</v>
+      </c>
+      <c r="N56" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>3</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="C57" s="35" t="s">
+        <v>637</v>
+      </c>
+      <c r="D57" s="20" t="s">
+        <v>317</v>
+      </c>
+      <c r="E57" t="s">
+        <v>638</v>
+      </c>
+      <c r="F57" s="46" t="s">
+        <v>710</v>
+      </c>
+      <c r="G57" s="20" t="s">
+        <v>376</v>
+      </c>
+      <c r="H57" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="I57" t="s">
+        <v>639</v>
+      </c>
+      <c r="J57" s="5" t="s">
+        <v>462</v>
+      </c>
+      <c r="K57" s="69"/>
+      <c r="L57" s="20" t="s">
+        <v>675</v>
+      </c>
+      <c r="M57" t="s">
+        <v>522</v>
+      </c>
+      <c r="N57" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>4</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="C58" s="35" t="s">
+        <v>645</v>
+      </c>
+      <c r="D58" s="20" t="s">
+        <v>648</v>
+      </c>
+      <c r="E58" s="5" t="s">
+        <v>649</v>
+      </c>
+      <c r="F58" s="74" t="s">
+        <v>644</v>
+      </c>
+      <c r="G58" s="20" t="s">
+        <v>321</v>
+      </c>
+      <c r="H58" t="s">
+        <v>61</v>
+      </c>
+      <c r="I58" t="s">
+        <v>640</v>
+      </c>
+      <c r="J58" s="5" t="s">
+        <v>462</v>
+      </c>
+      <c r="K58" s="69"/>
+      <c r="L58" s="20" t="s">
+        <v>675</v>
+      </c>
+      <c r="M58" t="s">
+        <v>651</v>
+      </c>
+      <c r="N58" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>5</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="C59" s="75" t="s">
+        <v>646</v>
+      </c>
+      <c r="D59" s="20" t="s">
+        <v>647</v>
+      </c>
+      <c r="E59" s="66" t="s">
+        <v>650</v>
+      </c>
+      <c r="F59" s="74" t="s">
+        <v>643</v>
+      </c>
+      <c r="G59" s="20" t="s">
+        <v>321</v>
+      </c>
+      <c r="H59" t="s">
+        <v>61</v>
+      </c>
+      <c r="I59" t="s">
+        <v>619</v>
+      </c>
+      <c r="J59" s="5" t="s">
+        <v>464</v>
+      </c>
+      <c r="K59" s="69"/>
+      <c r="L59" s="20" t="s">
+        <v>675</v>
+      </c>
+      <c r="M59" s="20" t="s">
+        <v>676</v>
+      </c>
+      <c r="N59" s="20" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>6</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="C60" s="67" t="s">
+        <v>329</v>
+      </c>
+      <c r="D60" s="20" t="s">
+        <v>325</v>
+      </c>
+      <c r="E60" t="s">
+        <v>641</v>
+      </c>
+      <c r="F60" s="24" t="s">
+        <v>275</v>
+      </c>
+      <c r="G60" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="H60" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="I60" t="s">
+        <v>642</v>
+      </c>
+      <c r="J60" s="5" t="s">
+        <v>464</v>
+      </c>
+      <c r="K60" s="56"/>
+      <c r="L60" s="20" t="s">
+        <v>523</v>
+      </c>
+      <c r="M60" s="20" t="s">
+        <v>520</v>
+      </c>
+      <c r="N60" s="20" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>7</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="C61" s="8" t="s">
+        <v>661</v>
+      </c>
+      <c r="D61" s="71" t="s">
+        <v>664</v>
+      </c>
+      <c r="E61" s="8" t="s">
+        <v>662</v>
+      </c>
+      <c r="F61" s="24" t="s">
+        <v>339</v>
+      </c>
+      <c r="G61" s="20" t="s">
+        <v>321</v>
+      </c>
+      <c r="H61" t="s">
+        <v>61</v>
+      </c>
+      <c r="I61" t="s">
+        <v>666</v>
+      </c>
+      <c r="J61" s="5" t="s">
+        <v>464</v>
+      </c>
+      <c r="K61" s="69"/>
+      <c r="L61" s="20" t="s">
+        <v>675</v>
+      </c>
+      <c r="M61" s="20" t="s">
+        <v>507</v>
+      </c>
+      <c r="N61" s="20" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>8</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="C62" s="67" t="s">
+        <v>660</v>
+      </c>
+      <c r="D62" s="71" t="s">
+        <v>665</v>
+      </c>
+      <c r="E62" s="8" t="s">
+        <v>663</v>
+      </c>
+      <c r="F62" s="24" t="s">
+        <v>339</v>
+      </c>
+      <c r="G62" s="20" t="s">
+        <v>321</v>
+      </c>
+      <c r="H62" t="s">
+        <v>61</v>
+      </c>
+      <c r="I62" t="s">
+        <v>667</v>
+      </c>
+      <c r="J62" s="5" t="s">
+        <v>464</v>
+      </c>
+      <c r="K62" s="69"/>
+      <c r="L62" s="20" t="s">
+        <v>675</v>
+      </c>
+      <c r="M62" s="20" t="s">
+        <v>506</v>
+      </c>
+      <c r="N62" s="20" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>9</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="C63" s="67" t="s">
+        <v>442</v>
+      </c>
+      <c r="D63" s="20" t="s">
+        <v>440</v>
+      </c>
+      <c r="E63" s="5" t="s">
+        <v>484</v>
+      </c>
+      <c r="F63" s="24" t="s">
+        <v>448</v>
+      </c>
+      <c r="G63" s="20" t="s">
+        <v>126</v>
+      </c>
+      <c r="H63" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="I63" t="s">
+        <v>565</v>
+      </c>
+      <c r="J63" s="5" t="s">
+        <v>464</v>
+      </c>
+      <c r="K63" s="56"/>
+      <c r="L63" s="20" t="s">
+        <v>603</v>
+      </c>
+      <c r="M63" s="20" t="s">
+        <v>509</v>
+      </c>
+      <c r="N63" s="20" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <v>10</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>692</v>
+      </c>
+      <c r="C64" s="67" t="s">
+        <v>443</v>
+      </c>
+      <c r="D64" s="20" t="s">
+        <v>441</v>
+      </c>
+      <c r="E64" s="5" t="s">
+        <v>485</v>
+      </c>
+      <c r="F64" s="24" t="s">
+        <v>448</v>
+      </c>
+      <c r="G64" s="20" t="s">
+        <v>126</v>
+      </c>
+      <c r="H64" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="I64" t="s">
+        <v>566</v>
+      </c>
+      <c r="J64" s="5" t="s">
+        <v>464</v>
+      </c>
+      <c r="K64" s="56"/>
+      <c r="L64" s="20" t="s">
+        <v>603</v>
+      </c>
+      <c r="M64" s="20" t="s">
+        <v>509</v>
+      </c>
+      <c r="N64" s="20" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="65" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>11</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>691</v>
+      </c>
+      <c r="C65" s="67" t="s">
+        <v>345</v>
+      </c>
+      <c r="D65" s="20" t="s">
+        <v>346</v>
+      </c>
+      <c r="E65" s="5" t="s">
+        <v>677</v>
+      </c>
+      <c r="F65" s="24" t="s">
+        <v>348</v>
+      </c>
+      <c r="G65" s="20" t="s">
+        <v>239</v>
+      </c>
+      <c r="H65" t="s">
+        <v>61</v>
+      </c>
+      <c r="I65" t="s">
+        <v>679</v>
+      </c>
+      <c r="J65" s="5" t="s">
+        <v>466</v>
+      </c>
+      <c r="K65" s="56"/>
+      <c r="L65" s="20" t="s">
+        <v>678</v>
+      </c>
+      <c r="M65" t="s">
+        <v>505</v>
+      </c>
+      <c r="N65" s="20" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="66" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <v>12</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>691</v>
+      </c>
+      <c r="C66" s="67" t="s">
+        <v>351</v>
+      </c>
+      <c r="D66" s="20" t="s">
+        <v>350</v>
+      </c>
+      <c r="E66" t="s">
+        <v>486</v>
+      </c>
+      <c r="F66" s="24" t="s">
+        <v>348</v>
+      </c>
+      <c r="G66" s="20" t="s">
+        <v>239</v>
+      </c>
+      <c r="H66" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="I66" s="36" t="s">
+        <v>680</v>
+      </c>
+      <c r="J66" s="5" t="s">
+        <v>466</v>
+      </c>
+      <c r="K66" s="57"/>
+      <c r="L66" s="20" t="s">
+        <v>681</v>
+      </c>
+      <c r="M66" t="s">
+        <v>504</v>
+      </c>
+      <c r="N66" s="20" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="67" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A67">
+        <v>13</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>693</v>
+      </c>
+      <c r="C67" s="75" t="s">
+        <v>359</v>
+      </c>
+      <c r="D67" s="20" t="s">
+        <v>356</v>
+      </c>
+      <c r="E67" t="s">
+        <v>487</v>
+      </c>
+      <c r="F67" s="24" t="s">
+        <v>354</v>
+      </c>
+      <c r="G67" s="20" t="s">
+        <v>239</v>
+      </c>
+      <c r="H67" t="s">
+        <v>61</v>
+      </c>
+      <c r="I67" t="s">
+        <v>568</v>
+      </c>
+      <c r="J67" s="5" t="s">
+        <v>466</v>
+      </c>
+      <c r="K67" s="77"/>
+      <c r="L67" s="20" t="s">
+        <v>604</v>
+      </c>
+      <c r="M67" t="s">
+        <v>524</v>
+      </c>
+      <c r="N67" s="20" t="s">
+        <v>547</v>
+      </c>
+      <c r="O67" s="20"/>
+    </row>
+    <row r="68" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A68">
+        <v>14</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>693</v>
+      </c>
+      <c r="C68" s="75" t="s">
+        <v>706</v>
+      </c>
+      <c r="D68" s="20" t="s">
+        <v>356</v>
+      </c>
+      <c r="E68" t="s">
+        <v>707</v>
+      </c>
+      <c r="F68" s="24" t="s">
+        <v>709</v>
+      </c>
+      <c r="G68" s="20" t="s">
+        <v>321</v>
+      </c>
+      <c r="H68" t="s">
+        <v>61</v>
+      </c>
+      <c r="I68" t="s">
+        <v>708</v>
+      </c>
+      <c r="J68" s="5" t="s">
+        <v>466</v>
+      </c>
+      <c r="K68" s="77"/>
+      <c r="L68" s="20" t="s">
+        <v>705</v>
+      </c>
+      <c r="M68" t="s">
+        <v>524</v>
+      </c>
+      <c r="N68" s="20" t="s">
+        <v>547</v>
+      </c>
+      <c r="O68" s="20"/>
+    </row>
+    <row r="69" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A69">
+        <v>15</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>692</v>
+      </c>
+      <c r="C69" s="76" t="s">
+        <v>360</v>
+      </c>
+      <c r="D69" s="20" t="s">
+        <v>401</v>
+      </c>
+      <c r="E69" s="5" t="s">
+        <v>488</v>
+      </c>
+      <c r="F69" s="46" t="s">
+        <v>421</v>
+      </c>
+      <c r="G69" s="20" t="s">
+        <v>239</v>
+      </c>
+      <c r="H69" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="I69" t="s">
+        <v>569</v>
+      </c>
+      <c r="J69" s="5" t="s">
+        <v>464</v>
+      </c>
+      <c r="K69" s="59"/>
+      <c r="L69" s="20" t="s">
+        <v>670</v>
+      </c>
+      <c r="M69" t="s">
+        <v>525</v>
+      </c>
+      <c r="N69" s="20" t="s">
+        <v>548</v>
+      </c>
+      <c r="O69" s="20" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="70" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A70">
+        <v>16</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>692</v>
+      </c>
+      <c r="C70" s="76" t="s">
+        <v>400</v>
+      </c>
+      <c r="D70" s="20" t="s">
+        <v>554</v>
+      </c>
+      <c r="E70" s="5" t="s">
+        <v>489</v>
+      </c>
+      <c r="F70" s="46" t="s">
+        <v>403</v>
+      </c>
+      <c r="G70" s="20" t="s">
+        <v>239</v>
+      </c>
+      <c r="H70" t="s">
+        <v>61</v>
+      </c>
+      <c r="I70" s="65" t="s">
+        <v>570</v>
+      </c>
+      <c r="J70" s="5" t="s">
+        <v>464</v>
+      </c>
+      <c r="K70" s="59"/>
+      <c r="L70" s="20" t="s">
+        <v>670</v>
+      </c>
+      <c r="M70" t="s">
+        <v>526</v>
+      </c>
+      <c r="N70" s="20" t="s">
+        <v>700</v>
+      </c>
+      <c r="O70" s="20" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="71" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A71">
+        <v>17</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>694</v>
+      </c>
+      <c r="C71" s="76" t="s">
+        <v>553</v>
+      </c>
+      <c r="D71" s="20" t="s">
+        <v>555</v>
+      </c>
+      <c r="E71" s="5" t="s">
+        <v>556</v>
+      </c>
+      <c r="F71" s="46" t="s">
+        <v>557</v>
+      </c>
+      <c r="G71" s="20" t="s">
+        <v>239</v>
+      </c>
+      <c r="H71" t="s">
+        <v>61</v>
+      </c>
+      <c r="I71" t="s">
+        <v>571</v>
+      </c>
+      <c r="J71" s="5" t="s">
+        <v>464</v>
+      </c>
+      <c r="K71" s="59"/>
+      <c r="L71" s="20" t="s">
+        <v>670</v>
+      </c>
+      <c r="M71" t="s">
+        <v>526</v>
+      </c>
+      <c r="N71" s="20" t="s">
+        <v>699</v>
+      </c>
+      <c r="O71" s="20" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="72" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A72">
+        <v>18</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>695</v>
+      </c>
+      <c r="C72" s="75" t="s">
+        <v>361</v>
+      </c>
+      <c r="D72" s="20" t="s">
+        <v>363</v>
+      </c>
+      <c r="E72" t="s">
+        <v>490</v>
+      </c>
+      <c r="F72" s="24" t="s">
+        <v>701</v>
+      </c>
+      <c r="G72" s="20" t="s">
+        <v>321</v>
+      </c>
+      <c r="H72" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="I72" t="s">
+        <v>572</v>
+      </c>
+      <c r="J72" s="5" t="s">
+        <v>464</v>
+      </c>
+      <c r="K72" s="69"/>
+      <c r="L72" s="20" t="s">
+        <v>683</v>
+      </c>
+      <c r="M72" s="20" t="s">
+        <v>504</v>
+      </c>
+      <c r="N72" s="20" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="73" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A73">
+        <v>19</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>694</v>
+      </c>
+      <c r="C73" s="75" t="s">
+        <v>366</v>
+      </c>
+      <c r="D73" s="20" t="s">
+        <v>367</v>
+      </c>
+      <c r="E73" t="s">
+        <v>491</v>
+      </c>
+      <c r="F73" s="24" t="s">
+        <v>430</v>
+      </c>
+      <c r="G73" s="20" t="s">
+        <v>376</v>
+      </c>
+      <c r="H73" t="s">
+        <v>61</v>
+      </c>
+      <c r="I73" t="s">
+        <v>573</v>
+      </c>
+      <c r="J73" s="5" t="s">
+        <v>464</v>
+      </c>
+      <c r="K73" s="69"/>
+      <c r="L73" s="20" t="s">
+        <v>683</v>
+      </c>
+      <c r="M73" s="63">
+        <v>1</v>
+      </c>
+      <c r="N73" s="20" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="74" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A74">
+        <v>20</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>695</v>
+      </c>
+      <c r="C74" s="67" t="s">
+        <v>370</v>
+      </c>
+      <c r="D74" s="20" t="s">
+        <v>371</v>
+      </c>
+      <c r="E74" t="s">
+        <v>492</v>
+      </c>
+      <c r="F74" s="24" t="s">
+        <v>688</v>
+      </c>
+      <c r="G74" s="20" t="s">
+        <v>376</v>
+      </c>
+      <c r="H74" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="I74" t="s">
+        <v>574</v>
+      </c>
+      <c r="J74" s="5" t="s">
+        <v>464</v>
+      </c>
+      <c r="K74" s="56"/>
+      <c r="L74" s="20" t="s">
+        <v>683</v>
+      </c>
+      <c r="M74" s="63">
+        <v>1</v>
+      </c>
+      <c r="N74" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="75" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A75">
+        <v>21</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>695</v>
+      </c>
+      <c r="C75" s="76" t="s">
+        <v>684</v>
+      </c>
+      <c r="D75" s="20" t="s">
+        <v>685</v>
+      </c>
+      <c r="E75" s="8" t="s">
+        <v>686</v>
+      </c>
+      <c r="F75" s="46" t="s">
+        <v>687</v>
+      </c>
+      <c r="G75" s="20" t="s">
+        <v>239</v>
+      </c>
+      <c r="H75" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="I75" s="20" t="s">
+        <v>697</v>
+      </c>
+      <c r="J75" s="5" t="s">
+        <v>464</v>
+      </c>
+      <c r="K75" s="57"/>
+      <c r="L75" s="20" t="s">
+        <v>683</v>
+      </c>
+      <c r="M75" t="s">
+        <v>526</v>
+      </c>
+      <c r="N75" s="20" t="s">
+        <v>698</v>
+      </c>
+      <c r="O75" s="20" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="76" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A76">
+        <v>22</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>695</v>
+      </c>
+      <c r="C76" s="67" t="s">
+        <v>383</v>
+      </c>
+      <c r="D76" s="20" t="s">
+        <v>380</v>
+      </c>
+      <c r="E76" t="s">
+        <v>493</v>
+      </c>
+      <c r="F76" s="24" t="s">
+        <v>701</v>
+      </c>
+      <c r="G76" s="20" t="s">
+        <v>321</v>
+      </c>
+      <c r="H76" t="s">
+        <v>61</v>
+      </c>
+      <c r="I76" t="s">
+        <v>575</v>
+      </c>
+      <c r="J76" s="5" t="s">
+        <v>464</v>
+      </c>
+      <c r="K76" s="57"/>
+      <c r="L76" s="20" t="s">
+        <v>682</v>
+      </c>
+      <c r="M76" s="20" t="s">
+        <v>527</v>
+      </c>
+      <c r="N76" s="20" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="77" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A77">
+        <v>23</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="C77" s="67" t="s">
+        <v>384</v>
+      </c>
+      <c r="D77" s="20" t="s">
+        <v>381</v>
+      </c>
+      <c r="E77" t="s">
+        <v>494</v>
+      </c>
+      <c r="F77" s="24" t="s">
+        <v>112</v>
+      </c>
+      <c r="G77" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="H77" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="I77" t="s">
+        <v>576</v>
+      </c>
+      <c r="J77" s="5" t="s">
+        <v>465</v>
+      </c>
+      <c r="K77" s="57"/>
+      <c r="L77" s="20" t="s">
+        <v>682</v>
+      </c>
+      <c r="M77" s="63">
+        <v>1</v>
+      </c>
+      <c r="N77" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="78" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A78">
+        <v>24</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>694</v>
+      </c>
+      <c r="C78" s="67" t="s">
+        <v>388</v>
+      </c>
+      <c r="D78" s="20" t="s">
+        <v>387</v>
+      </c>
+      <c r="E78" t="s">
+        <v>495</v>
+      </c>
+      <c r="F78" s="24" t="s">
+        <v>232</v>
+      </c>
+      <c r="G78" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="H78" t="s">
+        <v>61</v>
+      </c>
+      <c r="I78" t="s">
+        <v>577</v>
+      </c>
+      <c r="J78" s="5" t="s">
+        <v>465</v>
+      </c>
+      <c r="K78" s="57"/>
+      <c r="L78" s="20" t="s">
+        <v>682</v>
+      </c>
+      <c r="M78" s="63">
+        <v>1</v>
+      </c>
+      <c r="N78" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="79" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A79">
+        <v>25</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="C79" s="67" t="s">
+        <v>390</v>
+      </c>
+      <c r="D79" s="20" t="s">
+        <v>391</v>
+      </c>
+      <c r="E79" t="s">
+        <v>496</v>
+      </c>
+      <c r="F79" s="24" t="s">
+        <v>232</v>
+      </c>
+      <c r="G79" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="H79" t="s">
+        <v>61</v>
+      </c>
+      <c r="I79" t="s">
+        <v>578</v>
+      </c>
+      <c r="J79" s="5" t="s">
+        <v>465</v>
+      </c>
+      <c r="K79" s="57"/>
+      <c r="L79" s="20" t="s">
+        <v>682</v>
+      </c>
+      <c r="M79" s="63">
+        <v>1</v>
+      </c>
+      <c r="N79" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="80" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A80">
+        <v>26</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>694</v>
+      </c>
+      <c r="C80" s="67" t="s">
+        <v>395</v>
+      </c>
+      <c r="D80" s="20" t="s">
+        <v>393</v>
+      </c>
+      <c r="E80" t="s">
+        <v>497</v>
+      </c>
+      <c r="F80" s="24" t="s">
+        <v>396</v>
+      </c>
+      <c r="G80" s="20" t="s">
+        <v>239</v>
+      </c>
+      <c r="H80" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="I80" t="s">
+        <v>579</v>
+      </c>
+      <c r="J80" s="5" t="s">
+        <v>465</v>
+      </c>
+      <c r="K80" s="57"/>
+      <c r="L80" s="20" t="s">
+        <v>682</v>
+      </c>
+      <c r="M80" s="64">
+        <v>1</v>
+      </c>
+      <c r="N80" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="81" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A81">
+        <v>27</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>695</v>
+      </c>
+      <c r="C81" s="67" t="s">
+        <v>398</v>
+      </c>
+      <c r="D81" s="20" t="s">
+        <v>399</v>
+      </c>
+      <c r="E81" t="s">
+        <v>498</v>
+      </c>
+      <c r="F81" s="24" t="s">
+        <v>232</v>
+      </c>
+      <c r="G81" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="H81" t="s">
+        <v>61</v>
+      </c>
+      <c r="I81" t="s">
+        <v>580</v>
+      </c>
+      <c r="J81" s="5" t="s">
+        <v>465</v>
+      </c>
+      <c r="K81" s="57"/>
+      <c r="L81" s="20" t="s">
+        <v>682</v>
+      </c>
+      <c r="M81" s="64">
+        <v>1</v>
+      </c>
+      <c r="N81" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="82" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A82">
+        <v>28</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>691</v>
+      </c>
+      <c r="C82" s="67" t="s">
+        <v>433</v>
+      </c>
+      <c r="D82" s="20" t="s">
+        <v>434</v>
+      </c>
+      <c r="E82" s="5" t="s">
+        <v>435</v>
+      </c>
+      <c r="F82" s="24" t="s">
+        <v>436</v>
+      </c>
+      <c r="G82" s="20" t="s">
+        <v>126</v>
+      </c>
+      <c r="H82" t="s">
+        <v>61</v>
+      </c>
+      <c r="I82" t="s">
+        <v>437</v>
+      </c>
+      <c r="J82" s="5" t="s">
+        <v>464</v>
+      </c>
+      <c r="K82" s="56"/>
+      <c r="L82" s="20" t="s">
+        <v>467</v>
+      </c>
+      <c r="M82" t="s">
+        <v>524</v>
+      </c>
+      <c r="N82" s="20" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="83" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A83">
+        <v>29</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>691</v>
+      </c>
+      <c r="C83" s="8" t="s">
+        <v>511</v>
+      </c>
+      <c r="D83" s="71" t="s">
+        <v>512</v>
+      </c>
+      <c r="E83" s="5" t="s">
+        <v>510</v>
+      </c>
+      <c r="F83" s="24" t="s">
+        <v>263</v>
+      </c>
+      <c r="G83" s="20" t="s">
+        <v>239</v>
+      </c>
+      <c r="H83" t="s">
+        <v>61</v>
+      </c>
+      <c r="I83" t="s">
+        <v>513</v>
+      </c>
+      <c r="J83" s="5" t="s">
+        <v>466</v>
+      </c>
+      <c r="K83" s="57"/>
+      <c r="L83" s="20" t="s">
+        <v>673</v>
+      </c>
+      <c r="M83" s="20" t="s">
+        <v>504</v>
+      </c>
+      <c r="N83" s="20" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="84" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A84">
+        <v>30</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>691</v>
+      </c>
+      <c r="C84" s="8" t="s">
+        <v>515</v>
+      </c>
+      <c r="D84" s="71" t="s">
+        <v>516</v>
+      </c>
+      <c r="E84" s="5" t="s">
+        <v>514</v>
+      </c>
+      <c r="F84" s="24" t="s">
+        <v>263</v>
+      </c>
+      <c r="G84" s="20" t="s">
+        <v>239</v>
+      </c>
+      <c r="H84" t="s">
+        <v>61</v>
+      </c>
+      <c r="I84" t="s">
+        <v>517</v>
+      </c>
+      <c r="J84" s="5" t="s">
+        <v>466</v>
+      </c>
+      <c r="K84" s="57"/>
+      <c r="L84" s="20" t="s">
+        <v>673</v>
+      </c>
+      <c r="M84" s="20" t="s">
+        <v>518</v>
+      </c>
+      <c r="N84" s="20" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="85" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A85">
+        <v>31</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="C85" s="66" t="s">
+        <v>584</v>
+      </c>
+      <c r="D85" s="71" t="s">
+        <v>585</v>
+      </c>
+      <c r="E85" s="20" t="s">
+        <v>586</v>
+      </c>
+      <c r="F85" s="24" t="s">
+        <v>589</v>
+      </c>
+      <c r="G85" s="20" t="s">
+        <v>608</v>
+      </c>
+      <c r="H85" t="s">
+        <v>61</v>
+      </c>
+      <c r="I85" t="s">
+        <v>588</v>
+      </c>
+      <c r="J85" s="5" t="s">
+        <v>466</v>
+      </c>
+      <c r="K85" s="59"/>
+      <c r="L85" s="20" t="s">
+        <v>670</v>
+      </c>
+      <c r="M85" s="20" t="s">
+        <v>504</v>
+      </c>
+      <c r="N85" s="20" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="86" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A86">
+        <v>32</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="C86" s="66" t="s">
+        <v>653</v>
+      </c>
+      <c r="D86" s="71" t="s">
+        <v>655</v>
+      </c>
+      <c r="E86" s="66" t="s">
+        <v>657</v>
+      </c>
+      <c r="F86" s="24" t="s">
+        <v>711</v>
+      </c>
+      <c r="G86" s="20" t="s">
+        <v>376</v>
+      </c>
+      <c r="H86" t="s">
+        <v>61</v>
+      </c>
+      <c r="I86" t="s">
+        <v>652</v>
+      </c>
+      <c r="J86" s="5" t="s">
+        <v>464</v>
+      </c>
+      <c r="K86" s="56"/>
+      <c r="L86" s="20" t="s">
+        <v>606</v>
+      </c>
+      <c r="M86" s="20" t="s">
+        <v>504</v>
+      </c>
+      <c r="N86" s="20" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="87" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A87">
+        <v>33</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="C87" s="66" t="s">
+        <v>654</v>
+      </c>
+      <c r="D87" s="71" t="s">
+        <v>656</v>
+      </c>
+      <c r="E87" s="66" t="s">
+        <v>658</v>
+      </c>
+      <c r="F87" s="24" t="s">
+        <v>711</v>
+      </c>
+      <c r="G87" s="20" t="s">
+        <v>376</v>
+      </c>
+      <c r="H87" t="s">
+        <v>61</v>
+      </c>
+      <c r="I87" t="s">
+        <v>659</v>
+      </c>
+      <c r="J87" s="5" t="s">
+        <v>466</v>
+      </c>
+      <c r="K87" s="57"/>
+      <c r="L87" s="20" t="s">
+        <v>671</v>
+      </c>
+      <c r="M87" s="20" t="s">
+        <v>504</v>
+      </c>
+      <c r="N87" s="20" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="88" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C88" s="5"/>
+      <c r="J88" s="5"/>
+      <c r="K88" s="5"/>
+      <c r="L88" s="5"/>
+      <c r="M88" s="5"/>
+    </row>
+    <row r="89" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B89" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="C89" s="27"/>
+      <c r="D89" s="27"/>
+      <c r="E89" s="27"/>
+      <c r="F89" s="27"/>
+      <c r="G89" s="27"/>
+      <c r="H89" s="28"/>
+      <c r="K89" s="58" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="90" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C90" s="24" t="s">
+        <v>82</v>
+      </c>
+      <c r="K90" s="59"/>
+      <c r="L90" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="91" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C91" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="D91" s="42" t="s">
+        <v>84</v>
+      </c>
+      <c r="E91" t="s">
+        <v>85</v>
+      </c>
+      <c r="K91" s="60"/>
+      <c r="L91" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="92" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C92" t="s">
+        <v>423</v>
+      </c>
+      <c r="D92" s="42" t="s">
+        <v>280</v>
+      </c>
+      <c r="E92" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="F92" s="5" t="s">
+        <v>431</v>
+      </c>
+      <c r="K92" s="70"/>
+      <c r="L92" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="93" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C93" t="s">
+        <v>424</v>
+      </c>
+      <c r="D93" s="47" t="s">
+        <v>280</v>
+      </c>
+      <c r="E93" s="64" t="s">
+        <v>280</v>
+      </c>
+      <c r="F93" s="5" t="s">
+        <v>431</v>
+      </c>
+      <c r="K93" s="61"/>
+      <c r="L93" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="94" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C94" t="s">
+        <v>425</v>
+      </c>
+      <c r="D94" s="47" t="s">
+        <v>280</v>
+      </c>
+      <c r="E94" s="64" t="s">
+        <v>280</v>
+      </c>
+      <c r="F94" s="5" t="s">
+        <v>431</v>
+      </c>
+      <c r="J94" s="62" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="95" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C95" t="s">
+        <v>426</v>
+      </c>
+      <c r="D95" s="47" t="s">
+        <v>280</v>
+      </c>
+      <c r="E95" s="64" t="s">
+        <v>280</v>
+      </c>
+      <c r="F95" s="5" t="s">
+        <v>431</v>
+      </c>
+      <c r="J95" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="K95" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="96" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C96" t="s">
+        <v>427</v>
+      </c>
+      <c r="D96" s="47" t="s">
+        <v>280</v>
+      </c>
+      <c r="E96" s="64" t="s">
+        <v>280</v>
+      </c>
+      <c r="F96" s="5" t="s">
+        <v>431</v>
+      </c>
+      <c r="J96" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="K96" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="97" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C97" t="s">
+        <v>428</v>
+      </c>
+      <c r="D97" s="47" t="s">
+        <v>280</v>
+      </c>
+      <c r="E97" s="64" t="s">
+        <v>280</v>
+      </c>
+      <c r="F97" s="5" t="s">
+        <v>431</v>
+      </c>
+      <c r="J97" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="K97" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="98" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C98" t="s">
+        <v>611</v>
+      </c>
+      <c r="D98" s="64" t="s">
+        <v>418</v>
+      </c>
+      <c r="E98" s="64" t="s">
+        <v>612</v>
+      </c>
+      <c r="F98" s="64" t="s">
+        <v>613</v>
+      </c>
+      <c r="J98" s="1"/>
+    </row>
+    <row r="99" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="J99" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="K99" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="100" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B100" s="26" t="s">
+        <v>104</v>
+      </c>
+      <c r="C100" s="27"/>
+      <c r="D100" s="27"/>
+      <c r="E100" s="27"/>
+      <c r="F100" s="27"/>
+      <c r="G100" s="27"/>
+      <c r="H100" s="28"/>
+    </row>
+    <row r="101" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C101" s="24" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="102" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C102" t="s">
+        <v>277</v>
+      </c>
+      <c r="D102" s="42" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="103" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C103" t="s">
+        <v>278</v>
+      </c>
+      <c r="D103" s="42" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="104" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C104" t="s">
+        <v>279</v>
+      </c>
+      <c r="D104" s="42" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="105" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C105" s="5"/>
+      <c r="D105" s="5"/>
+    </row>
+    <row r="106" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C106" s="5"/>
+      <c r="D106" s="5"/>
+    </row>
+    <row r="107" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B107" s="26" t="s">
+        <v>417</v>
+      </c>
+      <c r="C107" s="27"/>
+      <c r="D107" s="27"/>
+      <c r="E107" s="27"/>
+      <c r="F107" s="27"/>
+      <c r="G107" s="27"/>
+      <c r="H107" s="28"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:O107"/>
+  <sheetViews>
+    <sheetView topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="3" topLeftCell="E1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="I86" sqref="I86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2776,7 +5664,7 @@
         <v>0</v>
       </c>
       <c r="D5" s="42" t="s">
-        <v>282</v>
+        <v>614</v>
       </c>
       <c r="I5" s="20"/>
       <c r="J5" s="9"/>
@@ -5142,12 +8030,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:K100"/>
   <sheetViews>
-    <sheetView topLeftCell="E49" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C74" sqref="C74"/>
+    <sheetView topLeftCell="A49" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A57" sqref="A57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6807,7 +9695,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:K87"/>
   <sheetViews>
@@ -8007,7 +10895,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:K52"/>
   <sheetViews>
@@ -8646,7 +11534,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:K69"/>
   <sheetViews>

</xml_diff>

<commit_message>
G7+IC model running through.
</commit_message>
<xml_diff>
--- a/RECC_Config.xlsx
+++ b/RECC_Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="8652" windowHeight="4896" tabRatio="844" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8652" windowHeight="4896" tabRatio="844" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="5" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2310" uniqueCount="713">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2332" uniqueCount="728">
   <si>
     <t>Description</t>
   </si>
@@ -1920,9 +1920,6 @@
     <t>7910f0c7-c7dc-4b54-a35e-961771d9d23a</t>
   </si>
   <si>
-    <t>[2,4,9,12,13,31,32,33,34,35,36,37,38,39]</t>
-  </si>
-  <si>
     <t>2_S_RECC_FinalProducts_2015_G7IC</t>
   </si>
   <si>
@@ -2082,9 +2079,6 @@
     <t>4_EI_WasteMgtEnergyIntensity</t>
   </si>
   <si>
-    <t>specific energy consumption of waste management and remelting processes</t>
-  </si>
-  <si>
     <t>4_EI_WasteMgtEnergyIntensity_V1.0</t>
   </si>
   <si>
@@ -2097,9 +2091,6 @@
     <t>[18:26)</t>
   </si>
   <si>
-    <t>[21:36)</t>
-  </si>
-  <si>
     <t>external</t>
   </si>
   <si>
@@ -2164,6 +2155,60 @@
   </si>
   <si>
     <t>waste management and remelting industries</t>
+  </si>
+  <si>
+    <t>Mining and extraction</t>
+  </si>
+  <si>
+    <t>Obsolete stocks</t>
+  </si>
+  <si>
+    <t>industry/transformation/storage</t>
+  </si>
+  <si>
+    <t>landfills</t>
+  </si>
+  <si>
+    <t>final disposal distribution</t>
+  </si>
+  <si>
+    <t>energy and servie supply</t>
+  </si>
+  <si>
+    <t>energy markets</t>
+  </si>
+  <si>
+    <t>[2,4,9,12,13,31,32,33,34,35,36,37,38,39,40]</t>
+  </si>
+  <si>
+    <t>[0,1,2,3,4,5,6,8,10,11,12,13,14]</t>
+  </si>
+  <si>
+    <t>Environment</t>
+  </si>
+  <si>
+    <t>environment</t>
+  </si>
+  <si>
+    <t>[21,22,23,24,25,26,27,29,31,32,33,34,35]</t>
+  </si>
+  <si>
+    <t>4_EI_RemeltingEnergyIntensity</t>
+  </si>
+  <si>
+    <t>specific energy consumption of waste management (dismantling and sorting) processes</t>
+  </si>
+  <si>
+    <t>specific energy consumption of remelting processes</t>
+  </si>
+  <si>
+    <t>4_EI_RemeltingEnergyIntensity_V1.0</t>
+  </si>
+  <si>
+    <t>d3373d05-627b-486a-aab8-3ffc7bcfa36d</t>
+  </si>
+  <si>
+    <t>gWncr</t>
   </si>
 </sst>
 </file>
@@ -2406,7 +2451,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -2549,6 +2594,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -2875,7 +2921,7 @@
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="6" t="s">
-        <v>702</v>
+        <v>699</v>
       </c>
       <c r="G4" s="48"/>
     </row>
@@ -3026,10 +3072,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:O107"/>
+  <dimension ref="A2:O114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F74" sqref="F74"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C75" sqref="C75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3039,7 +3085,7 @@
     <col min="4" max="4" width="65.77734375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="50.6640625" customWidth="1"/>
     <col min="6" max="6" width="24.6640625" customWidth="1"/>
-    <col min="7" max="7" width="38.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="38.44140625" customWidth="1"/>
     <col min="8" max="8" width="28.21875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="45.109375" customWidth="1"/>
     <col min="12" max="12" width="73.5546875" bestFit="1" customWidth="1"/>
@@ -3078,7 +3124,7 @@
         <v>8</v>
       </c>
       <c r="D4" s="42" t="s">
-        <v>703</v>
+        <v>700</v>
       </c>
       <c r="I4" s="20"/>
       <c r="J4" s="20"/>
@@ -3100,7 +3146,7 @@
         <v>9</v>
       </c>
       <c r="D6" s="43" t="s">
-        <v>704</v>
+        <v>701</v>
       </c>
       <c r="I6" s="20"/>
       <c r="J6" s="20"/>
@@ -3335,7 +3381,7 @@
         <v>40</v>
       </c>
       <c r="G20" t="s">
-        <v>631</v>
+        <v>717</v>
       </c>
       <c r="H20" s="29" t="s">
         <v>45</v>
@@ -3358,7 +3404,7 @@
         <v>155</v>
       </c>
       <c r="G21" t="s">
-        <v>690</v>
+        <v>721</v>
       </c>
       <c r="H21" s="29" t="s">
         <v>184</v>
@@ -3427,7 +3473,7 @@
         <v>106</v>
       </c>
       <c r="G24" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="H24" s="29" t="s">
         <v>48</v>
@@ -3450,7 +3496,7 @@
         <v>134</v>
       </c>
       <c r="G25" t="s">
-        <v>420</v>
+        <v>718</v>
       </c>
       <c r="H25" s="29" t="s">
         <v>337</v>
@@ -3718,54 +3764,63 @@
     </row>
     <row r="39" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C39" s="53">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D39" t="s">
-        <v>450</v>
+        <v>719</v>
       </c>
       <c r="E39" t="s">
-        <v>405</v>
-      </c>
+        <v>720</v>
+      </c>
+      <c r="F39" s="78"/>
+      <c r="G39" s="5"/>
+      <c r="H39" s="5"/>
     </row>
     <row r="40" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C40" s="53">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D40" t="s">
-        <v>452</v>
+        <v>710</v>
       </c>
       <c r="E40" t="s">
-        <v>404</v>
-      </c>
+        <v>712</v>
+      </c>
+      <c r="F40" s="78"/>
+      <c r="G40" s="5"/>
+      <c r="H40" s="5"/>
     </row>
     <row r="41" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C41" s="53">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D41" t="s">
-        <v>453</v>
+        <v>95</v>
       </c>
       <c r="E41" t="s">
         <v>404</v>
       </c>
+      <c r="F41" s="78"/>
+      <c r="G41" s="5"/>
+      <c r="H41" s="5"/>
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C42" s="53">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D42" t="s">
-        <v>407</v>
+        <v>450</v>
       </c>
       <c r="E42" t="s">
-        <v>405</v>
+        <v>712</v>
       </c>
     </row>
     <row r="43" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C43" s="53">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D43" t="s">
-        <v>408</v>
+        <v>452</v>
       </c>
       <c r="E43" t="s">
         <v>404</v>
@@ -3773,24 +3828,21 @@
     </row>
     <row r="44" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C44" s="53">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D44" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="E44" t="s">
-        <v>405</v>
-      </c>
-      <c r="F44" t="s">
-        <v>264</v>
+        <v>712</v>
       </c>
     </row>
     <row r="45" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C45" s="53">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D45" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="E45" t="s">
         <v>404</v>
@@ -3798,21 +3850,21 @@
     </row>
     <row r="46" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C46" s="53">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D46" t="s">
+        <v>409</v>
+      </c>
+      <c r="E46" t="s">
         <v>712</v>
-      </c>
-      <c r="E46" t="s">
-        <v>405</v>
       </c>
     </row>
     <row r="47" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C47" s="53">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D47" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="E47" t="s">
         <v>404</v>
@@ -3820,702 +3872,509 @@
     </row>
     <row r="48" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C48" s="53">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D48" t="s">
-        <v>415</v>
+        <v>709</v>
       </c>
       <c r="E48" t="s">
-        <v>405</v>
-      </c>
-      <c r="F48" t="s">
-        <v>413</v>
+        <v>712</v>
       </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C49" s="53">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D49" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="E49" t="s">
         <v>404</v>
       </c>
-      <c r="F49" t="s">
-        <v>414</v>
-      </c>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="C50" s="73">
+      <c r="C50" s="53">
+        <v>11</v>
+      </c>
+      <c r="D50" t="s">
+        <v>711</v>
+      </c>
+      <c r="E50" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C51" s="53">
+        <v>12</v>
+      </c>
+      <c r="D51" t="s">
+        <v>453</v>
+      </c>
+      <c r="E51" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C52" s="73">
+        <v>13</v>
+      </c>
+      <c r="D52" t="s">
+        <v>713</v>
+      </c>
+      <c r="E52" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C53" s="73">
+        <v>14</v>
+      </c>
+      <c r="D53" t="s">
+        <v>714</v>
+      </c>
+      <c r="E53" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C54" s="73">
         <v>15</v>
       </c>
-      <c r="D50" t="s">
+      <c r="D54" t="s">
+        <v>715</v>
+      </c>
+      <c r="E54" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C55" s="73">
+        <v>16</v>
+      </c>
+      <c r="D55" t="s">
+        <v>716</v>
+      </c>
+      <c r="E55" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C56" s="73">
+        <v>17</v>
+      </c>
+      <c r="D56" t="s">
         <v>628</v>
       </c>
-      <c r="E50" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B52" s="26" t="s">
+      <c r="E56" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B58" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="C52" s="27"/>
-      <c r="D52" s="27"/>
-      <c r="E52" s="27"/>
-      <c r="F52" s="27"/>
-      <c r="G52" s="27"/>
-      <c r="H52" s="28"/>
-    </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B53" s="34" t="s">
+      <c r="C58" s="27"/>
+      <c r="D58" s="27"/>
+      <c r="E58" s="27"/>
+      <c r="F58" s="27"/>
+      <c r="G58" s="27"/>
+      <c r="H58" s="28"/>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B59" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="C53" s="34" t="s">
+      <c r="C59" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="D53" s="31" t="s">
+      <c r="D59" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="E53" s="31" t="s">
+      <c r="E59" s="31" t="s">
         <v>107</v>
       </c>
-      <c r="F53" s="31" t="s">
+      <c r="F59" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="G53" s="31" t="s">
+      <c r="G59" s="31" t="s">
         <v>71</v>
       </c>
-      <c r="H53" s="31" t="s">
+      <c r="H59" s="31" t="s">
         <v>60</v>
       </c>
-      <c r="I53" s="31" t="s">
+      <c r="I59" s="31" t="s">
         <v>297</v>
       </c>
-      <c r="J53" s="54" t="s">
+      <c r="J59" s="54" t="s">
         <v>460</v>
       </c>
-      <c r="K53" s="54" t="s">
+      <c r="K59" s="54" t="s">
         <v>475</v>
       </c>
-      <c r="L53" s="54" t="s">
-        <v>668</v>
-      </c>
-      <c r="M53" s="55" t="s">
+      <c r="L59" s="54" t="s">
+        <v>667</v>
+      </c>
+      <c r="M59" s="55" t="s">
         <v>499</v>
       </c>
-      <c r="N53" s="55" t="s">
+      <c r="N59" s="55" t="s">
         <v>508</v>
-      </c>
-    </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A54">
-        <v>0</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>691</v>
-      </c>
-      <c r="C54" s="35" t="s">
-        <v>292</v>
-      </c>
-      <c r="D54" t="s">
-        <v>293</v>
-      </c>
-      <c r="E54" s="20" t="s">
-        <v>616</v>
-      </c>
-      <c r="F54" s="24" t="s">
-        <v>263</v>
-      </c>
-      <c r="G54" t="s">
-        <v>239</v>
-      </c>
-      <c r="H54" t="s">
-        <v>61</v>
-      </c>
-      <c r="I54" t="s">
-        <v>615</v>
-      </c>
-      <c r="J54" s="5" t="s">
-        <v>462</v>
-      </c>
-      <c r="K54" s="56"/>
-      <c r="L54" s="20" t="s">
-        <v>629</v>
-      </c>
-      <c r="M54" s="20" t="s">
-        <v>501</v>
-      </c>
-      <c r="N54" s="20" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A55">
-        <v>1</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>409</v>
-      </c>
-      <c r="C55" s="35" t="s">
-        <v>632</v>
-      </c>
-      <c r="D55" t="s">
-        <v>301</v>
-      </c>
-      <c r="E55" s="20" t="s">
-        <v>633</v>
-      </c>
-      <c r="F55" s="46" t="s">
-        <v>303</v>
-      </c>
-      <c r="G55" s="20" t="s">
-        <v>239</v>
-      </c>
-      <c r="H55" t="s">
-        <v>61</v>
-      </c>
-      <c r="I55" t="s">
-        <v>630</v>
-      </c>
-      <c r="J55" s="5" t="s">
-        <v>464</v>
-      </c>
-      <c r="K55" s="69"/>
-      <c r="L55" s="20" t="s">
-        <v>675</v>
-      </c>
-      <c r="M55" t="s">
-        <v>500</v>
-      </c>
-      <c r="N55" t="s">
-        <v>533</v>
-      </c>
-    </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A56">
-        <v>2</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>409</v>
-      </c>
-      <c r="C56" s="35" t="s">
-        <v>634</v>
-      </c>
-      <c r="D56" t="s">
-        <v>306</v>
-      </c>
-      <c r="E56" s="20" t="s">
-        <v>635</v>
-      </c>
-      <c r="F56" s="46" t="s">
-        <v>590</v>
-      </c>
-      <c r="G56" s="20" t="s">
-        <v>239</v>
-      </c>
-      <c r="H56" t="s">
-        <v>61</v>
-      </c>
-      <c r="I56" t="s">
-        <v>636</v>
-      </c>
-      <c r="J56" s="5" t="s">
-        <v>462</v>
-      </c>
-      <c r="K56" s="59"/>
-      <c r="L56" s="20" t="s">
-        <v>670</v>
-      </c>
-      <c r="M56" t="s">
-        <v>502</v>
-      </c>
-      <c r="N56" t="s">
-        <v>534</v>
-      </c>
-    </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A57">
-        <v>3</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>409</v>
-      </c>
-      <c r="C57" s="35" t="s">
-        <v>637</v>
-      </c>
-      <c r="D57" s="20" t="s">
-        <v>317</v>
-      </c>
-      <c r="E57" t="s">
-        <v>638</v>
-      </c>
-      <c r="F57" s="46" t="s">
-        <v>710</v>
-      </c>
-      <c r="G57" s="20" t="s">
-        <v>376</v>
-      </c>
-      <c r="H57" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="I57" t="s">
-        <v>639</v>
-      </c>
-      <c r="J57" s="5" t="s">
-        <v>462</v>
-      </c>
-      <c r="K57" s="69"/>
-      <c r="L57" s="20" t="s">
-        <v>675</v>
-      </c>
-      <c r="M57" t="s">
-        <v>522</v>
-      </c>
-      <c r="N57" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A58">
-        <v>4</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>409</v>
-      </c>
-      <c r="C58" s="35" t="s">
-        <v>645</v>
-      </c>
-      <c r="D58" s="20" t="s">
-        <v>648</v>
-      </c>
-      <c r="E58" s="5" t="s">
-        <v>649</v>
-      </c>
-      <c r="F58" s="74" t="s">
-        <v>644</v>
-      </c>
-      <c r="G58" s="20" t="s">
-        <v>321</v>
-      </c>
-      <c r="H58" t="s">
-        <v>61</v>
-      </c>
-      <c r="I58" t="s">
-        <v>640</v>
-      </c>
-      <c r="J58" s="5" t="s">
-        <v>462</v>
-      </c>
-      <c r="K58" s="69"/>
-      <c r="L58" s="20" t="s">
-        <v>675</v>
-      </c>
-      <c r="M58" t="s">
-        <v>651</v>
-      </c>
-      <c r="N58" t="s">
-        <v>539</v>
-      </c>
-    </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A59">
-        <v>5</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>409</v>
-      </c>
-      <c r="C59" s="75" t="s">
-        <v>646</v>
-      </c>
-      <c r="D59" s="20" t="s">
-        <v>647</v>
-      </c>
-      <c r="E59" s="66" t="s">
-        <v>650</v>
-      </c>
-      <c r="F59" s="74" t="s">
-        <v>643</v>
-      </c>
-      <c r="G59" s="20" t="s">
-        <v>321</v>
-      </c>
-      <c r="H59" t="s">
-        <v>61</v>
-      </c>
-      <c r="I59" t="s">
-        <v>619</v>
-      </c>
-      <c r="J59" s="5" t="s">
-        <v>464</v>
-      </c>
-      <c r="K59" s="69"/>
-      <c r="L59" s="20" t="s">
-        <v>675</v>
-      </c>
-      <c r="M59" s="20" t="s">
-        <v>676</v>
-      </c>
-      <c r="N59" s="20" t="s">
-        <v>618</v>
       </c>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A60">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>409</v>
-      </c>
-      <c r="C60" s="67" t="s">
-        <v>329</v>
-      </c>
-      <c r="D60" s="20" t="s">
-        <v>325</v>
-      </c>
-      <c r="E60" t="s">
-        <v>641</v>
+        <v>688</v>
+      </c>
+      <c r="C60" s="35" t="s">
+        <v>292</v>
+      </c>
+      <c r="D60" t="s">
+        <v>293</v>
+      </c>
+      <c r="E60" s="20" t="s">
+        <v>616</v>
       </c>
       <c r="F60" s="24" t="s">
-        <v>275</v>
-      </c>
-      <c r="G60" s="20" t="s">
-        <v>113</v>
-      </c>
-      <c r="H60" s="20" t="s">
+        <v>263</v>
+      </c>
+      <c r="G60" t="s">
+        <v>239</v>
+      </c>
+      <c r="H60" t="s">
         <v>61</v>
       </c>
       <c r="I60" t="s">
-        <v>642</v>
+        <v>615</v>
       </c>
       <c r="J60" s="5" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="K60" s="56"/>
       <c r="L60" s="20" t="s">
-        <v>523</v>
+        <v>629</v>
       </c>
       <c r="M60" s="20" t="s">
-        <v>520</v>
+        <v>501</v>
       </c>
       <c r="N60" s="20" t="s">
-        <v>545</v>
+        <v>532</v>
       </c>
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A61">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>409</v>
       </c>
-      <c r="C61" s="8" t="s">
-        <v>661</v>
-      </c>
-      <c r="D61" s="71" t="s">
-        <v>664</v>
-      </c>
-      <c r="E61" s="8" t="s">
-        <v>662</v>
-      </c>
-      <c r="F61" s="24" t="s">
-        <v>339</v>
+      <c r="C61" s="35" t="s">
+        <v>631</v>
+      </c>
+      <c r="D61" t="s">
+        <v>301</v>
+      </c>
+      <c r="E61" s="20" t="s">
+        <v>632</v>
+      </c>
+      <c r="F61" s="46" t="s">
+        <v>303</v>
       </c>
       <c r="G61" s="20" t="s">
-        <v>321</v>
+        <v>239</v>
       </c>
       <c r="H61" t="s">
         <v>61</v>
       </c>
       <c r="I61" t="s">
-        <v>666</v>
+        <v>630</v>
       </c>
       <c r="J61" s="5" t="s">
         <v>464</v>
       </c>
       <c r="K61" s="69"/>
       <c r="L61" s="20" t="s">
-        <v>675</v>
-      </c>
-      <c r="M61" s="20" t="s">
-        <v>507</v>
-      </c>
-      <c r="N61" s="20" t="s">
-        <v>540</v>
+        <v>674</v>
+      </c>
+      <c r="M61" t="s">
+        <v>500</v>
+      </c>
+      <c r="N61" t="s">
+        <v>533</v>
       </c>
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A62">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>409</v>
       </c>
-      <c r="C62" s="67" t="s">
-        <v>660</v>
-      </c>
-      <c r="D62" s="71" t="s">
-        <v>665</v>
-      </c>
-      <c r="E62" s="8" t="s">
-        <v>663</v>
-      </c>
-      <c r="F62" s="24" t="s">
-        <v>339</v>
+      <c r="C62" s="35" t="s">
+        <v>633</v>
+      </c>
+      <c r="D62" t="s">
+        <v>306</v>
+      </c>
+      <c r="E62" s="20" t="s">
+        <v>634</v>
+      </c>
+      <c r="F62" s="46" t="s">
+        <v>590</v>
       </c>
       <c r="G62" s="20" t="s">
-        <v>321</v>
+        <v>239</v>
       </c>
       <c r="H62" t="s">
         <v>61</v>
       </c>
       <c r="I62" t="s">
-        <v>667</v>
+        <v>635</v>
       </c>
       <c r="J62" s="5" t="s">
-        <v>464</v>
-      </c>
-      <c r="K62" s="69"/>
+        <v>462</v>
+      </c>
+      <c r="K62" s="59"/>
       <c r="L62" s="20" t="s">
-        <v>675</v>
-      </c>
-      <c r="M62" s="20" t="s">
-        <v>506</v>
-      </c>
-      <c r="N62" s="20" t="s">
-        <v>540</v>
+        <v>669</v>
+      </c>
+      <c r="M62" t="s">
+        <v>502</v>
+      </c>
+      <c r="N62" t="s">
+        <v>534</v>
       </c>
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A63">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>409</v>
       </c>
-      <c r="C63" s="67" t="s">
-        <v>442</v>
+      <c r="C63" s="35" t="s">
+        <v>636</v>
       </c>
       <c r="D63" s="20" t="s">
-        <v>440</v>
-      </c>
-      <c r="E63" s="5" t="s">
-        <v>484</v>
-      </c>
-      <c r="F63" s="24" t="s">
-        <v>448</v>
+        <v>317</v>
+      </c>
+      <c r="E63" t="s">
+        <v>637</v>
+      </c>
+      <c r="F63" s="46" t="s">
+        <v>707</v>
       </c>
       <c r="G63" s="20" t="s">
-        <v>126</v>
+        <v>376</v>
       </c>
       <c r="H63" s="20" t="s">
         <v>61</v>
       </c>
       <c r="I63" t="s">
-        <v>565</v>
+        <v>638</v>
       </c>
       <c r="J63" s="5" t="s">
-        <v>464</v>
-      </c>
-      <c r="K63" s="56"/>
+        <v>462</v>
+      </c>
+      <c r="K63" s="69"/>
       <c r="L63" s="20" t="s">
-        <v>603</v>
-      </c>
-      <c r="M63" s="20" t="s">
-        <v>509</v>
-      </c>
-      <c r="N63" s="20" t="s">
-        <v>541</v>
+        <v>674</v>
+      </c>
+      <c r="M63" t="s">
+        <v>522</v>
+      </c>
+      <c r="N63" t="s">
+        <v>538</v>
       </c>
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A64">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>692</v>
-      </c>
-      <c r="C64" s="67" t="s">
-        <v>443</v>
+        <v>409</v>
+      </c>
+      <c r="C64" s="35" t="s">
+        <v>644</v>
       </c>
       <c r="D64" s="20" t="s">
-        <v>441</v>
+        <v>647</v>
       </c>
       <c r="E64" s="5" t="s">
-        <v>485</v>
-      </c>
-      <c r="F64" s="24" t="s">
-        <v>448</v>
+        <v>648</v>
+      </c>
+      <c r="F64" s="74" t="s">
+        <v>643</v>
       </c>
       <c r="G64" s="20" t="s">
-        <v>126</v>
-      </c>
-      <c r="H64" s="20" t="s">
+        <v>321</v>
+      </c>
+      <c r="H64" t="s">
         <v>61</v>
       </c>
       <c r="I64" t="s">
-        <v>566</v>
+        <v>639</v>
       </c>
       <c r="J64" s="5" t="s">
-        <v>464</v>
-      </c>
-      <c r="K64" s="56"/>
+        <v>462</v>
+      </c>
+      <c r="K64" s="69"/>
       <c r="L64" s="20" t="s">
-        <v>603</v>
-      </c>
-      <c r="M64" s="20" t="s">
-        <v>509</v>
-      </c>
-      <c r="N64" s="20" t="s">
-        <v>542</v>
+        <v>674</v>
+      </c>
+      <c r="M64" t="s">
+        <v>650</v>
+      </c>
+      <c r="N64" t="s">
+        <v>539</v>
       </c>
     </row>
     <row r="65" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A65">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>691</v>
-      </c>
-      <c r="C65" s="67" t="s">
-        <v>345</v>
+        <v>409</v>
+      </c>
+      <c r="C65" s="75" t="s">
+        <v>645</v>
       </c>
       <c r="D65" s="20" t="s">
-        <v>346</v>
-      </c>
-      <c r="E65" s="5" t="s">
-        <v>677</v>
-      </c>
-      <c r="F65" s="24" t="s">
-        <v>348</v>
+        <v>646</v>
+      </c>
+      <c r="E65" s="66" t="s">
+        <v>649</v>
+      </c>
+      <c r="F65" s="74" t="s">
+        <v>642</v>
       </c>
       <c r="G65" s="20" t="s">
-        <v>239</v>
+        <v>321</v>
       </c>
       <c r="H65" t="s">
         <v>61</v>
       </c>
       <c r="I65" t="s">
-        <v>679</v>
+        <v>619</v>
       </c>
       <c r="J65" s="5" t="s">
-        <v>466</v>
-      </c>
-      <c r="K65" s="56"/>
+        <v>464</v>
+      </c>
+      <c r="K65" s="69"/>
       <c r="L65" s="20" t="s">
-        <v>678</v>
-      </c>
-      <c r="M65" t="s">
-        <v>505</v>
+        <v>674</v>
+      </c>
+      <c r="M65" s="20" t="s">
+        <v>675</v>
       </c>
       <c r="N65" s="20" t="s">
-        <v>543</v>
+        <v>618</v>
       </c>
     </row>
     <row r="66" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A66">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>691</v>
+        <v>409</v>
       </c>
       <c r="C66" s="67" t="s">
-        <v>351</v>
+        <v>329</v>
       </c>
       <c r="D66" s="20" t="s">
-        <v>350</v>
+        <v>325</v>
       </c>
       <c r="E66" t="s">
-        <v>486</v>
+        <v>640</v>
       </c>
       <c r="F66" s="24" t="s">
-        <v>348</v>
+        <v>275</v>
       </c>
       <c r="G66" s="20" t="s">
-        <v>239</v>
+        <v>113</v>
       </c>
       <c r="H66" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="I66" s="36" t="s">
-        <v>680</v>
+      <c r="I66" t="s">
+        <v>641</v>
       </c>
       <c r="J66" s="5" t="s">
-        <v>466</v>
-      </c>
-      <c r="K66" s="57"/>
+        <v>464</v>
+      </c>
+      <c r="K66" s="56"/>
       <c r="L66" s="20" t="s">
-        <v>681</v>
-      </c>
-      <c r="M66" t="s">
-        <v>504</v>
+        <v>523</v>
+      </c>
+      <c r="M66" s="20" t="s">
+        <v>520</v>
       </c>
       <c r="N66" s="20" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
     </row>
     <row r="67" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A67">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>693</v>
-      </c>
-      <c r="C67" s="75" t="s">
-        <v>359</v>
-      </c>
-      <c r="D67" s="20" t="s">
-        <v>356</v>
-      </c>
-      <c r="E67" t="s">
-        <v>487</v>
+        <v>409</v>
+      </c>
+      <c r="C67" s="8" t="s">
+        <v>660</v>
+      </c>
+      <c r="D67" s="71" t="s">
+        <v>663</v>
+      </c>
+      <c r="E67" s="8" t="s">
+        <v>661</v>
       </c>
       <c r="F67" s="24" t="s">
-        <v>354</v>
+        <v>339</v>
       </c>
       <c r="G67" s="20" t="s">
-        <v>239</v>
+        <v>321</v>
       </c>
       <c r="H67" t="s">
         <v>61</v>
       </c>
       <c r="I67" t="s">
-        <v>568</v>
+        <v>665</v>
       </c>
       <c r="J67" s="5" t="s">
-        <v>466</v>
-      </c>
-      <c r="K67" s="77"/>
+        <v>464</v>
+      </c>
+      <c r="K67" s="69"/>
       <c r="L67" s="20" t="s">
-        <v>604</v>
-      </c>
-      <c r="M67" t="s">
-        <v>524</v>
+        <v>674</v>
+      </c>
+      <c r="M67" s="20" t="s">
+        <v>507</v>
       </c>
       <c r="N67" s="20" t="s">
-        <v>547</v>
-      </c>
-      <c r="O67" s="20"/>
+        <v>540</v>
+      </c>
     </row>
     <row r="68" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A68">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>693</v>
-      </c>
-      <c r="C68" s="75" t="s">
-        <v>706</v>
-      </c>
-      <c r="D68" s="20" t="s">
-        <v>356</v>
-      </c>
-      <c r="E68" t="s">
-        <v>707</v>
+        <v>409</v>
+      </c>
+      <c r="C68" s="67" t="s">
+        <v>659</v>
+      </c>
+      <c r="D68" s="71" t="s">
+        <v>664</v>
+      </c>
+      <c r="E68" s="8" t="s">
+        <v>662</v>
       </c>
       <c r="F68" s="24" t="s">
-        <v>709</v>
+        <v>339</v>
       </c>
       <c r="G68" s="20" t="s">
         <v>321</v>
@@ -4524,131 +4383,124 @@
         <v>61</v>
       </c>
       <c r="I68" t="s">
-        <v>708</v>
+        <v>666</v>
       </c>
       <c r="J68" s="5" t="s">
-        <v>466</v>
-      </c>
-      <c r="K68" s="77"/>
+        <v>464</v>
+      </c>
+      <c r="K68" s="69"/>
       <c r="L68" s="20" t="s">
-        <v>705</v>
-      </c>
-      <c r="M68" t="s">
-        <v>524</v>
+        <v>674</v>
+      </c>
+      <c r="M68" s="20" t="s">
+        <v>506</v>
       </c>
       <c r="N68" s="20" t="s">
-        <v>547</v>
-      </c>
-      <c r="O68" s="20"/>
+        <v>540</v>
+      </c>
     </row>
     <row r="69" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A69">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>692</v>
-      </c>
-      <c r="C69" s="76" t="s">
-        <v>360</v>
+        <v>409</v>
+      </c>
+      <c r="C69" s="67" t="s">
+        <v>442</v>
       </c>
       <c r="D69" s="20" t="s">
-        <v>401</v>
+        <v>440</v>
       </c>
       <c r="E69" s="5" t="s">
-        <v>488</v>
-      </c>
-      <c r="F69" s="46" t="s">
-        <v>421</v>
+        <v>484</v>
+      </c>
+      <c r="F69" s="24" t="s">
+        <v>448</v>
       </c>
       <c r="G69" s="20" t="s">
-        <v>239</v>
+        <v>126</v>
       </c>
       <c r="H69" s="20" t="s">
         <v>61</v>
       </c>
       <c r="I69" t="s">
-        <v>569</v>
+        <v>565</v>
       </c>
       <c r="J69" s="5" t="s">
         <v>464</v>
       </c>
-      <c r="K69" s="59"/>
+      <c r="K69" s="56"/>
       <c r="L69" s="20" t="s">
-        <v>670</v>
-      </c>
-      <c r="M69" t="s">
-        <v>525</v>
+        <v>603</v>
+      </c>
+      <c r="M69" s="20" t="s">
+        <v>509</v>
       </c>
       <c r="N69" s="20" t="s">
-        <v>548</v>
-      </c>
-      <c r="O69" s="20" t="s">
-        <v>696</v>
+        <v>541</v>
       </c>
     </row>
     <row r="70" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A70">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>692</v>
-      </c>
-      <c r="C70" s="76" t="s">
-        <v>400</v>
+        <v>689</v>
+      </c>
+      <c r="C70" s="67" t="s">
+        <v>443</v>
       </c>
       <c r="D70" s="20" t="s">
-        <v>554</v>
+        <v>441</v>
       </c>
       <c r="E70" s="5" t="s">
-        <v>489</v>
-      </c>
-      <c r="F70" s="46" t="s">
-        <v>403</v>
+        <v>485</v>
+      </c>
+      <c r="F70" s="24" t="s">
+        <v>448</v>
       </c>
       <c r="G70" s="20" t="s">
-        <v>239</v>
-      </c>
-      <c r="H70" t="s">
+        <v>126</v>
+      </c>
+      <c r="H70" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="I70" s="65" t="s">
-        <v>570</v>
+      <c r="I70" t="s">
+        <v>566</v>
       </c>
       <c r="J70" s="5" t="s">
         <v>464</v>
       </c>
-      <c r="K70" s="59"/>
+      <c r="K70" s="56"/>
       <c r="L70" s="20" t="s">
-        <v>670</v>
-      </c>
-      <c r="M70" t="s">
-        <v>526</v>
+        <v>603</v>
+      </c>
+      <c r="M70" s="20" t="s">
+        <v>509</v>
       </c>
       <c r="N70" s="20" t="s">
-        <v>700</v>
-      </c>
-      <c r="O70" s="20" t="s">
-        <v>696</v>
+        <v>542</v>
       </c>
     </row>
     <row r="71" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A71">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>694</v>
-      </c>
-      <c r="C71" s="76" t="s">
-        <v>553</v>
+        <v>688</v>
+      </c>
+      <c r="C71" s="67" t="s">
+        <v>345</v>
       </c>
       <c r="D71" s="20" t="s">
-        <v>555</v>
+        <v>346</v>
       </c>
       <c r="E71" s="5" t="s">
-        <v>556</v>
-      </c>
-      <c r="F71" s="46" t="s">
-        <v>557</v>
+        <v>676</v>
+      </c>
+      <c r="F71" s="24" t="s">
+        <v>348</v>
       </c>
       <c r="G71" s="20" t="s">
         <v>239</v>
@@ -4657,169 +4509,168 @@
         <v>61</v>
       </c>
       <c r="I71" t="s">
-        <v>571</v>
+        <v>678</v>
       </c>
       <c r="J71" s="5" t="s">
-        <v>464</v>
-      </c>
-      <c r="K71" s="59"/>
+        <v>466</v>
+      </c>
+      <c r="K71" s="56"/>
       <c r="L71" s="20" t="s">
-        <v>670</v>
+        <v>677</v>
       </c>
       <c r="M71" t="s">
-        <v>526</v>
+        <v>505</v>
       </c>
       <c r="N71" s="20" t="s">
-        <v>699</v>
-      </c>
-      <c r="O71" s="20" t="s">
-        <v>696</v>
+        <v>543</v>
       </c>
     </row>
     <row r="72" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A72">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>695</v>
-      </c>
-      <c r="C72" s="75" t="s">
-        <v>361</v>
+        <v>688</v>
+      </c>
+      <c r="C72" s="67" t="s">
+        <v>351</v>
       </c>
       <c r="D72" s="20" t="s">
-        <v>363</v>
+        <v>350</v>
       </c>
       <c r="E72" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
       <c r="F72" s="24" t="s">
-        <v>701</v>
+        <v>348</v>
       </c>
       <c r="G72" s="20" t="s">
-        <v>321</v>
+        <v>239</v>
       </c>
       <c r="H72" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="I72" t="s">
-        <v>572</v>
+      <c r="I72" s="36" t="s">
+        <v>679</v>
       </c>
       <c r="J72" s="5" t="s">
-        <v>464</v>
-      </c>
-      <c r="K72" s="69"/>
+        <v>466</v>
+      </c>
+      <c r="K72" s="57"/>
       <c r="L72" s="20" t="s">
-        <v>683</v>
-      </c>
-      <c r="M72" s="20" t="s">
+        <v>680</v>
+      </c>
+      <c r="M72" t="s">
         <v>504</v>
       </c>
       <c r="N72" s="20" t="s">
-        <v>550</v>
+        <v>544</v>
       </c>
     </row>
     <row r="73" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A73">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>694</v>
+        <v>690</v>
       </c>
       <c r="C73" s="75" t="s">
-        <v>366</v>
+        <v>359</v>
       </c>
       <c r="D73" s="20" t="s">
-        <v>367</v>
+        <v>356</v>
       </c>
       <c r="E73" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="F73" s="24" t="s">
-        <v>430</v>
+        <v>354</v>
       </c>
       <c r="G73" s="20" t="s">
-        <v>376</v>
+        <v>239</v>
       </c>
       <c r="H73" t="s">
         <v>61</v>
       </c>
       <c r="I73" t="s">
-        <v>573</v>
+        <v>568</v>
       </c>
       <c r="J73" s="5" t="s">
-        <v>464</v>
-      </c>
-      <c r="K73" s="69"/>
+        <v>466</v>
+      </c>
+      <c r="K73" s="77"/>
       <c r="L73" s="20" t="s">
-        <v>683</v>
-      </c>
-      <c r="M73" s="63">
-        <v>1</v>
+        <v>604</v>
+      </c>
+      <c r="M73" t="s">
+        <v>524</v>
       </c>
       <c r="N73" s="20" t="s">
-        <v>552</v>
-      </c>
+        <v>547</v>
+      </c>
+      <c r="O73" s="20"/>
     </row>
     <row r="74" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A74">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>695</v>
-      </c>
-      <c r="C74" s="67" t="s">
-        <v>370</v>
+        <v>690</v>
+      </c>
+      <c r="C74" s="75" t="s">
+        <v>703</v>
       </c>
       <c r="D74" s="20" t="s">
-        <v>371</v>
+        <v>356</v>
       </c>
       <c r="E74" t="s">
-        <v>492</v>
+        <v>704</v>
       </c>
       <c r="F74" s="24" t="s">
-        <v>688</v>
+        <v>706</v>
       </c>
       <c r="G74" s="20" t="s">
-        <v>376</v>
-      </c>
-      <c r="H74" s="20" t="s">
+        <v>321</v>
+      </c>
+      <c r="H74" t="s">
         <v>61</v>
       </c>
       <c r="I74" t="s">
-        <v>574</v>
+        <v>705</v>
       </c>
       <c r="J74" s="5" t="s">
-        <v>464</v>
-      </c>
-      <c r="K74" s="56"/>
+        <v>466</v>
+      </c>
+      <c r="K74" s="77"/>
       <c r="L74" s="20" t="s">
-        <v>683</v>
-      </c>
-      <c r="M74" s="63">
-        <v>1</v>
-      </c>
-      <c r="N74" t="s">
-        <v>551</v>
-      </c>
+        <v>702</v>
+      </c>
+      <c r="M74" t="s">
+        <v>524</v>
+      </c>
+      <c r="N74" s="20" t="s">
+        <v>547</v>
+      </c>
+      <c r="O74" s="20"/>
     </row>
     <row r="75" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A75">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>695</v>
+        <v>689</v>
       </c>
       <c r="C75" s="76" t="s">
-        <v>684</v>
+        <v>360</v>
       </c>
       <c r="D75" s="20" t="s">
-        <v>685</v>
-      </c>
-      <c r="E75" s="8" t="s">
-        <v>686</v>
+        <v>401</v>
+      </c>
+      <c r="E75" s="5" t="s">
+        <v>488</v>
       </c>
       <c r="F75" s="46" t="s">
-        <v>687</v>
+        <v>421</v>
       </c>
       <c r="G75" s="20" t="s">
         <v>239</v>
@@ -4827,762 +4678,1020 @@
       <c r="H75" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="I75" s="20" t="s">
-        <v>697</v>
+      <c r="I75" t="s">
+        <v>569</v>
       </c>
       <c r="J75" s="5" t="s">
         <v>464</v>
       </c>
-      <c r="K75" s="57"/>
+      <c r="K75" s="59"/>
       <c r="L75" s="20" t="s">
-        <v>683</v>
+        <v>669</v>
       </c>
       <c r="M75" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="N75" s="20" t="s">
-        <v>698</v>
+        <v>548</v>
       </c>
       <c r="O75" s="20" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
     </row>
     <row r="76" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A76">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>695</v>
-      </c>
-      <c r="C76" s="67" t="s">
-        <v>383</v>
+        <v>689</v>
+      </c>
+      <c r="C76" s="76" t="s">
+        <v>400</v>
       </c>
       <c r="D76" s="20" t="s">
-        <v>380</v>
-      </c>
-      <c r="E76" t="s">
-        <v>493</v>
-      </c>
-      <c r="F76" s="24" t="s">
-        <v>701</v>
+        <v>554</v>
+      </c>
+      <c r="E76" s="5" t="s">
+        <v>489</v>
+      </c>
+      <c r="F76" s="46" t="s">
+        <v>403</v>
       </c>
       <c r="G76" s="20" t="s">
-        <v>321</v>
+        <v>239</v>
       </c>
       <c r="H76" t="s">
         <v>61</v>
       </c>
-      <c r="I76" t="s">
-        <v>575</v>
+      <c r="I76" s="65" t="s">
+        <v>570</v>
       </c>
       <c r="J76" s="5" t="s">
         <v>464</v>
       </c>
-      <c r="K76" s="57"/>
+      <c r="K76" s="59"/>
       <c r="L76" s="20" t="s">
-        <v>682</v>
-      </c>
-      <c r="M76" s="20" t="s">
-        <v>527</v>
+        <v>669</v>
+      </c>
+      <c r="M76" t="s">
+        <v>526</v>
       </c>
       <c r="N76" s="20" t="s">
-        <v>528</v>
+        <v>697</v>
+      </c>
+      <c r="O76" s="20" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="77" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A77">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>409</v>
-      </c>
-      <c r="C77" s="67" t="s">
-        <v>384</v>
+        <v>691</v>
+      </c>
+      <c r="C77" s="76" t="s">
+        <v>553</v>
       </c>
       <c r="D77" s="20" t="s">
-        <v>381</v>
-      </c>
-      <c r="E77" t="s">
-        <v>494</v>
-      </c>
-      <c r="F77" s="24" t="s">
-        <v>112</v>
+        <v>555</v>
+      </c>
+      <c r="E77" s="5" t="s">
+        <v>556</v>
+      </c>
+      <c r="F77" s="46" t="s">
+        <v>557</v>
       </c>
       <c r="G77" s="20" t="s">
-        <v>113</v>
-      </c>
-      <c r="H77" s="20" t="s">
+        <v>239</v>
+      </c>
+      <c r="H77" t="s">
         <v>61</v>
       </c>
       <c r="I77" t="s">
-        <v>576</v>
+        <v>571</v>
       </c>
       <c r="J77" s="5" t="s">
-        <v>465</v>
-      </c>
-      <c r="K77" s="57"/>
+        <v>464</v>
+      </c>
+      <c r="K77" s="59"/>
       <c r="L77" s="20" t="s">
-        <v>682</v>
-      </c>
-      <c r="M77" s="63">
-        <v>1</v>
-      </c>
-      <c r="N77" t="s">
-        <v>529</v>
+        <v>669</v>
+      </c>
+      <c r="M77" t="s">
+        <v>526</v>
+      </c>
+      <c r="N77" s="20" t="s">
+        <v>696</v>
+      </c>
+      <c r="O77" s="20" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="78" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A78">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>694</v>
-      </c>
-      <c r="C78" s="67" t="s">
-        <v>388</v>
+        <v>692</v>
+      </c>
+      <c r="C78" s="75" t="s">
+        <v>361</v>
       </c>
       <c r="D78" s="20" t="s">
-        <v>387</v>
+        <v>363</v>
       </c>
       <c r="E78" t="s">
-        <v>495</v>
+        <v>490</v>
       </c>
       <c r="F78" s="24" t="s">
-        <v>232</v>
+        <v>698</v>
       </c>
       <c r="G78" s="20" t="s">
-        <v>113</v>
-      </c>
-      <c r="H78" t="s">
+        <v>321</v>
+      </c>
+      <c r="H78" s="20" t="s">
         <v>61</v>
       </c>
       <c r="I78" t="s">
-        <v>577</v>
+        <v>572</v>
       </c>
       <c r="J78" s="5" t="s">
-        <v>465</v>
-      </c>
-      <c r="K78" s="57"/>
+        <v>464</v>
+      </c>
+      <c r="K78" s="69"/>
       <c r="L78" s="20" t="s">
         <v>682</v>
       </c>
-      <c r="M78" s="63">
-        <v>1</v>
-      </c>
-      <c r="N78" t="s">
-        <v>535</v>
+      <c r="M78" s="20" t="s">
+        <v>504</v>
+      </c>
+      <c r="N78" s="20" t="s">
+        <v>550</v>
       </c>
     </row>
     <row r="79" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A79">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>409</v>
-      </c>
-      <c r="C79" s="67" t="s">
-        <v>390</v>
+        <v>691</v>
+      </c>
+      <c r="C79" s="75" t="s">
+        <v>366</v>
       </c>
       <c r="D79" s="20" t="s">
-        <v>391</v>
+        <v>367</v>
       </c>
       <c r="E79" t="s">
-        <v>496</v>
+        <v>491</v>
       </c>
       <c r="F79" s="24" t="s">
-        <v>232</v>
+        <v>430</v>
       </c>
       <c r="G79" s="20" t="s">
-        <v>113</v>
+        <v>376</v>
       </c>
       <c r="H79" t="s">
         <v>61</v>
       </c>
       <c r="I79" t="s">
-        <v>578</v>
+        <v>573</v>
       </c>
       <c r="J79" s="5" t="s">
-        <v>465</v>
-      </c>
-      <c r="K79" s="57"/>
+        <v>464</v>
+      </c>
+      <c r="K79" s="69"/>
       <c r="L79" s="20" t="s">
         <v>682</v>
       </c>
       <c r="M79" s="63">
         <v>1</v>
       </c>
-      <c r="N79" t="s">
-        <v>530</v>
+      <c r="N79" s="20" t="s">
+        <v>552</v>
       </c>
     </row>
     <row r="80" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A80">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="C80" s="67" t="s">
-        <v>395</v>
+        <v>370</v>
       </c>
       <c r="D80" s="20" t="s">
-        <v>393</v>
+        <v>371</v>
       </c>
       <c r="E80" t="s">
-        <v>497</v>
+        <v>492</v>
       </c>
       <c r="F80" s="24" t="s">
-        <v>396</v>
+        <v>686</v>
       </c>
       <c r="G80" s="20" t="s">
-        <v>239</v>
+        <v>376</v>
       </c>
       <c r="H80" s="20" t="s">
         <v>61</v>
       </c>
       <c r="I80" t="s">
-        <v>579</v>
+        <v>574</v>
       </c>
       <c r="J80" s="5" t="s">
-        <v>465</v>
-      </c>
-      <c r="K80" s="57"/>
+        <v>464</v>
+      </c>
+      <c r="K80" s="56"/>
       <c r="L80" s="20" t="s">
         <v>682</v>
       </c>
-      <c r="M80" s="64">
+      <c r="M80" s="63">
         <v>1</v>
       </c>
       <c r="N80" t="s">
-        <v>536</v>
-      </c>
-    </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.3">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="81" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A81">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>695</v>
-      </c>
-      <c r="C81" s="67" t="s">
-        <v>398</v>
+        <v>692</v>
+      </c>
+      <c r="C81" s="76" t="s">
+        <v>683</v>
       </c>
       <c r="D81" s="20" t="s">
-        <v>399</v>
-      </c>
-      <c r="E81" t="s">
-        <v>498</v>
-      </c>
-      <c r="F81" s="24" t="s">
-        <v>232</v>
+        <v>723</v>
+      </c>
+      <c r="E81" s="8" t="s">
+        <v>684</v>
+      </c>
+      <c r="F81" s="46" t="s">
+        <v>727</v>
       </c>
       <c r="G81" s="20" t="s">
-        <v>113</v>
-      </c>
-      <c r="H81" t="s">
+        <v>321</v>
+      </c>
+      <c r="H81" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="I81" t="s">
-        <v>580</v>
+      <c r="I81" s="20" t="s">
+        <v>694</v>
       </c>
       <c r="J81" s="5" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="K81" s="57"/>
       <c r="L81" s="20" t="s">
         <v>682</v>
       </c>
-      <c r="M81" s="64">
-        <v>1</v>
-      </c>
-      <c r="N81" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="M81" t="s">
+        <v>526</v>
+      </c>
+      <c r="N81" s="20" t="s">
+        <v>695</v>
+      </c>
+      <c r="O81" s="20" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="82" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A82">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>691</v>
-      </c>
-      <c r="C82" s="67" t="s">
-        <v>433</v>
+        <v>692</v>
+      </c>
+      <c r="C82" s="76" t="s">
+        <v>722</v>
       </c>
       <c r="D82" s="20" t="s">
-        <v>434</v>
-      </c>
-      <c r="E82" s="5" t="s">
-        <v>435</v>
-      </c>
-      <c r="F82" s="24" t="s">
-        <v>436</v>
+        <v>724</v>
+      </c>
+      <c r="E82" s="8" t="s">
+        <v>725</v>
+      </c>
+      <c r="F82" s="46" t="s">
+        <v>685</v>
       </c>
       <c r="G82" s="20" t="s">
-        <v>126</v>
-      </c>
-      <c r="H82" t="s">
+        <v>239</v>
+      </c>
+      <c r="H82" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="I82" t="s">
-        <v>437</v>
+      <c r="I82" s="20" t="s">
+        <v>726</v>
       </c>
       <c r="J82" s="5" t="s">
         <v>464</v>
       </c>
-      <c r="K82" s="56"/>
+      <c r="K82" s="57"/>
       <c r="L82" s="20" t="s">
-        <v>467</v>
+        <v>682</v>
       </c>
       <c r="M82" t="s">
-        <v>524</v>
+        <v>526</v>
       </c>
       <c r="N82" s="20" t="s">
-        <v>546</v>
-      </c>
-    </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.3">
+        <v>695</v>
+      </c>
+      <c r="O82" s="20" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="83" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A83">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>691</v>
-      </c>
-      <c r="C83" s="8" t="s">
-        <v>511</v>
-      </c>
-      <c r="D83" s="71" t="s">
-        <v>512</v>
-      </c>
-      <c r="E83" s="5" t="s">
-        <v>510</v>
+        <v>692</v>
+      </c>
+      <c r="C83" s="67" t="s">
+        <v>383</v>
+      </c>
+      <c r="D83" s="20" t="s">
+        <v>380</v>
+      </c>
+      <c r="E83" t="s">
+        <v>493</v>
       </c>
       <c r="F83" s="24" t="s">
-        <v>263</v>
+        <v>698</v>
       </c>
       <c r="G83" s="20" t="s">
-        <v>239</v>
+        <v>321</v>
       </c>
       <c r="H83" t="s">
         <v>61</v>
       </c>
       <c r="I83" t="s">
-        <v>513</v>
+        <v>575</v>
       </c>
       <c r="J83" s="5" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="K83" s="57"/>
       <c r="L83" s="20" t="s">
-        <v>673</v>
+        <v>681</v>
       </c>
       <c r="M83" s="20" t="s">
-        <v>504</v>
+        <v>527</v>
       </c>
       <c r="N83" s="20" t="s">
-        <v>519</v>
-      </c>
-    </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.3">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="84" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A84">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>691</v>
-      </c>
-      <c r="C84" s="8" t="s">
-        <v>515</v>
-      </c>
-      <c r="D84" s="71" t="s">
-        <v>516</v>
-      </c>
-      <c r="E84" s="5" t="s">
-        <v>514</v>
+        <v>409</v>
+      </c>
+      <c r="C84" s="67" t="s">
+        <v>384</v>
+      </c>
+      <c r="D84" s="20" t="s">
+        <v>381</v>
+      </c>
+      <c r="E84" t="s">
+        <v>494</v>
       </c>
       <c r="F84" s="24" t="s">
-        <v>263</v>
+        <v>112</v>
       </c>
       <c r="G84" s="20" t="s">
-        <v>239</v>
-      </c>
-      <c r="H84" t="s">
+        <v>113</v>
+      </c>
+      <c r="H84" s="20" t="s">
         <v>61</v>
       </c>
       <c r="I84" t="s">
-        <v>517</v>
+        <v>576</v>
       </c>
       <c r="J84" s="5" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="K84" s="57"/>
       <c r="L84" s="20" t="s">
-        <v>673</v>
-      </c>
-      <c r="M84" s="20" t="s">
-        <v>518</v>
-      </c>
-      <c r="N84" s="20" t="s">
-        <v>519</v>
-      </c>
-    </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.3">
+        <v>681</v>
+      </c>
+      <c r="M84" s="63">
+        <v>1</v>
+      </c>
+      <c r="N84" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="85" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A85">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>409</v>
-      </c>
-      <c r="C85" s="66" t="s">
-        <v>584</v>
-      </c>
-      <c r="D85" s="71" t="s">
-        <v>585</v>
-      </c>
-      <c r="E85" s="20" t="s">
-        <v>586</v>
+        <v>691</v>
+      </c>
+      <c r="C85" s="67" t="s">
+        <v>388</v>
+      </c>
+      <c r="D85" s="20" t="s">
+        <v>387</v>
+      </c>
+      <c r="E85" t="s">
+        <v>495</v>
       </c>
       <c r="F85" s="24" t="s">
-        <v>589</v>
+        <v>232</v>
       </c>
       <c r="G85" s="20" t="s">
-        <v>608</v>
+        <v>113</v>
       </c>
       <c r="H85" t="s">
         <v>61</v>
       </c>
       <c r="I85" t="s">
-        <v>588</v>
+        <v>577</v>
       </c>
       <c r="J85" s="5" t="s">
-        <v>466</v>
-      </c>
-      <c r="K85" s="59"/>
+        <v>465</v>
+      </c>
+      <c r="K85" s="57"/>
       <c r="L85" s="20" t="s">
-        <v>670</v>
-      </c>
-      <c r="M85" s="20" t="s">
-        <v>504</v>
-      </c>
-      <c r="N85" s="20" t="s">
-        <v>587</v>
-      </c>
-    </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.3">
+        <v>681</v>
+      </c>
+      <c r="M85" s="63">
+        <v>1</v>
+      </c>
+      <c r="N85" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="86" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A86">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>409</v>
       </c>
-      <c r="C86" s="66" t="s">
-        <v>653</v>
-      </c>
-      <c r="D86" s="71" t="s">
-        <v>655</v>
-      </c>
-      <c r="E86" s="66" t="s">
-        <v>657</v>
+      <c r="C86" s="67" t="s">
+        <v>390</v>
+      </c>
+      <c r="D86" s="20" t="s">
+        <v>391</v>
+      </c>
+      <c r="E86" t="s">
+        <v>496</v>
       </c>
       <c r="F86" s="24" t="s">
-        <v>711</v>
+        <v>232</v>
       </c>
       <c r="G86" s="20" t="s">
-        <v>376</v>
+        <v>113</v>
       </c>
       <c r="H86" t="s">
         <v>61</v>
       </c>
       <c r="I86" t="s">
-        <v>652</v>
+        <v>578</v>
       </c>
       <c r="J86" s="5" t="s">
-        <v>464</v>
-      </c>
-      <c r="K86" s="56"/>
+        <v>465</v>
+      </c>
+      <c r="K86" s="57"/>
       <c r="L86" s="20" t="s">
-        <v>606</v>
-      </c>
-      <c r="M86" s="20" t="s">
-        <v>504</v>
-      </c>
-      <c r="N86" s="20" t="s">
-        <v>672</v>
-      </c>
-    </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.3">
+        <v>681</v>
+      </c>
+      <c r="M86" s="63">
+        <v>1</v>
+      </c>
+      <c r="N86" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="87" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A87">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>409</v>
-      </c>
-      <c r="C87" s="66" t="s">
-        <v>654</v>
-      </c>
-      <c r="D87" s="71" t="s">
-        <v>656</v>
-      </c>
-      <c r="E87" s="66" t="s">
-        <v>658</v>
+        <v>691</v>
+      </c>
+      <c r="C87" s="67" t="s">
+        <v>395</v>
+      </c>
+      <c r="D87" s="20" t="s">
+        <v>393</v>
+      </c>
+      <c r="E87" t="s">
+        <v>497</v>
       </c>
       <c r="F87" s="24" t="s">
-        <v>711</v>
+        <v>396</v>
       </c>
       <c r="G87" s="20" t="s">
-        <v>376</v>
-      </c>
-      <c r="H87" t="s">
+        <v>239</v>
+      </c>
+      <c r="H87" s="20" t="s">
         <v>61</v>
       </c>
       <c r="I87" t="s">
-        <v>659</v>
+        <v>579</v>
       </c>
       <c r="J87" s="5" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="K87" s="57"/>
       <c r="L87" s="20" t="s">
+        <v>681</v>
+      </c>
+      <c r="M87" s="64">
+        <v>1</v>
+      </c>
+      <c r="N87" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="88" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A88">
+        <v>28</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>692</v>
+      </c>
+      <c r="C88" s="67" t="s">
+        <v>398</v>
+      </c>
+      <c r="D88" s="20" t="s">
+        <v>399</v>
+      </c>
+      <c r="E88" t="s">
+        <v>498</v>
+      </c>
+      <c r="F88" s="24" t="s">
+        <v>232</v>
+      </c>
+      <c r="G88" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="H88" t="s">
+        <v>61</v>
+      </c>
+      <c r="I88" t="s">
+        <v>580</v>
+      </c>
+      <c r="J88" s="5" t="s">
+        <v>465</v>
+      </c>
+      <c r="K88" s="57"/>
+      <c r="L88" s="20" t="s">
+        <v>681</v>
+      </c>
+      <c r="M88" s="64">
+        <v>1</v>
+      </c>
+      <c r="N88" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="89" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A89">
+        <v>29</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>688</v>
+      </c>
+      <c r="C89" s="67" t="s">
+        <v>433</v>
+      </c>
+      <c r="D89" s="20" t="s">
+        <v>434</v>
+      </c>
+      <c r="E89" s="5" t="s">
+        <v>435</v>
+      </c>
+      <c r="F89" s="24" t="s">
+        <v>436</v>
+      </c>
+      <c r="G89" s="20" t="s">
+        <v>126</v>
+      </c>
+      <c r="H89" t="s">
+        <v>61</v>
+      </c>
+      <c r="I89" t="s">
+        <v>437</v>
+      </c>
+      <c r="J89" s="5" t="s">
+        <v>464</v>
+      </c>
+      <c r="K89" s="56"/>
+      <c r="L89" s="20" t="s">
+        <v>467</v>
+      </c>
+      <c r="M89" t="s">
+        <v>524</v>
+      </c>
+      <c r="N89" s="20" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="90" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A90">
+        <v>30</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>688</v>
+      </c>
+      <c r="C90" s="8" t="s">
+        <v>511</v>
+      </c>
+      <c r="D90" s="71" t="s">
+        <v>512</v>
+      </c>
+      <c r="E90" s="5" t="s">
+        <v>510</v>
+      </c>
+      <c r="F90" s="24" t="s">
+        <v>263</v>
+      </c>
+      <c r="G90" s="20" t="s">
+        <v>239</v>
+      </c>
+      <c r="H90" t="s">
+        <v>61</v>
+      </c>
+      <c r="I90" t="s">
+        <v>513</v>
+      </c>
+      <c r="J90" s="5" t="s">
+        <v>466</v>
+      </c>
+      <c r="K90" s="57"/>
+      <c r="L90" s="20" t="s">
+        <v>672</v>
+      </c>
+      <c r="M90" s="20" t="s">
+        <v>504</v>
+      </c>
+      <c r="N90" s="20" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="91" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A91">
+        <v>31</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>688</v>
+      </c>
+      <c r="C91" s="8" t="s">
+        <v>515</v>
+      </c>
+      <c r="D91" s="71" t="s">
+        <v>516</v>
+      </c>
+      <c r="E91" s="5" t="s">
+        <v>514</v>
+      </c>
+      <c r="F91" s="24" t="s">
+        <v>263</v>
+      </c>
+      <c r="G91" s="20" t="s">
+        <v>239</v>
+      </c>
+      <c r="H91" t="s">
+        <v>61</v>
+      </c>
+      <c r="I91" t="s">
+        <v>517</v>
+      </c>
+      <c r="J91" s="5" t="s">
+        <v>466</v>
+      </c>
+      <c r="K91" s="57"/>
+      <c r="L91" s="20" t="s">
+        <v>672</v>
+      </c>
+      <c r="M91" s="20" t="s">
+        <v>518</v>
+      </c>
+      <c r="N91" s="20" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="92" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A92">
+        <v>32</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="C92" s="66" t="s">
+        <v>584</v>
+      </c>
+      <c r="D92" s="71" t="s">
+        <v>585</v>
+      </c>
+      <c r="E92" s="20" t="s">
+        <v>586</v>
+      </c>
+      <c r="F92" s="24" t="s">
+        <v>589</v>
+      </c>
+      <c r="G92" s="20" t="s">
+        <v>608</v>
+      </c>
+      <c r="H92" t="s">
+        <v>61</v>
+      </c>
+      <c r="I92" t="s">
+        <v>588</v>
+      </c>
+      <c r="J92" s="5" t="s">
+        <v>466</v>
+      </c>
+      <c r="K92" s="59"/>
+      <c r="L92" s="20" t="s">
+        <v>669</v>
+      </c>
+      <c r="M92" s="20" t="s">
+        <v>504</v>
+      </c>
+      <c r="N92" s="20" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="93" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A93">
+        <v>33</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="C93" s="66" t="s">
+        <v>652</v>
+      </c>
+      <c r="D93" s="71" t="s">
+        <v>654</v>
+      </c>
+      <c r="E93" s="66" t="s">
+        <v>656</v>
+      </c>
+      <c r="F93" s="24" t="s">
+        <v>708</v>
+      </c>
+      <c r="G93" s="20" t="s">
+        <v>376</v>
+      </c>
+      <c r="H93" t="s">
+        <v>61</v>
+      </c>
+      <c r="I93" t="s">
+        <v>651</v>
+      </c>
+      <c r="J93" s="5" t="s">
+        <v>464</v>
+      </c>
+      <c r="K93" s="56"/>
+      <c r="L93" s="20" t="s">
+        <v>606</v>
+      </c>
+      <c r="M93" s="20" t="s">
+        <v>504</v>
+      </c>
+      <c r="N93" s="20" t="s">
         <v>671</v>
       </c>
-      <c r="M87" s="20" t="s">
+    </row>
+    <row r="94" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A94">
+        <v>34</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="C94" s="66" t="s">
+        <v>653</v>
+      </c>
+      <c r="D94" s="71" t="s">
+        <v>655</v>
+      </c>
+      <c r="E94" s="66" t="s">
+        <v>657</v>
+      </c>
+      <c r="F94" s="24" t="s">
+        <v>708</v>
+      </c>
+      <c r="G94" s="20" t="s">
+        <v>376</v>
+      </c>
+      <c r="H94" t="s">
+        <v>61</v>
+      </c>
+      <c r="I94" t="s">
+        <v>658</v>
+      </c>
+      <c r="J94" s="5" t="s">
+        <v>466</v>
+      </c>
+      <c r="K94" s="57"/>
+      <c r="L94" s="20" t="s">
+        <v>670</v>
+      </c>
+      <c r="M94" s="20" t="s">
         <v>504</v>
       </c>
-      <c r="N87" s="20" t="s">
+      <c r="N94" s="20" t="s">
         <v>597</v>
       </c>
     </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="C88" s="5"/>
-      <c r="J88" s="5"/>
-      <c r="K88" s="5"/>
-      <c r="L88" s="5"/>
-      <c r="M88" s="5"/>
-    </row>
-    <row r="89" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B89" s="26" t="s">
+    <row r="95" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="C95" s="5"/>
+      <c r="J95" s="5"/>
+      <c r="K95" s="5"/>
+      <c r="L95" s="5"/>
+      <c r="M95" s="5"/>
+    </row>
+    <row r="96" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B96" s="26" t="s">
         <v>81</v>
       </c>
-      <c r="C89" s="27"/>
-      <c r="D89" s="27"/>
-      <c r="E89" s="27"/>
-      <c r="F89" s="27"/>
-      <c r="G89" s="27"/>
-      <c r="H89" s="28"/>
-      <c r="K89" s="58" t="s">
+      <c r="C96" s="27"/>
+      <c r="D96" s="27"/>
+      <c r="E96" s="27"/>
+      <c r="F96" s="27"/>
+      <c r="G96" s="27"/>
+      <c r="H96" s="28"/>
+      <c r="K96" s="58" t="s">
         <v>468</v>
       </c>
     </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="C90" s="24" t="s">
+    <row r="97" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="C97" s="24" t="s">
         <v>82</v>
       </c>
-      <c r="K90" s="59"/>
-      <c r="L90" t="s">
-        <v>669</v>
-      </c>
-    </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="C91" s="35" t="s">
+      <c r="K97" s="59"/>
+      <c r="L97" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="98" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="C98" s="35" t="s">
         <v>83</v>
       </c>
-      <c r="D91" s="42" t="s">
+      <c r="D98" s="42" t="s">
         <v>84</v>
       </c>
-      <c r="E91" t="s">
+      <c r="E98" t="s">
         <v>85</v>
       </c>
-      <c r="K91" s="60"/>
-      <c r="L91" t="s">
+      <c r="K98" s="60"/>
+      <c r="L98" t="s">
         <v>610</v>
       </c>
     </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="C92" t="s">
+    <row r="99" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="C99" t="s">
         <v>423</v>
       </c>
-      <c r="D92" s="42" t="s">
+      <c r="D99" s="42" t="s">
         <v>280</v>
       </c>
-      <c r="E92" s="5" t="s">
+      <c r="E99" s="5" t="s">
         <v>280</v>
       </c>
-      <c r="F92" s="5" t="s">
+      <c r="F99" s="5" t="s">
         <v>431</v>
       </c>
-      <c r="K92" s="70"/>
-      <c r="L92" t="s">
+      <c r="K99" s="70"/>
+      <c r="L99" t="s">
         <v>609</v>
       </c>
     </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="C93" t="s">
+    <row r="100" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="C100" t="s">
         <v>424</v>
       </c>
-      <c r="D93" s="47" t="s">
+      <c r="D100" s="47" t="s">
         <v>280</v>
       </c>
-      <c r="E93" s="64" t="s">
+      <c r="E100" s="64" t="s">
         <v>280</v>
       </c>
-      <c r="F93" s="5" t="s">
+      <c r="F100" s="5" t="s">
         <v>431</v>
       </c>
-      <c r="K93" s="61"/>
-      <c r="L93" t="s">
-        <v>674</v>
-      </c>
-    </row>
-    <row r="94" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C94" t="s">
+      <c r="K100" s="61"/>
+      <c r="L100" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="101" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C101" t="s">
         <v>425</v>
       </c>
-      <c r="D94" s="47" t="s">
+      <c r="D101" s="47" t="s">
         <v>280</v>
       </c>
-      <c r="E94" s="64" t="s">
+      <c r="E101" s="64" t="s">
         <v>280</v>
       </c>
-      <c r="F94" s="5" t="s">
+      <c r="F101" s="5" t="s">
         <v>431</v>
       </c>
-      <c r="J94" s="62" t="s">
+      <c r="J101" s="62" t="s">
         <v>470</v>
       </c>
     </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="C95" t="s">
+    <row r="102" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="C102" t="s">
         <v>426</v>
       </c>
-      <c r="D95" s="47" t="s">
+      <c r="D102" s="47" t="s">
         <v>280</v>
       </c>
-      <c r="E95" s="64" t="s">
+      <c r="E102" s="64" t="s">
         <v>280</v>
       </c>
-      <c r="F95" s="5" t="s">
+      <c r="F102" s="5" t="s">
         <v>431</v>
       </c>
-      <c r="J95" s="1" t="s">
+      <c r="J102" s="1" t="s">
         <v>462</v>
       </c>
-      <c r="K95" t="s">
+      <c r="K102" t="s">
         <v>471</v>
       </c>
     </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="C96" t="s">
+    <row r="103" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="C103" t="s">
         <v>427</v>
       </c>
-      <c r="D96" s="47" t="s">
+      <c r="D103" s="47" t="s">
         <v>280</v>
       </c>
-      <c r="E96" s="64" t="s">
+      <c r="E103" s="64" t="s">
         <v>280</v>
       </c>
-      <c r="F96" s="5" t="s">
+      <c r="F103" s="5" t="s">
         <v>431</v>
       </c>
-      <c r="J96" s="1" t="s">
+      <c r="J103" s="1" t="s">
         <v>466</v>
       </c>
-      <c r="K96" t="s">
+      <c r="K103" t="s">
         <v>472</v>
       </c>
     </row>
-    <row r="97" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="C97" t="s">
+    <row r="104" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="C104" t="s">
         <v>428</v>
       </c>
-      <c r="D97" s="47" t="s">
+      <c r="D104" s="47" t="s">
         <v>280</v>
       </c>
-      <c r="E97" s="64" t="s">
+      <c r="E104" s="64" t="s">
         <v>280</v>
       </c>
-      <c r="F97" s="5" t="s">
+      <c r="F104" s="5" t="s">
         <v>431</v>
       </c>
-      <c r="J97" s="1" t="s">
+      <c r="J104" s="1" t="s">
         <v>464</v>
       </c>
-      <c r="K97" t="s">
+      <c r="K104" t="s">
         <v>473</v>
       </c>
     </row>
-    <row r="98" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="C98" t="s">
+    <row r="105" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="C105" t="s">
         <v>611</v>
       </c>
-      <c r="D98" s="64" t="s">
+      <c r="D105" s="64" t="s">
         <v>418</v>
       </c>
-      <c r="E98" s="64" t="s">
+      <c r="E105" s="64" t="s">
         <v>612</v>
       </c>
-      <c r="F98" s="64" t="s">
+      <c r="F105" s="64" t="s">
         <v>613</v>
       </c>
-      <c r="J98" s="1"/>
-    </row>
-    <row r="99" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="J99" s="1" t="s">
+      <c r="J105" s="1"/>
+    </row>
+    <row r="106" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="J106" s="1" t="s">
         <v>465</v>
       </c>
-      <c r="K99" t="s">
+      <c r="K106" t="s">
         <v>474</v>
       </c>
     </row>
-    <row r="100" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B100" s="26" t="s">
+    <row r="107" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B107" s="26" t="s">
         <v>104</v>
-      </c>
-      <c r="C100" s="27"/>
-      <c r="D100" s="27"/>
-      <c r="E100" s="27"/>
-      <c r="F100" s="27"/>
-      <c r="G100" s="27"/>
-      <c r="H100" s="28"/>
-    </row>
-    <row r="101" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="C101" s="24" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="102" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="C102" t="s">
-        <v>277</v>
-      </c>
-      <c r="D102" s="42" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="103" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="C103" t="s">
-        <v>278</v>
-      </c>
-      <c r="D103" s="42" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="104" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="C104" t="s">
-        <v>279</v>
-      </c>
-      <c r="D104" s="42" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="105" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="C105" s="5"/>
-      <c r="D105" s="5"/>
-    </row>
-    <row r="106" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="C106" s="5"/>
-      <c r="D106" s="5"/>
-    </row>
-    <row r="107" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B107" s="26" t="s">
-        <v>417</v>
       </c>
       <c r="C107" s="27"/>
       <c r="D107" s="27"/>
@@ -5590,6 +5699,54 @@
       <c r="F107" s="27"/>
       <c r="G107" s="27"/>
       <c r="H107" s="28"/>
+    </row>
+    <row r="108" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="C108" s="24" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="109" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="C109" t="s">
+        <v>277</v>
+      </c>
+      <c r="D109" s="42" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="110" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="C110" t="s">
+        <v>278</v>
+      </c>
+      <c r="D110" s="42" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="111" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="C111" t="s">
+        <v>279</v>
+      </c>
+      <c r="D111" s="42" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="112" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="C112" s="5"/>
+      <c r="D112" s="5"/>
+    </row>
+    <row r="113" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C113" s="5"/>
+      <c r="D113" s="5"/>
+    </row>
+    <row r="114" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B114" s="26" t="s">
+        <v>417</v>
+      </c>
+      <c r="C114" s="27"/>
+      <c r="D114" s="27"/>
+      <c r="E114" s="27"/>
+      <c r="F114" s="27"/>
+      <c r="G114" s="27"/>
+      <c r="H114" s="28"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -5601,9 +5758,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:O107"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="3" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I86" sqref="I86"/>
+      <selection pane="topRight" activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8034,7 +8191,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:K100"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="A40" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="A57" sqref="A57"/>
     </sheetView>
   </sheetViews>
@@ -9699,7 +9856,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:K87"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Model running through for G7IC.
</commit_message>
<xml_diff>
--- a/RECC_Config.xlsx
+++ b/RECC_Config.xlsx
@@ -3074,8 +3074,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:O114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C75" sqref="C75"/>
+    <sheetView tabSelected="1" topLeftCell="A77" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C102" sqref="C102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5557,8 +5557,8 @@
       <c r="C99" t="s">
         <v>423</v>
       </c>
-      <c r="D99" s="42" t="s">
-        <v>280</v>
+      <c r="D99" s="5" t="s">
+        <v>431</v>
       </c>
       <c r="E99" s="5" t="s">
         <v>280</v>
@@ -5575,8 +5575,8 @@
       <c r="C100" t="s">
         <v>424</v>
       </c>
-      <c r="D100" s="47" t="s">
-        <v>280</v>
+      <c r="D100" s="5" t="s">
+        <v>431</v>
       </c>
       <c r="E100" s="64" t="s">
         <v>280</v>
@@ -5593,8 +5593,8 @@
       <c r="C101" t="s">
         <v>425</v>
       </c>
-      <c r="D101" s="47" t="s">
-        <v>280</v>
+      <c r="D101" s="5" t="s">
+        <v>431</v>
       </c>
       <c r="E101" s="64" t="s">
         <v>280</v>
@@ -5610,8 +5610,8 @@
       <c r="C102" t="s">
         <v>426</v>
       </c>
-      <c r="D102" s="47" t="s">
-        <v>280</v>
+      <c r="D102" s="5" t="s">
+        <v>431</v>
       </c>
       <c r="E102" s="64" t="s">
         <v>280</v>
@@ -5630,8 +5630,8 @@
       <c r="C103" t="s">
         <v>427</v>
       </c>
-      <c r="D103" s="47" t="s">
-        <v>280</v>
+      <c r="D103" s="5" t="s">
+        <v>431</v>
       </c>
       <c r="E103" s="64" t="s">
         <v>280</v>
@@ -5650,8 +5650,8 @@
       <c r="C104" t="s">
         <v>428</v>
       </c>
-      <c r="D104" s="47" t="s">
-        <v>280</v>
+      <c r="D104" s="5" t="s">
+        <v>431</v>
       </c>
       <c r="E104" s="64" t="s">
         <v>280</v>

</xml_diff>

<commit_message>
Several fixes: secondary material export, material content fabrication, mass balance.
</commit_message>
<xml_diff>
--- a/RECC_Config.xlsx
+++ b/RECC_Config.xlsx
@@ -3074,8 +3074,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:O114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A77" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C102" sqref="C102"/>
+    <sheetView tabSelected="1" topLeftCell="B72" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D88" sqref="D88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5558,7 +5558,7 @@
         <v>423</v>
       </c>
       <c r="D99" s="5" t="s">
-        <v>431</v>
+        <v>280</v>
       </c>
       <c r="E99" s="5" t="s">
         <v>280</v>
@@ -5575,8 +5575,8 @@
       <c r="C100" t="s">
         <v>424</v>
       </c>
-      <c r="D100" s="5" t="s">
-        <v>431</v>
+      <c r="D100" s="64" t="s">
+        <v>280</v>
       </c>
       <c r="E100" s="64" t="s">
         <v>280</v>
@@ -5593,8 +5593,8 @@
       <c r="C101" t="s">
         <v>425</v>
       </c>
-      <c r="D101" s="5" t="s">
-        <v>431</v>
+      <c r="D101" s="64" t="s">
+        <v>280</v>
       </c>
       <c r="E101" s="64" t="s">
         <v>280</v>
@@ -5610,8 +5610,8 @@
       <c r="C102" t="s">
         <v>426</v>
       </c>
-      <c r="D102" s="5" t="s">
-        <v>431</v>
+      <c r="D102" s="64" t="s">
+        <v>280</v>
       </c>
       <c r="E102" s="64" t="s">
         <v>280</v>
@@ -5630,8 +5630,8 @@
       <c r="C103" t="s">
         <v>427</v>
       </c>
-      <c r="D103" s="5" t="s">
-        <v>431</v>
+      <c r="D103" s="64" t="s">
+        <v>280</v>
       </c>
       <c r="E103" s="64" t="s">
         <v>280</v>
@@ -5650,8 +5650,8 @@
       <c r="C104" t="s">
         <v>428</v>
       </c>
-      <c r="D104" s="5" t="s">
-        <v>431</v>
+      <c r="D104" s="64" t="s">
+        <v>280</v>
       </c>
       <c r="E104" s="64" t="s">
         <v>280</v>

</xml_diff>

<commit_message>
This is the version with which the Feb15 intermediate report figures were created.
</commit_message>
<xml_diff>
--- a/RECC_Config.xlsx
+++ b/RECC_Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="8652" windowHeight="4896" tabRatio="844" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8652" windowHeight="4896" tabRatio="844" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="5" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5166" uniqueCount="777">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5183" uniqueCount="780">
   <si>
     <t>Description</t>
   </si>
@@ -2359,7 +2359,16 @@
     <t>USA+EU</t>
   </si>
   <si>
-    <t>RECC_USA_V1</t>
+    <t>ScrapExportRecyclingCredit</t>
+  </si>
+  <si>
+    <t>True if an emissions credit for avoided primary production is given.</t>
+  </si>
+  <si>
+    <t>RECC_EU_V1</t>
+  </si>
+  <si>
+    <t>residential buildings</t>
   </si>
 </sst>
 </file>
@@ -3067,7 +3076,7 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3110,7 +3119,7 @@
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="6" t="s">
-        <v>776</v>
+        <v>778</v>
       </c>
       <c r="G4" s="48"/>
     </row>
@@ -4733,10 +4742,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:O120"/>
+  <dimension ref="A2:O121"/>
   <sheetViews>
-    <sheetView topLeftCell="A85" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView topLeftCell="A46" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D120" sqref="D120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7375,33 +7384,38 @@
         <v>474</v>
       </c>
     </row>
-    <row r="108" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B108" s="26" t="s">
+    <row r="107" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="C107" t="s">
+        <v>776</v>
+      </c>
+      <c r="D107" s="64" t="s">
+        <v>280</v>
+      </c>
+      <c r="E107" s="64" t="s">
+        <v>777</v>
+      </c>
+      <c r="F107" s="64"/>
+      <c r="J107" s="1"/>
+    </row>
+    <row r="109" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B109" s="26" t="s">
         <v>104</v>
       </c>
-      <c r="C108" s="27"/>
-      <c r="D108" s="27"/>
-      <c r="E108" s="27"/>
-      <c r="F108" s="27"/>
-      <c r="G108" s="27"/>
-      <c r="H108" s="28"/>
-    </row>
-    <row r="109" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="C109" s="24" t="s">
+      <c r="C109" s="27"/>
+      <c r="D109" s="27"/>
+      <c r="E109" s="27"/>
+      <c r="F109" s="27"/>
+      <c r="G109" s="27"/>
+      <c r="H109" s="28"/>
+    </row>
+    <row r="110" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="C110" s="24" t="s">
         <v>70</v>
-      </c>
-    </row>
-    <row r="110" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="C110" t="s">
-        <v>277</v>
-      </c>
-      <c r="D110" s="42" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="111" spans="2:14" x14ac:dyDescent="0.3">
       <c r="C111" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D111" s="42" t="s">
         <v>280</v>
@@ -7409,23 +7423,23 @@
     </row>
     <row r="112" spans="2:14" x14ac:dyDescent="0.3">
       <c r="C112" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D112" s="42" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="113" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C113" s="63" t="s">
-        <v>735</v>
-      </c>
-      <c r="D113" s="47">
-        <v>5000</v>
+      <c r="C113" t="s">
+        <v>279</v>
+      </c>
+      <c r="D113" s="42" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="114" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C114" s="63" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="D114" s="47">
         <v>5000</v>
@@ -7433,50 +7447,58 @@
     </row>
     <row r="115" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C115" s="63" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="D115" s="47">
-        <v>5000</v>
+        <v>200</v>
       </c>
     </row>
     <row r="116" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C116" s="63" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="D116" s="47">
-        <v>5000</v>
+        <v>100</v>
       </c>
     </row>
     <row r="117" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C117" s="63" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="D117" s="47">
-        <v>5000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="118" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C118" s="63" t="s">
+        <v>739</v>
+      </c>
+      <c r="D118" s="47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C119" s="63" t="s">
         <v>740</v>
       </c>
-      <c r="D118" s="47">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="119" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C119" s="5"/>
-      <c r="D119" s="5"/>
+      <c r="D119" s="47">
+        <v>0</v>
+      </c>
     </row>
     <row r="120" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B120" s="26" t="s">
+      <c r="C120" s="5"/>
+      <c r="D120" s="5"/>
+    </row>
+    <row r="121" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B121" s="26" t="s">
         <v>417</v>
       </c>
-      <c r="C120" s="27"/>
-      <c r="D120" s="27"/>
-      <c r="E120" s="27"/>
-      <c r="F120" s="27"/>
-      <c r="G120" s="27"/>
-      <c r="H120" s="28"/>
+      <c r="C121" s="27"/>
+      <c r="D121" s="27"/>
+      <c r="E121" s="27"/>
+      <c r="F121" s="27"/>
+      <c r="G121" s="27"/>
+      <c r="H121" s="28"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -7486,10 +7508,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:O122"/>
+  <dimension ref="A2:O123"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView topLeftCell="A73" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B104" sqref="B104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10128,33 +10150,38 @@
         <v>474</v>
       </c>
     </row>
-    <row r="108" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B108" s="26" t="s">
+    <row r="107" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="C107" t="s">
+        <v>776</v>
+      </c>
+      <c r="D107" s="64" t="s">
+        <v>280</v>
+      </c>
+      <c r="E107" s="64" t="s">
+        <v>777</v>
+      </c>
+      <c r="F107" s="64"/>
+      <c r="J107" s="1"/>
+    </row>
+    <row r="109" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B109" s="26" t="s">
         <v>104</v>
       </c>
-      <c r="C108" s="27"/>
-      <c r="D108" s="27"/>
-      <c r="E108" s="27"/>
-      <c r="F108" s="27"/>
-      <c r="G108" s="27"/>
-      <c r="H108" s="28"/>
-    </row>
-    <row r="109" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="C109" s="24" t="s">
+      <c r="C109" s="27"/>
+      <c r="D109" s="27"/>
+      <c r="E109" s="27"/>
+      <c r="F109" s="27"/>
+      <c r="G109" s="27"/>
+      <c r="H109" s="28"/>
+    </row>
+    <row r="110" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="C110" s="24" t="s">
         <v>70</v>
-      </c>
-    </row>
-    <row r="110" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="C110" t="s">
-        <v>277</v>
-      </c>
-      <c r="D110" s="42" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="111" spans="2:14" x14ac:dyDescent="0.3">
       <c r="C111" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D111" s="42" t="s">
         <v>280</v>
@@ -10162,63 +10189,67 @@
     </row>
     <row r="112" spans="2:14" x14ac:dyDescent="0.3">
       <c r="C112" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D112" s="42" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="113" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C113" s="63" t="s">
-        <v>735</v>
-      </c>
-      <c r="D113" s="47">
-        <v>200</v>
+      <c r="C113" t="s">
+        <v>279</v>
+      </c>
+      <c r="D113" s="42" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="114" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C114" s="63" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="D114" s="47">
-        <v>5000</v>
+        <v>200</v>
       </c>
     </row>
     <row r="115" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C115" s="63" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="D115" s="47">
-        <v>5000</v>
+        <v>75</v>
       </c>
     </row>
     <row r="116" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C116" s="63" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="D116" s="47">
-        <v>5000</v>
+        <v>10</v>
       </c>
     </row>
     <row r="117" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C117" s="63" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="D117" s="47">
-        <v>5000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="118" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C118" s="63" t="s">
+        <v>739</v>
+      </c>
+      <c r="D118" s="47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C119" s="63" t="s">
         <v>740</v>
       </c>
-      <c r="D118" s="47">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="119" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C119" s="5"/>
-      <c r="D119" s="5"/>
+      <c r="D119" s="47">
+        <v>0</v>
+      </c>
     </row>
     <row r="120" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C120" s="5"/>
@@ -10229,15 +10260,19 @@
       <c r="D121" s="5"/>
     </row>
     <row r="122" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B122" s="26" t="s">
+      <c r="C122" s="5"/>
+      <c r="D122" s="5"/>
+    </row>
+    <row r="123" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B123" s="26" t="s">
         <v>417</v>
       </c>
-      <c r="C122" s="27"/>
-      <c r="D122" s="27"/>
-      <c r="E122" s="27"/>
-      <c r="F122" s="27"/>
-      <c r="G122" s="27"/>
-      <c r="H122" s="28"/>
+      <c r="C123" s="27"/>
+      <c r="D123" s="27"/>
+      <c r="E123" s="27"/>
+      <c r="F123" s="27"/>
+      <c r="G123" s="27"/>
+      <c r="H123" s="28"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -10246,10 +10281,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:O122"/>
+  <dimension ref="A2:O123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B82" workbookViewId="0">
-      <selection activeCell="D103" sqref="D103"/>
+    <sheetView topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="B104" sqref="B104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12747,7 +12782,7 @@
       <c r="C100" t="s">
         <v>423</v>
       </c>
-      <c r="D100" s="64" t="s">
+      <c r="D100" s="5" t="s">
         <v>280</v>
       </c>
       <c r="E100" s="5" t="s">
@@ -12832,8 +12867,8 @@
       <c r="C104" t="s">
         <v>427</v>
       </c>
-      <c r="D104" s="5" t="s">
-        <v>431</v>
+      <c r="D104" s="64" t="s">
+        <v>280</v>
       </c>
       <c r="E104" s="64" t="s">
         <v>280</v>
@@ -12852,8 +12887,8 @@
       <c r="C105" t="s">
         <v>428</v>
       </c>
-      <c r="D105" s="5" t="s">
-        <v>431</v>
+      <c r="D105" s="64" t="s">
+        <v>280</v>
       </c>
       <c r="E105" s="64" t="s">
         <v>280</v>
@@ -12873,7 +12908,7 @@
         <v>611</v>
       </c>
       <c r="D106" s="64" t="s">
-        <v>418</v>
+        <v>779</v>
       </c>
       <c r="E106" s="64" t="s">
         <v>612</v>
@@ -12888,33 +12923,38 @@
         <v>474</v>
       </c>
     </row>
-    <row r="108" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B108" s="26" t="s">
+    <row r="107" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="C107" t="s">
+        <v>776</v>
+      </c>
+      <c r="D107" s="64" t="s">
+        <v>280</v>
+      </c>
+      <c r="E107" s="64" t="s">
+        <v>777</v>
+      </c>
+      <c r="F107" s="64"/>
+      <c r="J107" s="1"/>
+    </row>
+    <row r="109" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B109" s="26" t="s">
         <v>104</v>
       </c>
-      <c r="C108" s="27"/>
-      <c r="D108" s="27"/>
-      <c r="E108" s="27"/>
-      <c r="F108" s="27"/>
-      <c r="G108" s="27"/>
-      <c r="H108" s="28"/>
-    </row>
-    <row r="109" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="C109" s="24" t="s">
+      <c r="C109" s="27"/>
+      <c r="D109" s="27"/>
+      <c r="E109" s="27"/>
+      <c r="F109" s="27"/>
+      <c r="G109" s="27"/>
+      <c r="H109" s="28"/>
+    </row>
+    <row r="110" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="C110" s="24" t="s">
         <v>70</v>
-      </c>
-    </row>
-    <row r="110" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="C110" t="s">
-        <v>277</v>
-      </c>
-      <c r="D110" s="42" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="111" spans="2:14" x14ac:dyDescent="0.3">
       <c r="C111" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D111" s="42" t="s">
         <v>280</v>
@@ -12922,63 +12962,67 @@
     </row>
     <row r="112" spans="2:14" x14ac:dyDescent="0.3">
       <c r="C112" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D112" s="42" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="113" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C113" s="63" t="s">
-        <v>735</v>
-      </c>
-      <c r="D113" s="47">
-        <v>2000</v>
+      <c r="C113" t="s">
+        <v>279</v>
+      </c>
+      <c r="D113" s="42" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="114" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C114" s="63" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="D114" s="47">
-        <v>5000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="115" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C115" s="63" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="D115" s="47">
-        <v>5000</v>
+        <v>200</v>
       </c>
     </row>
     <row r="116" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C116" s="63" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="D116" s="47">
-        <v>5000</v>
+        <v>100</v>
       </c>
     </row>
     <row r="117" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C117" s="63" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="D117" s="47">
-        <v>5000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="118" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C118" s="63" t="s">
+        <v>739</v>
+      </c>
+      <c r="D118" s="47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C119" s="63" t="s">
         <v>740</v>
       </c>
-      <c r="D118" s="47">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="119" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C119" s="5"/>
-      <c r="D119" s="5"/>
+      <c r="D119" s="47">
+        <v>0</v>
+      </c>
     </row>
     <row r="120" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C120" s="5"/>
@@ -12989,15 +13033,19 @@
       <c r="D121" s="5"/>
     </row>
     <row r="122" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B122" s="26" t="s">
+      <c r="C122" s="5"/>
+      <c r="D122" s="5"/>
+    </row>
+    <row r="123" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B123" s="26" t="s">
         <v>417</v>
       </c>
-      <c r="C122" s="27"/>
-      <c r="D122" s="27"/>
-      <c r="E122" s="27"/>
-      <c r="F122" s="27"/>
-      <c r="G122" s="27"/>
-      <c r="H122" s="28"/>
+      <c r="C123" s="27"/>
+      <c r="D123" s="27"/>
+      <c r="E123" s="27"/>
+      <c r="F123" s="27"/>
+      <c r="G123" s="27"/>
+      <c r="H123" s="28"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -13006,10 +13054,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:O120"/>
+  <dimension ref="A2:O121"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="D104" sqref="D104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15632,8 +15680,8 @@
       <c r="C106" t="s">
         <v>611</v>
       </c>
-      <c r="D106" s="64" t="s">
-        <v>418</v>
+      <c r="D106" s="19" t="s">
+        <v>779</v>
       </c>
       <c r="E106" s="64" t="s">
         <v>612</v>
@@ -15641,6 +15689,9 @@
       <c r="F106" s="64" t="s">
         <v>613</v>
       </c>
+      <c r="G106" s="19" t="s">
+        <v>779</v>
+      </c>
       <c r="J106" s="1" t="s">
         <v>465</v>
       </c>
@@ -15648,33 +15699,38 @@
         <v>474</v>
       </c>
     </row>
-    <row r="108" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B108" s="26" t="s">
+    <row r="107" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="C107" t="s">
+        <v>776</v>
+      </c>
+      <c r="D107" s="64" t="s">
+        <v>280</v>
+      </c>
+      <c r="E107" s="64" t="s">
+        <v>777</v>
+      </c>
+      <c r="F107" s="64"/>
+      <c r="J107" s="1"/>
+    </row>
+    <row r="109" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B109" s="26" t="s">
         <v>104</v>
       </c>
-      <c r="C108" s="27"/>
-      <c r="D108" s="27"/>
-      <c r="E108" s="27"/>
-      <c r="F108" s="27"/>
-      <c r="G108" s="27"/>
-      <c r="H108" s="28"/>
-    </row>
-    <row r="109" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="C109" s="24" t="s">
+      <c r="C109" s="27"/>
+      <c r="D109" s="27"/>
+      <c r="E109" s="27"/>
+      <c r="F109" s="27"/>
+      <c r="G109" s="27"/>
+      <c r="H109" s="28"/>
+    </row>
+    <row r="110" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="C110" s="24" t="s">
         <v>70</v>
-      </c>
-    </row>
-    <row r="110" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="C110" t="s">
-        <v>277</v>
-      </c>
-      <c r="D110" s="42" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="111" spans="2:14" x14ac:dyDescent="0.3">
       <c r="C111" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D111" s="42" t="s">
         <v>280</v>
@@ -15682,74 +15738,82 @@
     </row>
     <row r="112" spans="2:14" x14ac:dyDescent="0.3">
       <c r="C112" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D112" s="42" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="113" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C113" s="63" t="s">
-        <v>735</v>
-      </c>
-      <c r="D113" s="47">
-        <v>500</v>
+      <c r="C113" t="s">
+        <v>279</v>
+      </c>
+      <c r="D113" s="42" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="114" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C114" s="63" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="D114" s="47">
-        <v>5000</v>
+        <v>500</v>
       </c>
     </row>
     <row r="115" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C115" s="63" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="D115" s="47">
-        <v>5000</v>
+        <v>75</v>
       </c>
     </row>
     <row r="116" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C116" s="63" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="D116" s="47">
-        <v>5000</v>
+        <v>10</v>
       </c>
     </row>
     <row r="117" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C117" s="63" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="D117" s="47">
-        <v>5000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="118" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C118" s="63" t="s">
+        <v>739</v>
+      </c>
+      <c r="D118" s="47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C119" s="63" t="s">
         <v>740</v>
       </c>
-      <c r="D118" s="47">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="119" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C119" s="5"/>
-      <c r="D119" s="5"/>
+      <c r="D119" s="47">
+        <v>0</v>
+      </c>
     </row>
     <row r="120" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B120" s="26" t="s">
+      <c r="C120" s="5"/>
+      <c r="D120" s="5"/>
+    </row>
+    <row r="121" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B121" s="26" t="s">
         <v>417</v>
       </c>
-      <c r="C120" s="27"/>
-      <c r="D120" s="27"/>
-      <c r="E120" s="27"/>
-      <c r="F120" s="27"/>
-      <c r="G120" s="27"/>
-      <c r="H120" s="28"/>
+      <c r="C121" s="27"/>
+      <c r="D121" s="27"/>
+      <c r="E121" s="27"/>
+      <c r="F121" s="27"/>
+      <c r="G121" s="27"/>
+      <c r="H121" s="28"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -15758,10 +15822,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:O120"/>
+  <dimension ref="A2:O121"/>
   <sheetViews>
-    <sheetView topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="D113" sqref="D113"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="B101" sqref="B101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -18281,7 +18345,7 @@
       <c r="C101" t="s">
         <v>424</v>
       </c>
-      <c r="D101" s="5" t="s">
+      <c r="D101" s="64" t="s">
         <v>280</v>
       </c>
       <c r="E101" s="64" t="s">
@@ -18303,7 +18367,7 @@
       <c r="C102" t="s">
         <v>425</v>
       </c>
-      <c r="D102" s="5" t="s">
+      <c r="D102" s="64" t="s">
         <v>280</v>
       </c>
       <c r="E102" s="64" t="s">
@@ -18324,7 +18388,7 @@
       <c r="C103" t="s">
         <v>426</v>
       </c>
-      <c r="D103" s="5" t="s">
+      <c r="D103" s="64" t="s">
         <v>280</v>
       </c>
       <c r="E103" s="64" t="s">
@@ -18344,8 +18408,8 @@
       <c r="C104" t="s">
         <v>427</v>
       </c>
-      <c r="D104" s="5" t="s">
-        <v>431</v>
+      <c r="D104" s="64" t="s">
+        <v>280</v>
       </c>
       <c r="E104" s="64" t="s">
         <v>280</v>
@@ -18364,8 +18428,8 @@
       <c r="C105" t="s">
         <v>428</v>
       </c>
-      <c r="D105" s="5" t="s">
-        <v>431</v>
+      <c r="D105" s="64" t="s">
+        <v>280</v>
       </c>
       <c r="E105" s="64" t="s">
         <v>280</v>
@@ -18384,8 +18448,8 @@
       <c r="C106" t="s">
         <v>611</v>
       </c>
-      <c r="D106" s="64" t="s">
-        <v>418</v>
+      <c r="D106" s="19" t="s">
+        <v>779</v>
       </c>
       <c r="E106" s="64" t="s">
         <v>612</v>
@@ -18393,6 +18457,9 @@
       <c r="F106" s="64" t="s">
         <v>613</v>
       </c>
+      <c r="G106" s="19" t="s">
+        <v>779</v>
+      </c>
       <c r="J106" s="1" t="s">
         <v>465</v>
       </c>
@@ -18400,33 +18467,38 @@
         <v>474</v>
       </c>
     </row>
-    <row r="108" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B108" s="26" t="s">
+    <row r="107" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="C107" t="s">
+        <v>776</v>
+      </c>
+      <c r="D107" s="64" t="s">
+        <v>280</v>
+      </c>
+      <c r="E107" s="64" t="s">
+        <v>777</v>
+      </c>
+      <c r="F107" s="64"/>
+      <c r="J107" s="1"/>
+    </row>
+    <row r="109" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B109" s="26" t="s">
         <v>104</v>
       </c>
-      <c r="C108" s="27"/>
-      <c r="D108" s="27"/>
-      <c r="E108" s="27"/>
-      <c r="F108" s="27"/>
-      <c r="G108" s="27"/>
-      <c r="H108" s="28"/>
-    </row>
-    <row r="109" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="C109" s="24" t="s">
+      <c r="C109" s="27"/>
+      <c r="D109" s="27"/>
+      <c r="E109" s="27"/>
+      <c r="F109" s="27"/>
+      <c r="G109" s="27"/>
+      <c r="H109" s="28"/>
+    </row>
+    <row r="110" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="C110" s="24" t="s">
         <v>70</v>
-      </c>
-    </row>
-    <row r="110" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="C110" t="s">
-        <v>277</v>
-      </c>
-      <c r="D110" s="42" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="111" spans="2:14" x14ac:dyDescent="0.3">
       <c r="C111" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D111" s="42" t="s">
         <v>280</v>
@@ -18434,74 +18506,82 @@
     </row>
     <row r="112" spans="2:14" x14ac:dyDescent="0.3">
       <c r="C112" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D112" s="42" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="113" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C113" s="63" t="s">
-        <v>735</v>
-      </c>
-      <c r="D113" s="47">
-        <v>2000</v>
+      <c r="C113" t="s">
+        <v>279</v>
+      </c>
+      <c r="D113" s="42" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="114" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C114" s="63" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="D114" s="47">
-        <v>5000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="115" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C115" s="63" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="D115" s="47">
-        <v>5000</v>
+        <v>300</v>
       </c>
     </row>
     <row r="116" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C116" s="63" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="D116" s="47">
-        <v>5000</v>
+        <v>50</v>
       </c>
     </row>
     <row r="117" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C117" s="63" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="D117" s="47">
-        <v>5000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="118" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C118" s="63" t="s">
+        <v>739</v>
+      </c>
+      <c r="D118" s="47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C119" s="63" t="s">
         <v>740</v>
       </c>
-      <c r="D118" s="47">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="119" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C119" s="5"/>
-      <c r="D119" s="5"/>
+      <c r="D119" s="47">
+        <v>0</v>
+      </c>
     </row>
     <row r="120" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B120" s="26" t="s">
+      <c r="C120" s="5"/>
+      <c r="D120" s="5"/>
+    </row>
+    <row r="121" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B121" s="26" t="s">
         <v>417</v>
       </c>
-      <c r="C120" s="27"/>
-      <c r="D120" s="27"/>
-      <c r="E120" s="27"/>
-      <c r="F120" s="27"/>
-      <c r="G120" s="27"/>
-      <c r="H120" s="28"/>
+      <c r="C121" s="27"/>
+      <c r="D121" s="27"/>
+      <c r="E121" s="27"/>
+      <c r="F121" s="27"/>
+      <c r="G121" s="27"/>
+      <c r="H121" s="28"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added area plot code for RE strategy cascade.
</commit_message>
<xml_diff>
--- a/RECC_Config.xlsx
+++ b/RECC_Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="8652" windowHeight="4896" tabRatio="707" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8652" windowHeight="4896" tabRatio="707" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="5" r:id="rId1"/>
@@ -5734,8 +5734,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:Q129"/>
   <sheetViews>
-    <sheetView topLeftCell="C70" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E77" sqref="E77:I77"/>
+    <sheetView tabSelected="1" topLeftCell="C10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8901,8 +8901,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:Q129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D107" sqref="D107"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11754,7 +11754,7 @@
         <v>187</v>
       </c>
       <c r="D106" s="5" t="s">
-        <v>125</v>
+        <v>191</v>
       </c>
       <c r="E106" s="5" t="s">
         <v>125</v>
@@ -11889,7 +11889,7 @@
         <v>185</v>
       </c>
       <c r="D112" s="5" t="s">
-        <v>191</v>
+        <v>125</v>
       </c>
       <c r="E112" s="58" t="s">
         <v>125</v>
@@ -11927,7 +11927,7 @@
         <v>284</v>
       </c>
       <c r="D114" s="58" t="s">
-        <v>286</v>
+        <v>523</v>
       </c>
       <c r="E114" s="58" t="s">
         <v>285</v>

</xml_diff>

<commit_message>
Added new reuse routine. Exact mass balance for all processes now.
</commit_message>
<xml_diff>
--- a/RECC_Config.xlsx
+++ b/RECC_Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="8652" windowHeight="4896" tabRatio="707" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8652" windowHeight="4896" tabRatio="707" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="5" r:id="rId1"/>
@@ -1650,7 +1650,7 @@
     <t>R32CAN</t>
   </si>
   <si>
-    <t>RECC_G7</t>
+    <t>RECC_Germany</t>
   </si>
 </sst>
 </file>
@@ -9066,8 +9066,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:Q132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D111" sqref="D111:D112"/>
+    <sheetView topLeftCell="A85" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C111" sqref="C111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12061,7 +12061,7 @@
         <v>185</v>
       </c>
       <c r="D111" s="5" t="s">
-        <v>190</v>
+        <v>124</v>
       </c>
       <c r="E111" s="58" t="s">
         <v>124</v>
@@ -12090,7 +12090,7 @@
         <v>184</v>
       </c>
       <c r="D112" s="5" t="s">
-        <v>124</v>
+        <v>190</v>
       </c>
       <c r="E112" s="58" t="s">
         <v>124</v>
@@ -22030,8 +22030,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:Q132"/>
   <sheetViews>
-    <sheetView topLeftCell="A85" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D113" sqref="D113"/>
+    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D110" sqref="D110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -25104,7 +25104,7 @@
         <v>283</v>
       </c>
       <c r="D114" s="58" t="s">
-        <v>521</v>
+        <v>285</v>
       </c>
       <c r="E114" s="58" t="s">
         <v>284</v>

</xml_diff>

<commit_message>
Added sensitivity analysis folders and refined plots.
</commit_message>
<xml_diff>
--- a/RECC_Config.xlsx
+++ b/RECC_Config.xlsx
@@ -16143,8 +16143,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:Q136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B118" sqref="B118"/>
+    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D120" sqref="D120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19169,7 +19169,7 @@
         <v>583</v>
       </c>
       <c r="D111" s="101" t="s">
-        <v>124</v>
+        <v>190</v>
       </c>
       <c r="E111" s="58" t="s">
         <v>124</v>

</xml_diff>

<commit_message>
Latest minor changes for 19 June 2019 full scenario run.
</commit_message>
<xml_diff>
--- a/RECC_Config.xlsx
+++ b/RECC_Config.xlsx
@@ -5834,7 +5834,7 @@
       </c>
       <c r="D118" s="81" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="E118" s="39" t="inlineStr">
@@ -10930,7 +10930,7 @@
       </c>
       <c r="D118" s="81" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="E118" s="39" t="inlineStr">
@@ -16026,7 +16026,7 @@
       </c>
       <c r="D118" s="81" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="E118" s="39" t="inlineStr">
@@ -21122,7 +21122,7 @@
       </c>
       <c r="D118" s="81" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="E118" s="39" t="inlineStr">
@@ -26218,7 +26218,7 @@
       </c>
       <c r="D118" s="81" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="E118" s="39" t="inlineStr">
@@ -41313,7 +41313,7 @@
       </c>
       <c r="D118" s="81" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="E118" s="39" t="inlineStr">
@@ -51505,7 +51505,7 @@
       </c>
       <c r="D118" s="81" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="E118" s="39" t="inlineStr">
@@ -56601,7 +56601,7 @@
       </c>
       <c r="D118" s="81" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="E118" s="39" t="inlineStr">
@@ -61697,7 +61697,7 @@
       </c>
       <c r="D118" s="81" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="E118" s="39" t="inlineStr">
@@ -66793,7 +66793,7 @@
       </c>
       <c r="D118" s="81" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="E118" s="39" t="inlineStr">

</xml_diff>

<commit_message>
replaced / by np.divide.
</commit_message>
<xml_diff>
--- a/RECC_Config.xlsx
+++ b/RECC_Config.xlsx
@@ -46161,7 +46161,7 @@
       </c>
       <c r="D112" s="70" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="E112" s="39" t="inlineStr">
@@ -46372,7 +46372,7 @@
       </c>
       <c r="D117" s="81" t="inlineStr">
         <is>
-          <t>residential buildings</t>
+          <t>passenger vehicles</t>
         </is>
       </c>
       <c r="E117" s="39" t="inlineStr">
@@ -46409,7 +46409,7 @@
       </c>
       <c r="D118" s="81" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="E118" s="39" t="inlineStr">
@@ -46428,7 +46428,7 @@
       </c>
       <c r="D119" s="81" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="E119" s="39" t="inlineStr">

</xml_diff>

<commit_message>
June 25 full model run. New parameter values lead to different extrapolation needs. Added export of MJ/km and MJ/m2.
</commit_message>
<xml_diff>
--- a/RECC_Config.xlsx
+++ b/RECC_Config.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView activeTab="2" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView activeTab="6" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="9402" windowWidth="20730" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Config" sheetId="1" state="visible" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RECC_India" sheetId="14" state="visible" r:id="rId14"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -747,14 +747,14 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col bestFit="1" customWidth="1" max="1" min="1" style="42" width="12.6640625"/>
+    <col bestFit="1" customWidth="1" max="1" min="1" style="42" width="12.68359375"/>
     <col bestFit="1" customWidth="1" max="2" min="2" style="42" width="31"/>
-    <col customWidth="1" max="4" min="4" style="42" width="26.5546875"/>
+    <col customWidth="1" max="4" min="4" style="42" width="26.5234375"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -950,19 +950,19 @@
       <selection activeCell="C112" sqref="C112"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col customWidth="1" max="2" min="2" style="42" width="36.33203125"/>
+    <col customWidth="1" max="2" min="2" style="42" width="36.3125"/>
     <col customWidth="1" max="3" min="3" style="42" width="44"/>
-    <col customWidth="1" max="4" min="4" style="42" width="39.6640625"/>
-    <col customWidth="1" max="5" min="5" style="42" width="25.6640625"/>
-    <col customWidth="1" max="6" min="6" style="42" width="21.6640625"/>
-    <col customWidth="1" max="7" min="7" style="42" width="38.44140625"/>
-    <col customWidth="1" max="8" min="8" style="42" width="12.33203125"/>
-    <col customWidth="1" max="9" min="9" style="42" width="38.44140625"/>
-    <col customWidth="1" max="11" min="10" style="42" width="11.5546875"/>
-    <col customWidth="1" max="12" min="12" style="42" width="73.5546875"/>
-    <col customWidth="1" max="13" min="13" style="42" width="39.88671875"/>
+    <col customWidth="1" max="4" min="4" style="42" width="39.68359375"/>
+    <col customWidth="1" max="5" min="5" style="42" width="25.68359375"/>
+    <col customWidth="1" max="6" min="6" style="42" width="21.68359375"/>
+    <col customWidth="1" max="7" min="7" style="42" width="38.41796875"/>
+    <col customWidth="1" max="8" min="8" style="42" width="12.3125"/>
+    <col customWidth="1" max="9" min="9" style="42" width="38.41796875"/>
+    <col customWidth="1" max="11" min="10" style="42" width="11.5234375"/>
+    <col customWidth="1" max="12" min="12" style="42" width="73.5234375"/>
+    <col customWidth="1" max="13" min="13" style="42" width="39.89453125"/>
     <col customWidth="1" max="14" min="14" style="42" width="90"/>
   </cols>
   <sheetData>
@@ -1138,7 +1138,7 @@
       <c r="H15" s="16" t="n"/>
       <c r="I15" s="22" t="inlineStr">
         <is>
-          <t>    *) Selector: specify string to select index values, choose one of four options: 'All' or list of indices to select: '[0,1,10,15,28]', or 'All except [3,4,5,6,7]', or semi-open interval '[260:401)'</t>
+          <t>*) Selector: specify string to select index values, choose one of four options: 'All' or list of indices to select: '[0,1,10,15,28]', or 'All except [3,4,5,6,7]', or semi-open interval '[260:401)'</t>
         </is>
       </c>
     </row>
@@ -1372,7 +1372,7 @@
       </c>
       <c r="D22" s="70" t="inlineStr">
         <is>
-          <t>Engineering material production processes </t>
+          <t>Engineering material production processes</t>
         </is>
       </c>
       <c r="E22" s="70" t="inlineStr">
@@ -3656,7 +3656,7 @@
       <c r="K80" s="43" t="n"/>
       <c r="L80" t="inlineStr">
         <is>
-          <t>Global average only, is applied to all countries by model script. </t>
+          <t>Global average only, is applied to all countries by model script.</t>
         </is>
       </c>
       <c r="M80" t="inlineStr">
@@ -3727,7 +3727,7 @@
       <c r="K81" s="43" t="n"/>
       <c r="L81" t="inlineStr">
         <is>
-          <t>Global average only, is applied to all countries by model script. </t>
+          <t>Global average only, is applied to all countries by model script.</t>
         </is>
       </c>
       <c r="M81" s="39" t="n">
@@ -3865,7 +3865,7 @@
       <c r="K83" s="43" t="n"/>
       <c r="L83" t="inlineStr">
         <is>
-          <t>Global average only, is applied to all countries by model script. </t>
+          <t>Global average only, is applied to all countries by model script.</t>
         </is>
       </c>
       <c r="M83" t="inlineStr">
@@ -3936,7 +3936,7 @@
       <c r="K84" s="43" t="n"/>
       <c r="L84" t="inlineStr">
         <is>
-          <t>Global average only, is applied to all countries by model script. </t>
+          <t>Global average only, is applied to all countries by model script.</t>
         </is>
       </c>
       <c r="M84" t="inlineStr">
@@ -6046,19 +6046,19 @@
       <selection activeCell="C112" sqref="C112"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col customWidth="1" max="2" min="2" style="42" width="36.33203125"/>
+    <col customWidth="1" max="2" min="2" style="42" width="36.3125"/>
     <col customWidth="1" max="3" min="3" style="42" width="44"/>
-    <col customWidth="1" max="4" min="4" style="42" width="39.6640625"/>
-    <col customWidth="1" max="5" min="5" style="42" width="25.6640625"/>
-    <col customWidth="1" max="6" min="6" style="42" width="21.6640625"/>
-    <col customWidth="1" max="7" min="7" style="42" width="38.44140625"/>
-    <col customWidth="1" max="8" min="8" style="42" width="12.33203125"/>
-    <col customWidth="1" max="9" min="9" style="42" width="38.44140625"/>
-    <col customWidth="1" max="11" min="10" style="42" width="11.5546875"/>
-    <col customWidth="1" max="12" min="12" style="42" width="73.5546875"/>
-    <col customWidth="1" max="13" min="13" style="42" width="39.88671875"/>
+    <col customWidth="1" max="4" min="4" style="42" width="39.68359375"/>
+    <col customWidth="1" max="5" min="5" style="42" width="25.68359375"/>
+    <col customWidth="1" max="6" min="6" style="42" width="21.68359375"/>
+    <col customWidth="1" max="7" min="7" style="42" width="38.41796875"/>
+    <col customWidth="1" max="8" min="8" style="42" width="12.3125"/>
+    <col customWidth="1" max="9" min="9" style="42" width="38.41796875"/>
+    <col customWidth="1" max="11" min="10" style="42" width="11.5234375"/>
+    <col customWidth="1" max="12" min="12" style="42" width="73.5234375"/>
+    <col customWidth="1" max="13" min="13" style="42" width="39.89453125"/>
     <col customWidth="1" max="14" min="14" style="42" width="90"/>
   </cols>
   <sheetData>
@@ -6234,7 +6234,7 @@
       <c r="H15" s="16" t="n"/>
       <c r="I15" s="22" t="inlineStr">
         <is>
-          <t>    *) Selector: specify string to select index values, choose one of four options: 'All' or list of indices to select: '[0,1,10,15,28]', or 'All except [3,4,5,6,7]', or semi-open interval '[260:401)'</t>
+          <t>*) Selector: specify string to select index values, choose one of four options: 'All' or list of indices to select: '[0,1,10,15,28]', or 'All except [3,4,5,6,7]', or semi-open interval '[260:401)'</t>
         </is>
       </c>
     </row>
@@ -6468,7 +6468,7 @@
       </c>
       <c r="D22" s="70" t="inlineStr">
         <is>
-          <t>Engineering material production processes </t>
+          <t>Engineering material production processes</t>
         </is>
       </c>
       <c r="E22" s="70" t="inlineStr">
@@ -8752,7 +8752,7 @@
       <c r="K80" s="43" t="n"/>
       <c r="L80" t="inlineStr">
         <is>
-          <t>Global average only, is applied to all countries by model script. </t>
+          <t>Global average only, is applied to all countries by model script.</t>
         </is>
       </c>
       <c r="M80" t="inlineStr">
@@ -8823,7 +8823,7 @@
       <c r="K81" s="43" t="n"/>
       <c r="L81" t="inlineStr">
         <is>
-          <t>Global average only, is applied to all countries by model script. </t>
+          <t>Global average only, is applied to all countries by model script.</t>
         </is>
       </c>
       <c r="M81" s="39" t="n">
@@ -8961,7 +8961,7 @@
       <c r="K83" s="43" t="n"/>
       <c r="L83" t="inlineStr">
         <is>
-          <t>Global average only, is applied to all countries by model script. </t>
+          <t>Global average only, is applied to all countries by model script.</t>
         </is>
       </c>
       <c r="M83" t="inlineStr">
@@ -9032,7 +9032,7 @@
       <c r="K84" s="43" t="n"/>
       <c r="L84" t="inlineStr">
         <is>
-          <t>Global average only, is applied to all countries by model script. </t>
+          <t>Global average only, is applied to all countries by model script.</t>
         </is>
       </c>
       <c r="M84" t="inlineStr">
@@ -11142,19 +11142,19 @@
       <selection activeCell="C112" sqref="C112"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col customWidth="1" max="2" min="2" style="42" width="36.33203125"/>
+    <col customWidth="1" max="2" min="2" style="42" width="36.3125"/>
     <col customWidth="1" max="3" min="3" style="42" width="44"/>
-    <col customWidth="1" max="4" min="4" style="42" width="39.6640625"/>
-    <col customWidth="1" max="5" min="5" style="42" width="25.6640625"/>
-    <col customWidth="1" max="6" min="6" style="42" width="21.6640625"/>
-    <col customWidth="1" max="7" min="7" style="42" width="38.44140625"/>
-    <col customWidth="1" max="8" min="8" style="42" width="12.33203125"/>
-    <col customWidth="1" max="9" min="9" style="42" width="38.44140625"/>
-    <col customWidth="1" max="11" min="10" style="42" width="11.5546875"/>
-    <col customWidth="1" max="12" min="12" style="42" width="73.5546875"/>
-    <col customWidth="1" max="13" min="13" style="42" width="39.88671875"/>
+    <col customWidth="1" max="4" min="4" style="42" width="39.68359375"/>
+    <col customWidth="1" max="5" min="5" style="42" width="25.68359375"/>
+    <col customWidth="1" max="6" min="6" style="42" width="21.68359375"/>
+    <col customWidth="1" max="7" min="7" style="42" width="38.41796875"/>
+    <col customWidth="1" max="8" min="8" style="42" width="12.3125"/>
+    <col customWidth="1" max="9" min="9" style="42" width="38.41796875"/>
+    <col customWidth="1" max="11" min="10" style="42" width="11.5234375"/>
+    <col customWidth="1" max="12" min="12" style="42" width="73.5234375"/>
+    <col customWidth="1" max="13" min="13" style="42" width="39.89453125"/>
     <col customWidth="1" max="14" min="14" style="42" width="90"/>
   </cols>
   <sheetData>
@@ -11330,7 +11330,7 @@
       <c r="H15" s="16" t="n"/>
       <c r="I15" s="22" t="inlineStr">
         <is>
-          <t>    *) Selector: specify string to select index values, choose one of four options: 'All' or list of indices to select: '[0,1,10,15,28]', or 'All except [3,4,5,6,7]', or semi-open interval '[260:401)'</t>
+          <t>*) Selector: specify string to select index values, choose one of four options: 'All' or list of indices to select: '[0,1,10,15,28]', or 'All except [3,4,5,6,7]', or semi-open interval '[260:401)'</t>
         </is>
       </c>
     </row>
@@ -11564,7 +11564,7 @@
       </c>
       <c r="D22" s="70" t="inlineStr">
         <is>
-          <t>Engineering material production processes </t>
+          <t>Engineering material production processes</t>
         </is>
       </c>
       <c r="E22" s="70" t="inlineStr">
@@ -13848,7 +13848,7 @@
       <c r="K80" s="43" t="n"/>
       <c r="L80" t="inlineStr">
         <is>
-          <t>Global average only, is applied to all countries by model script. </t>
+          <t>Global average only, is applied to all countries by model script.</t>
         </is>
       </c>
       <c r="M80" t="inlineStr">
@@ -13919,7 +13919,7 @@
       <c r="K81" s="43" t="n"/>
       <c r="L81" t="inlineStr">
         <is>
-          <t>Global average only, is applied to all countries by model script. </t>
+          <t>Global average only, is applied to all countries by model script.</t>
         </is>
       </c>
       <c r="M81" s="39" t="n">
@@ -14057,7 +14057,7 @@
       <c r="K83" s="43" t="n"/>
       <c r="L83" t="inlineStr">
         <is>
-          <t>Global average only, is applied to all countries by model script. </t>
+          <t>Global average only, is applied to all countries by model script.</t>
         </is>
       </c>
       <c r="M83" t="inlineStr">
@@ -14128,7 +14128,7 @@
       <c r="K84" s="43" t="n"/>
       <c r="L84" t="inlineStr">
         <is>
-          <t>Global average only, is applied to all countries by model script. </t>
+          <t>Global average only, is applied to all countries by model script.</t>
         </is>
       </c>
       <c r="M84" t="inlineStr">
@@ -16238,19 +16238,19 @@
       <selection activeCell="C112" sqref="C112"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col customWidth="1" max="2" min="2" style="42" width="36.33203125"/>
+    <col customWidth="1" max="2" min="2" style="42" width="36.3125"/>
     <col customWidth="1" max="3" min="3" style="42" width="44"/>
-    <col customWidth="1" max="4" min="4" style="42" width="39.6640625"/>
-    <col customWidth="1" max="5" min="5" style="42" width="25.6640625"/>
-    <col customWidth="1" max="6" min="6" style="42" width="21.6640625"/>
-    <col customWidth="1" max="7" min="7" style="42" width="38.44140625"/>
-    <col customWidth="1" max="8" min="8" style="42" width="12.33203125"/>
-    <col customWidth="1" max="9" min="9" style="42" width="38.44140625"/>
-    <col customWidth="1" max="11" min="10" style="42" width="11.5546875"/>
-    <col customWidth="1" max="12" min="12" style="42" width="73.5546875"/>
-    <col customWidth="1" max="13" min="13" style="42" width="39.88671875"/>
+    <col customWidth="1" max="4" min="4" style="42" width="39.68359375"/>
+    <col customWidth="1" max="5" min="5" style="42" width="25.68359375"/>
+    <col customWidth="1" max="6" min="6" style="42" width="21.68359375"/>
+    <col customWidth="1" max="7" min="7" style="42" width="38.41796875"/>
+    <col customWidth="1" max="8" min="8" style="42" width="12.3125"/>
+    <col customWidth="1" max="9" min="9" style="42" width="38.41796875"/>
+    <col customWidth="1" max="11" min="10" style="42" width="11.5234375"/>
+    <col customWidth="1" max="12" min="12" style="42" width="73.5234375"/>
+    <col customWidth="1" max="13" min="13" style="42" width="39.89453125"/>
     <col customWidth="1" max="14" min="14" style="42" width="90"/>
   </cols>
   <sheetData>
@@ -16426,7 +16426,7 @@
       <c r="H15" s="16" t="n"/>
       <c r="I15" s="22" t="inlineStr">
         <is>
-          <t>    *) Selector: specify string to select index values, choose one of four options: 'All' or list of indices to select: '[0,1,10,15,28]', or 'All except [3,4,5,6,7]', or semi-open interval '[260:401)'</t>
+          <t>*) Selector: specify string to select index values, choose one of four options: 'All' or list of indices to select: '[0,1,10,15,28]', or 'All except [3,4,5,6,7]', or semi-open interval '[260:401)'</t>
         </is>
       </c>
     </row>
@@ -16660,7 +16660,7 @@
       </c>
       <c r="D22" s="70" t="inlineStr">
         <is>
-          <t>Engineering material production processes </t>
+          <t>Engineering material production processes</t>
         </is>
       </c>
       <c r="E22" s="70" t="inlineStr">
@@ -18944,7 +18944,7 @@
       <c r="K80" s="43" t="n"/>
       <c r="L80" t="inlineStr">
         <is>
-          <t>Global average only, is applied to all countries by model script. </t>
+          <t>Global average only, is applied to all countries by model script.</t>
         </is>
       </c>
       <c r="M80" t="inlineStr">
@@ -19015,7 +19015,7 @@
       <c r="K81" s="43" t="n"/>
       <c r="L81" t="inlineStr">
         <is>
-          <t>Global average only, is applied to all countries by model script. </t>
+          <t>Global average only, is applied to all countries by model script.</t>
         </is>
       </c>
       <c r="M81" s="39" t="n">
@@ -19153,7 +19153,7 @@
       <c r="K83" s="43" t="n"/>
       <c r="L83" t="inlineStr">
         <is>
-          <t>Global average only, is applied to all countries by model script. </t>
+          <t>Global average only, is applied to all countries by model script.</t>
         </is>
       </c>
       <c r="M83" t="inlineStr">
@@ -19224,7 +19224,7 @@
       <c r="K84" s="43" t="n"/>
       <c r="L84" t="inlineStr">
         <is>
-          <t>Global average only, is applied to all countries by model script. </t>
+          <t>Global average only, is applied to all countries by model script.</t>
         </is>
       </c>
       <c r="M84" t="inlineStr">
@@ -21334,19 +21334,19 @@
       <selection activeCell="C112" sqref="C112"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col customWidth="1" max="2" min="2" style="42" width="36.33203125"/>
+    <col customWidth="1" max="2" min="2" style="42" width="36.3125"/>
     <col customWidth="1" max="3" min="3" style="42" width="44"/>
-    <col customWidth="1" max="4" min="4" style="42" width="39.6640625"/>
-    <col customWidth="1" max="5" min="5" style="42" width="25.6640625"/>
-    <col customWidth="1" max="6" min="6" style="42" width="21.6640625"/>
-    <col customWidth="1" max="7" min="7" style="42" width="38.44140625"/>
-    <col customWidth="1" max="8" min="8" style="42" width="12.33203125"/>
-    <col customWidth="1" max="9" min="9" style="42" width="38.44140625"/>
-    <col customWidth="1" max="11" min="10" style="42" width="11.5546875"/>
-    <col customWidth="1" max="12" min="12" style="42" width="73.5546875"/>
-    <col customWidth="1" max="13" min="13" style="42" width="39.88671875"/>
+    <col customWidth="1" max="4" min="4" style="42" width="39.68359375"/>
+    <col customWidth="1" max="5" min="5" style="42" width="25.68359375"/>
+    <col customWidth="1" max="6" min="6" style="42" width="21.68359375"/>
+    <col customWidth="1" max="7" min="7" style="42" width="38.41796875"/>
+    <col customWidth="1" max="8" min="8" style="42" width="12.3125"/>
+    <col customWidth="1" max="9" min="9" style="42" width="38.41796875"/>
+    <col customWidth="1" max="11" min="10" style="42" width="11.5234375"/>
+    <col customWidth="1" max="12" min="12" style="42" width="73.5234375"/>
+    <col customWidth="1" max="13" min="13" style="42" width="39.89453125"/>
     <col customWidth="1" max="14" min="14" style="42" width="90"/>
   </cols>
   <sheetData>
@@ -21522,7 +21522,7 @@
       <c r="H15" s="16" t="n"/>
       <c r="I15" s="22" t="inlineStr">
         <is>
-          <t>    *) Selector: specify string to select index values, choose one of four options: 'All' or list of indices to select: '[0,1,10,15,28]', or 'All except [3,4,5,6,7]', or semi-open interval '[260:401)'</t>
+          <t>*) Selector: specify string to select index values, choose one of four options: 'All' or list of indices to select: '[0,1,10,15,28]', or 'All except [3,4,5,6,7]', or semi-open interval '[260:401)'</t>
         </is>
       </c>
     </row>
@@ -21756,7 +21756,7 @@
       </c>
       <c r="D22" s="70" t="inlineStr">
         <is>
-          <t>Engineering material production processes </t>
+          <t>Engineering material production processes</t>
         </is>
       </c>
       <c r="E22" s="70" t="inlineStr">
@@ -24040,7 +24040,7 @@
       <c r="K80" s="43" t="n"/>
       <c r="L80" t="inlineStr">
         <is>
-          <t>Global average only, is applied to all countries by model script. </t>
+          <t>Global average only, is applied to all countries by model script.</t>
         </is>
       </c>
       <c r="M80" t="inlineStr">
@@ -24111,7 +24111,7 @@
       <c r="K81" s="43" t="n"/>
       <c r="L81" t="inlineStr">
         <is>
-          <t>Global average only, is applied to all countries by model script. </t>
+          <t>Global average only, is applied to all countries by model script.</t>
         </is>
       </c>
       <c r="M81" s="39" t="n">
@@ -24249,7 +24249,7 @@
       <c r="K83" s="43" t="n"/>
       <c r="L83" t="inlineStr">
         <is>
-          <t>Global average only, is applied to all countries by model script. </t>
+          <t>Global average only, is applied to all countries by model script.</t>
         </is>
       </c>
       <c r="M83" t="inlineStr">
@@ -24320,7 +24320,7 @@
       <c r="K84" s="43" t="n"/>
       <c r="L84" t="inlineStr">
         <is>
-          <t>Global average only, is applied to all countries by model script. </t>
+          <t>Global average only, is applied to all countries by model script.</t>
         </is>
       </c>
       <c r="M84" t="inlineStr">
@@ -26430,19 +26430,19 @@
       <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col customWidth="1" max="2" min="2" style="42" width="36.33203125"/>
+    <col customWidth="1" max="2" min="2" style="42" width="36.3125"/>
     <col customWidth="1" max="3" min="3" style="42" width="44"/>
-    <col customWidth="1" max="4" min="4" style="42" width="39.6640625"/>
-    <col customWidth="1" max="5" min="5" style="42" width="50.6640625"/>
-    <col customWidth="1" max="6" min="6" style="42" width="21.6640625"/>
-    <col customWidth="1" max="7" min="7" style="42" width="38.44140625"/>
-    <col customWidth="1" max="8" min="8" style="42" width="12.33203125"/>
-    <col customWidth="1" max="9" min="9" style="42" width="38.44140625"/>
-    <col customWidth="1" max="11" min="10" style="42" width="11.5546875"/>
-    <col customWidth="1" max="12" min="12" style="42" width="73.5546875"/>
-    <col customWidth="1" max="13" min="13" style="42" width="39.88671875"/>
+    <col customWidth="1" max="4" min="4" style="42" width="39.68359375"/>
+    <col customWidth="1" max="5" min="5" style="42" width="50.68359375"/>
+    <col customWidth="1" max="6" min="6" style="42" width="21.68359375"/>
+    <col customWidth="1" max="7" min="7" style="42" width="38.41796875"/>
+    <col customWidth="1" max="8" min="8" style="42" width="12.3125"/>
+    <col customWidth="1" max="9" min="9" style="42" width="38.41796875"/>
+    <col customWidth="1" max="11" min="10" style="42" width="11.5234375"/>
+    <col customWidth="1" max="12" min="12" style="42" width="73.5234375"/>
+    <col customWidth="1" max="13" min="13" style="42" width="39.89453125"/>
     <col customWidth="1" max="14" min="14" style="42" width="90"/>
   </cols>
   <sheetData>
@@ -26618,7 +26618,7 @@
       <c r="H15" s="16" t="n"/>
       <c r="I15" s="22" t="inlineStr">
         <is>
-          <t>    *) Selector: specify string to select index values, choose one of four options: 'All' or list of indices to select: '[0,1,10,15,28]', or 'All except [3,4,5,6,7]', or semi-open interval '[260:401)'</t>
+          <t>*) Selector: specify string to select index values, choose one of four options: 'All' or list of indices to select: '[0,1,10,15,28]', or 'All except [3,4,5,6,7]', or semi-open interval '[260:401)'</t>
         </is>
       </c>
     </row>
@@ -26852,7 +26852,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Engineering material production processes </t>
+          <t>Engineering material production processes</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -29170,7 +29170,7 @@
       <c r="K80" s="43" t="n"/>
       <c r="L80" t="inlineStr">
         <is>
-          <t>Global average only, is applied to all countries by model script. </t>
+          <t>Global average only, is applied to all countries by model script.</t>
         </is>
       </c>
       <c r="M80" t="inlineStr">
@@ -29241,7 +29241,7 @@
       <c r="K81" s="43" t="n"/>
       <c r="L81" t="inlineStr">
         <is>
-          <t>Global average only, is applied to all countries by model script. </t>
+          <t>Global average only, is applied to all countries by model script.</t>
         </is>
       </c>
       <c r="M81" s="39" t="n">
@@ -29379,7 +29379,7 @@
       <c r="K83" s="43" t="n"/>
       <c r="L83" t="inlineStr">
         <is>
-          <t>Global average only, is applied to all countries by model script. </t>
+          <t>Global average only, is applied to all countries by model script.</t>
         </is>
       </c>
       <c r="M83" t="inlineStr">
@@ -29450,7 +29450,7 @@
       <c r="K84" s="43" t="n"/>
       <c r="L84" t="inlineStr">
         <is>
-          <t>Global average only, is applied to all countries by model script. </t>
+          <t>Global average only, is applied to all countries by model script.</t>
         </is>
       </c>
       <c r="M84" t="inlineStr">
@@ -31328,23 +31328,23 @@
   </sheetPr>
   <dimension ref="A2:Q136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B103" workbookViewId="0" zoomScale="70" zoomScaleNormal="70">
+    <sheetView topLeftCell="B103" workbookViewId="0" zoomScale="70" zoomScaleNormal="70">
       <selection activeCell="G127" sqref="G127"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col customWidth="1" max="2" min="2" style="42" width="36.33203125"/>
+    <col customWidth="1" max="2" min="2" style="42" width="36.3125"/>
     <col customWidth="1" max="3" min="3" style="42" width="44"/>
-    <col customWidth="1" max="4" min="4" style="42" width="39.6640625"/>
-    <col customWidth="1" max="5" min="5" style="42" width="25.6640625"/>
-    <col customWidth="1" max="6" min="6" style="42" width="21.6640625"/>
-    <col customWidth="1" max="7" min="7" style="42" width="38.44140625"/>
-    <col customWidth="1" max="8" min="8" style="42" width="12.33203125"/>
-    <col customWidth="1" max="9" min="9" style="42" width="38.44140625"/>
-    <col customWidth="1" max="11" min="10" style="42" width="11.5546875"/>
-    <col customWidth="1" max="12" min="12" style="42" width="73.5546875"/>
-    <col customWidth="1" max="13" min="13" style="42" width="39.88671875"/>
+    <col customWidth="1" max="4" min="4" style="42" width="39.68359375"/>
+    <col customWidth="1" max="5" min="5" style="42" width="25.68359375"/>
+    <col customWidth="1" max="6" min="6" style="42" width="21.68359375"/>
+    <col customWidth="1" max="7" min="7" style="42" width="38.41796875"/>
+    <col customWidth="1" max="8" min="8" style="42" width="12.3125"/>
+    <col customWidth="1" max="9" min="9" style="42" width="38.41796875"/>
+    <col customWidth="1" max="11" min="10" style="42" width="11.5234375"/>
+    <col customWidth="1" max="12" min="12" style="42" width="73.5234375"/>
+    <col customWidth="1" max="13" min="13" style="42" width="39.89453125"/>
     <col customWidth="1" max="14" min="14" style="42" width="90"/>
   </cols>
   <sheetData>
@@ -31520,7 +31520,7 @@
       <c r="H15" s="16" t="n"/>
       <c r="I15" s="22" t="inlineStr">
         <is>
-          <t>    *) Selector: specify string to select index values, choose one of four options: 'All' or list of indices to select: '[0,1,10,15,28]', or 'All except [3,4,5,6,7]', or semi-open interval '[260:401)'</t>
+          <t>*) Selector: specify string to select index values, choose one of four options: 'All' or list of indices to select: '[0,1,10,15,28]', or 'All except [3,4,5,6,7]', or semi-open interval '[260:401)'</t>
         </is>
       </c>
     </row>
@@ -31754,7 +31754,7 @@
       </c>
       <c r="D22" s="70" t="inlineStr">
         <is>
-          <t>Engineering material production processes </t>
+          <t>Engineering material production processes</t>
         </is>
       </c>
       <c r="E22" s="70" t="inlineStr">
@@ -34038,7 +34038,7 @@
       <c r="K80" s="43" t="n"/>
       <c r="L80" t="inlineStr">
         <is>
-          <t>Global average only, is applied to all countries by model script. </t>
+          <t>Global average only, is applied to all countries by model script.</t>
         </is>
       </c>
       <c r="M80" t="inlineStr">
@@ -34109,7 +34109,7 @@
       <c r="K81" s="43" t="n"/>
       <c r="L81" t="inlineStr">
         <is>
-          <t>Global average only, is applied to all countries by model script. </t>
+          <t>Global average only, is applied to all countries by model script.</t>
         </is>
       </c>
       <c r="M81" s="39" t="n">
@@ -34247,7 +34247,7 @@
       <c r="K83" s="43" t="n"/>
       <c r="L83" t="inlineStr">
         <is>
-          <t>Global average only, is applied to all countries by model script. </t>
+          <t>Global average only, is applied to all countries by model script.</t>
         </is>
       </c>
       <c r="M83" t="inlineStr">
@@ -34318,7 +34318,7 @@
       <c r="K84" s="43" t="n"/>
       <c r="L84" t="inlineStr">
         <is>
-          <t>Global average only, is applied to all countries by model script. </t>
+          <t>Global average only, is applied to all countries by model script.</t>
         </is>
       </c>
       <c r="M84" t="inlineStr">
@@ -36429,19 +36429,19 @@
       <selection activeCell="C112" sqref="C112"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col customWidth="1" max="2" min="2" style="42" width="36.33203125"/>
+    <col customWidth="1" max="2" min="2" style="42" width="36.3125"/>
     <col customWidth="1" max="3" min="3" style="42" width="44"/>
-    <col customWidth="1" max="4" min="4" style="42" width="39.6640625"/>
-    <col customWidth="1" max="5" min="5" style="42" width="25.6640625"/>
-    <col customWidth="1" max="6" min="6" style="42" width="21.6640625"/>
-    <col customWidth="1" max="7" min="7" style="42" width="38.44140625"/>
-    <col customWidth="1" max="8" min="8" style="42" width="12.33203125"/>
-    <col customWidth="1" max="9" min="9" style="42" width="38.44140625"/>
-    <col customWidth="1" max="11" min="10" style="42" width="11.5546875"/>
-    <col customWidth="1" max="12" min="12" style="42" width="73.5546875"/>
-    <col customWidth="1" max="13" min="13" style="42" width="39.88671875"/>
+    <col customWidth="1" max="4" min="4" style="42" width="39.68359375"/>
+    <col customWidth="1" max="5" min="5" style="42" width="25.68359375"/>
+    <col customWidth="1" max="6" min="6" style="42" width="21.68359375"/>
+    <col customWidth="1" max="7" min="7" style="42" width="38.41796875"/>
+    <col customWidth="1" max="8" min="8" style="42" width="12.3125"/>
+    <col customWidth="1" max="9" min="9" style="42" width="38.41796875"/>
+    <col customWidth="1" max="11" min="10" style="42" width="11.5234375"/>
+    <col customWidth="1" max="12" min="12" style="42" width="73.5234375"/>
+    <col customWidth="1" max="13" min="13" style="42" width="39.89453125"/>
     <col customWidth="1" max="14" min="14" style="42" width="90"/>
   </cols>
   <sheetData>
@@ -36617,7 +36617,7 @@
       <c r="H15" s="16" t="n"/>
       <c r="I15" s="22" t="inlineStr">
         <is>
-          <t>    *) Selector: specify string to select index values, choose one of four options: 'All' or list of indices to select: '[0,1,10,15,28]', or 'All except [3,4,5,6,7]', or semi-open interval '[260:401)'</t>
+          <t>*) Selector: specify string to select index values, choose one of four options: 'All' or list of indices to select: '[0,1,10,15,28]', or 'All except [3,4,5,6,7]', or semi-open interval '[260:401)'</t>
         </is>
       </c>
     </row>
@@ -36851,7 +36851,7 @@
       </c>
       <c r="D22" s="70" t="inlineStr">
         <is>
-          <t>Engineering material production processes </t>
+          <t>Engineering material production processes</t>
         </is>
       </c>
       <c r="E22" s="70" t="inlineStr">
@@ -39135,7 +39135,7 @@
       <c r="K80" s="43" t="n"/>
       <c r="L80" t="inlineStr">
         <is>
-          <t>Global average only, is applied to all countries by model script. </t>
+          <t>Global average only, is applied to all countries by model script.</t>
         </is>
       </c>
       <c r="M80" t="inlineStr">
@@ -39206,7 +39206,7 @@
       <c r="K81" s="43" t="n"/>
       <c r="L81" t="inlineStr">
         <is>
-          <t>Global average only, is applied to all countries by model script. </t>
+          <t>Global average only, is applied to all countries by model script.</t>
         </is>
       </c>
       <c r="M81" s="39" t="n">
@@ -39344,7 +39344,7 @@
       <c r="K83" s="43" t="n"/>
       <c r="L83" t="inlineStr">
         <is>
-          <t>Global average only, is applied to all countries by model script. </t>
+          <t>Global average only, is applied to all countries by model script.</t>
         </is>
       </c>
       <c r="M83" t="inlineStr">
@@ -39415,7 +39415,7 @@
       <c r="K84" s="43" t="n"/>
       <c r="L84" t="inlineStr">
         <is>
-          <t>Global average only, is applied to all countries by model script. </t>
+          <t>Global average only, is applied to all countries by model script.</t>
         </is>
       </c>
       <c r="M84" t="inlineStr">
@@ -41525,19 +41525,19 @@
       <selection activeCell="C112" sqref="C112"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col customWidth="1" max="2" min="2" style="42" width="36.33203125"/>
+    <col customWidth="1" max="2" min="2" style="42" width="36.3125"/>
     <col customWidth="1" max="3" min="3" style="42" width="44"/>
-    <col customWidth="1" max="4" min="4" style="42" width="39.6640625"/>
-    <col customWidth="1" max="5" min="5" style="42" width="25.6640625"/>
-    <col customWidth="1" max="6" min="6" style="42" width="21.6640625"/>
-    <col customWidth="1" max="7" min="7" style="42" width="38.44140625"/>
-    <col customWidth="1" max="8" min="8" style="42" width="12.33203125"/>
-    <col customWidth="1" max="9" min="9" style="42" width="38.44140625"/>
-    <col customWidth="1" max="11" min="10" style="42" width="11.5546875"/>
-    <col customWidth="1" max="12" min="12" style="42" width="73.5546875"/>
-    <col customWidth="1" max="13" min="13" style="42" width="39.88671875"/>
+    <col customWidth="1" max="4" min="4" style="42" width="39.68359375"/>
+    <col customWidth="1" max="5" min="5" style="42" width="25.68359375"/>
+    <col customWidth="1" max="6" min="6" style="42" width="21.68359375"/>
+    <col customWidth="1" max="7" min="7" style="42" width="38.41796875"/>
+    <col customWidth="1" max="8" min="8" style="42" width="12.3125"/>
+    <col customWidth="1" max="9" min="9" style="42" width="38.41796875"/>
+    <col customWidth="1" max="11" min="10" style="42" width="11.5234375"/>
+    <col customWidth="1" max="12" min="12" style="42" width="73.5234375"/>
+    <col customWidth="1" max="13" min="13" style="42" width="39.89453125"/>
     <col customWidth="1" max="14" min="14" style="42" width="90"/>
   </cols>
   <sheetData>
@@ -41713,7 +41713,7 @@
       <c r="H15" s="16" t="n"/>
       <c r="I15" s="22" t="inlineStr">
         <is>
-          <t>    *) Selector: specify string to select index values, choose one of four options: 'All' or list of indices to select: '[0,1,10,15,28]', or 'All except [3,4,5,6,7]', or semi-open interval '[260:401)'</t>
+          <t>*) Selector: specify string to select index values, choose one of four options: 'All' or list of indices to select: '[0,1,10,15,28]', or 'All except [3,4,5,6,7]', or semi-open interval '[260:401)'</t>
         </is>
       </c>
     </row>
@@ -41947,7 +41947,7 @@
       </c>
       <c r="D22" s="70" t="inlineStr">
         <is>
-          <t>Engineering material production processes </t>
+          <t>Engineering material production processes</t>
         </is>
       </c>
       <c r="E22" s="70" t="inlineStr">
@@ -44231,7 +44231,7 @@
       <c r="K80" s="43" t="n"/>
       <c r="L80" t="inlineStr">
         <is>
-          <t>Global average only, is applied to all countries by model script. </t>
+          <t>Global average only, is applied to all countries by model script.</t>
         </is>
       </c>
       <c r="M80" t="inlineStr">
@@ -44302,7 +44302,7 @@
       <c r="K81" s="43" t="n"/>
       <c r="L81" t="inlineStr">
         <is>
-          <t>Global average only, is applied to all countries by model script. </t>
+          <t>Global average only, is applied to all countries by model script.</t>
         </is>
       </c>
       <c r="M81" s="39" t="n">
@@ -44440,7 +44440,7 @@
       <c r="K83" s="43" t="n"/>
       <c r="L83" t="inlineStr">
         <is>
-          <t>Global average only, is applied to all countries by model script. </t>
+          <t>Global average only, is applied to all countries by model script.</t>
         </is>
       </c>
       <c r="M83" t="inlineStr">
@@ -44511,7 +44511,7 @@
       <c r="K84" s="43" t="n"/>
       <c r="L84" t="inlineStr">
         <is>
-          <t>Global average only, is applied to all countries by model script. </t>
+          <t>Global average only, is applied to all countries by model script.</t>
         </is>
       </c>
       <c r="M84" t="inlineStr">
@@ -46161,7 +46161,7 @@
       </c>
       <c r="D112" s="70" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E112" s="39" t="inlineStr">
@@ -46372,7 +46372,7 @@
       </c>
       <c r="D117" s="81" t="inlineStr">
         <is>
-          <t>passenger vehicles</t>
+          <t>residential buildings</t>
         </is>
       </c>
       <c r="E117" s="39" t="inlineStr">
@@ -46409,7 +46409,7 @@
       </c>
       <c r="D118" s="81" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E118" s="39" t="inlineStr">
@@ -46428,7 +46428,7 @@
       </c>
       <c r="D119" s="81" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E119" s="39" t="inlineStr">
@@ -46621,19 +46621,19 @@
       <selection activeCell="C112" sqref="C112"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col customWidth="1" max="2" min="2" style="42" width="36.33203125"/>
+    <col customWidth="1" max="2" min="2" style="42" width="36.3125"/>
     <col customWidth="1" max="3" min="3" style="42" width="44"/>
-    <col customWidth="1" max="4" min="4" style="42" width="39.6640625"/>
-    <col customWidth="1" max="5" min="5" style="42" width="25.6640625"/>
-    <col customWidth="1" max="6" min="6" style="42" width="21.6640625"/>
-    <col customWidth="1" max="7" min="7" style="42" width="38.44140625"/>
-    <col customWidth="1" max="8" min="8" style="42" width="12.33203125"/>
-    <col customWidth="1" max="9" min="9" style="42" width="38.44140625"/>
-    <col customWidth="1" max="11" min="10" style="42" width="11.5546875"/>
-    <col customWidth="1" max="12" min="12" style="42" width="73.5546875"/>
-    <col customWidth="1" max="13" min="13" style="42" width="39.88671875"/>
+    <col customWidth="1" max="4" min="4" style="42" width="39.68359375"/>
+    <col customWidth="1" max="5" min="5" style="42" width="25.68359375"/>
+    <col customWidth="1" max="6" min="6" style="42" width="21.68359375"/>
+    <col customWidth="1" max="7" min="7" style="42" width="38.41796875"/>
+    <col customWidth="1" max="8" min="8" style="42" width="12.3125"/>
+    <col customWidth="1" max="9" min="9" style="42" width="38.41796875"/>
+    <col customWidth="1" max="11" min="10" style="42" width="11.5234375"/>
+    <col customWidth="1" max="12" min="12" style="42" width="73.5234375"/>
+    <col customWidth="1" max="13" min="13" style="42" width="39.89453125"/>
     <col customWidth="1" max="14" min="14" style="42" width="90"/>
   </cols>
   <sheetData>
@@ -46809,7 +46809,7 @@
       <c r="H15" s="16" t="n"/>
       <c r="I15" s="22" t="inlineStr">
         <is>
-          <t>    *) Selector: specify string to select index values, choose one of four options: 'All' or list of indices to select: '[0,1,10,15,28]', or 'All except [3,4,5,6,7]', or semi-open interval '[260:401)'</t>
+          <t>*) Selector: specify string to select index values, choose one of four options: 'All' or list of indices to select: '[0,1,10,15,28]', or 'All except [3,4,5,6,7]', or semi-open interval '[260:401)'</t>
         </is>
       </c>
     </row>
@@ -47043,7 +47043,7 @@
       </c>
       <c r="D22" s="70" t="inlineStr">
         <is>
-          <t>Engineering material production processes </t>
+          <t>Engineering material production processes</t>
         </is>
       </c>
       <c r="E22" s="70" t="inlineStr">
@@ -49327,7 +49327,7 @@
       <c r="K80" s="43" t="n"/>
       <c r="L80" t="inlineStr">
         <is>
-          <t>Global average only, is applied to all countries by model script. </t>
+          <t>Global average only, is applied to all countries by model script.</t>
         </is>
       </c>
       <c r="M80" t="inlineStr">
@@ -49398,7 +49398,7 @@
       <c r="K81" s="43" t="n"/>
       <c r="L81" t="inlineStr">
         <is>
-          <t>Global average only, is applied to all countries by model script. </t>
+          <t>Global average only, is applied to all countries by model script.</t>
         </is>
       </c>
       <c r="M81" s="39" t="n">
@@ -49536,7 +49536,7 @@
       <c r="K83" s="43" t="n"/>
       <c r="L83" t="inlineStr">
         <is>
-          <t>Global average only, is applied to all countries by model script. </t>
+          <t>Global average only, is applied to all countries by model script.</t>
         </is>
       </c>
       <c r="M83" t="inlineStr">
@@ -49607,7 +49607,7 @@
       <c r="K84" s="43" t="n"/>
       <c r="L84" t="inlineStr">
         <is>
-          <t>Global average only, is applied to all countries by model script. </t>
+          <t>Global average only, is applied to all countries by model script.</t>
         </is>
       </c>
       <c r="M84" t="inlineStr">
@@ -51713,23 +51713,23 @@
   </sheetPr>
   <dimension ref="A2:Q136"/>
   <sheetViews>
-    <sheetView topLeftCell="A88" workbookViewId="0" zoomScale="70" zoomScaleNormal="70">
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0" zoomScale="70" zoomScaleNormal="70">
       <selection activeCell="C112" sqref="C112"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col customWidth="1" max="2" min="2" style="42" width="36.33203125"/>
+    <col customWidth="1" max="2" min="2" style="42" width="36.3125"/>
     <col customWidth="1" max="3" min="3" style="42" width="44"/>
-    <col customWidth="1" max="4" min="4" style="42" width="39.6640625"/>
-    <col customWidth="1" max="5" min="5" style="42" width="25.6640625"/>
-    <col customWidth="1" max="6" min="6" style="42" width="21.6640625"/>
-    <col customWidth="1" max="7" min="7" style="42" width="38.44140625"/>
-    <col customWidth="1" max="8" min="8" style="42" width="12.33203125"/>
-    <col customWidth="1" max="9" min="9" style="42" width="38.44140625"/>
-    <col customWidth="1" max="11" min="10" style="42" width="11.5546875"/>
-    <col customWidth="1" max="12" min="12" style="42" width="73.5546875"/>
-    <col customWidth="1" max="13" min="13" style="42" width="39.88671875"/>
+    <col customWidth="1" max="4" min="4" style="42" width="39.68359375"/>
+    <col customWidth="1" max="5" min="5" style="42" width="25.68359375"/>
+    <col customWidth="1" max="6" min="6" style="42" width="21.68359375"/>
+    <col customWidth="1" max="7" min="7" style="42" width="38.41796875"/>
+    <col customWidth="1" max="8" min="8" style="42" width="12.3125"/>
+    <col customWidth="1" max="9" min="9" style="42" width="38.41796875"/>
+    <col customWidth="1" max="11" min="10" style="42" width="11.5234375"/>
+    <col customWidth="1" max="12" min="12" style="42" width="73.5234375"/>
+    <col customWidth="1" max="13" min="13" style="42" width="39.89453125"/>
     <col customWidth="1" max="14" min="14" style="42" width="90"/>
   </cols>
   <sheetData>
@@ -51905,7 +51905,7 @@
       <c r="H15" s="16" t="n"/>
       <c r="I15" s="22" t="inlineStr">
         <is>
-          <t>    *) Selector: specify string to select index values, choose one of four options: 'All' or list of indices to select: '[0,1,10,15,28]', or 'All except [3,4,5,6,7]', or semi-open interval '[260:401)'</t>
+          <t>*) Selector: specify string to select index values, choose one of four options: 'All' or list of indices to select: '[0,1,10,15,28]', or 'All except [3,4,5,6,7]', or semi-open interval '[260:401)'</t>
         </is>
       </c>
     </row>
@@ -52139,7 +52139,7 @@
       </c>
       <c r="D22" s="70" t="inlineStr">
         <is>
-          <t>Engineering material production processes </t>
+          <t>Engineering material production processes</t>
         </is>
       </c>
       <c r="E22" s="70" t="inlineStr">
@@ -54423,7 +54423,7 @@
       <c r="K80" s="43" t="n"/>
       <c r="L80" t="inlineStr">
         <is>
-          <t>Global average only, is applied to all countries by model script. </t>
+          <t>Global average only, is applied to all countries by model script.</t>
         </is>
       </c>
       <c r="M80" t="inlineStr">
@@ -54494,7 +54494,7 @@
       <c r="K81" s="43" t="n"/>
       <c r="L81" t="inlineStr">
         <is>
-          <t>Global average only, is applied to all countries by model script. </t>
+          <t>Global average only, is applied to all countries by model script.</t>
         </is>
       </c>
       <c r="M81" s="39" t="n">
@@ -54632,7 +54632,7 @@
       <c r="K83" s="43" t="n"/>
       <c r="L83" t="inlineStr">
         <is>
-          <t>Global average only, is applied to all countries by model script. </t>
+          <t>Global average only, is applied to all countries by model script.</t>
         </is>
       </c>
       <c r="M83" t="inlineStr">
@@ -54703,7 +54703,7 @@
       <c r="K84" s="43" t="n"/>
       <c r="L84" t="inlineStr">
         <is>
-          <t>Global average only, is applied to all countries by model script. </t>
+          <t>Global average only, is applied to all countries by model script.</t>
         </is>
       </c>
       <c r="M84" t="inlineStr">
@@ -56813,19 +56813,19 @@
       <selection activeCell="C112" sqref="C112"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col customWidth="1" max="2" min="2" style="42" width="36.33203125"/>
+    <col customWidth="1" max="2" min="2" style="42" width="36.3125"/>
     <col customWidth="1" max="3" min="3" style="42" width="44"/>
-    <col customWidth="1" max="4" min="4" style="42" width="39.6640625"/>
-    <col customWidth="1" max="5" min="5" style="42" width="25.6640625"/>
-    <col customWidth="1" max="6" min="6" style="42" width="21.6640625"/>
-    <col customWidth="1" max="7" min="7" style="42" width="38.44140625"/>
-    <col customWidth="1" max="8" min="8" style="42" width="12.33203125"/>
-    <col customWidth="1" max="9" min="9" style="42" width="38.44140625"/>
-    <col customWidth="1" max="11" min="10" style="42" width="11.5546875"/>
-    <col customWidth="1" max="12" min="12" style="42" width="73.5546875"/>
-    <col customWidth="1" max="13" min="13" style="42" width="39.88671875"/>
+    <col customWidth="1" max="4" min="4" style="42" width="39.68359375"/>
+    <col customWidth="1" max="5" min="5" style="42" width="25.68359375"/>
+    <col customWidth="1" max="6" min="6" style="42" width="21.68359375"/>
+    <col customWidth="1" max="7" min="7" style="42" width="38.41796875"/>
+    <col customWidth="1" max="8" min="8" style="42" width="12.3125"/>
+    <col customWidth="1" max="9" min="9" style="42" width="38.41796875"/>
+    <col customWidth="1" max="11" min="10" style="42" width="11.5234375"/>
+    <col customWidth="1" max="12" min="12" style="42" width="73.5234375"/>
+    <col customWidth="1" max="13" min="13" style="42" width="39.89453125"/>
     <col customWidth="1" max="14" min="14" style="42" width="90"/>
   </cols>
   <sheetData>
@@ -57001,7 +57001,7 @@
       <c r="H15" s="16" t="n"/>
       <c r="I15" s="22" t="inlineStr">
         <is>
-          <t>    *) Selector: specify string to select index values, choose one of four options: 'All' or list of indices to select: '[0,1,10,15,28]', or 'All except [3,4,5,6,7]', or semi-open interval '[260:401)'</t>
+          <t>*) Selector: specify string to select index values, choose one of four options: 'All' or list of indices to select: '[0,1,10,15,28]', or 'All except [3,4,5,6,7]', or semi-open interval '[260:401)'</t>
         </is>
       </c>
     </row>
@@ -57235,7 +57235,7 @@
       </c>
       <c r="D22" s="70" t="inlineStr">
         <is>
-          <t>Engineering material production processes </t>
+          <t>Engineering material production processes</t>
         </is>
       </c>
       <c r="E22" s="70" t="inlineStr">
@@ -59519,7 +59519,7 @@
       <c r="K80" s="43" t="n"/>
       <c r="L80" t="inlineStr">
         <is>
-          <t>Global average only, is applied to all countries by model script. </t>
+          <t>Global average only, is applied to all countries by model script.</t>
         </is>
       </c>
       <c r="M80" t="inlineStr">
@@ -59590,7 +59590,7 @@
       <c r="K81" s="43" t="n"/>
       <c r="L81" t="inlineStr">
         <is>
-          <t>Global average only, is applied to all countries by model script. </t>
+          <t>Global average only, is applied to all countries by model script.</t>
         </is>
       </c>
       <c r="M81" s="39" t="n">
@@ -59728,7 +59728,7 @@
       <c r="K83" s="43" t="n"/>
       <c r="L83" t="inlineStr">
         <is>
-          <t>Global average only, is applied to all countries by model script. </t>
+          <t>Global average only, is applied to all countries by model script.</t>
         </is>
       </c>
       <c r="M83" t="inlineStr">
@@ -59799,7 +59799,7 @@
       <c r="K84" s="43" t="n"/>
       <c r="L84" t="inlineStr">
         <is>
-          <t>Global average only, is applied to all countries by model script. </t>
+          <t>Global average only, is applied to all countries by model script.</t>
         </is>
       </c>
       <c r="M84" t="inlineStr">
@@ -61909,19 +61909,19 @@
       <selection activeCell="C112" sqref="C112"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col customWidth="1" max="2" min="2" style="42" width="36.33203125"/>
+    <col customWidth="1" max="2" min="2" style="42" width="36.3125"/>
     <col customWidth="1" max="3" min="3" style="42" width="44"/>
-    <col customWidth="1" max="4" min="4" style="42" width="39.6640625"/>
-    <col customWidth="1" max="5" min="5" style="42" width="25.6640625"/>
-    <col customWidth="1" max="6" min="6" style="42" width="21.6640625"/>
-    <col customWidth="1" max="7" min="7" style="42" width="38.44140625"/>
-    <col customWidth="1" max="8" min="8" style="42" width="12.33203125"/>
-    <col customWidth="1" max="9" min="9" style="42" width="38.44140625"/>
-    <col customWidth="1" max="11" min="10" style="42" width="11.5546875"/>
-    <col customWidth="1" max="12" min="12" style="42" width="73.5546875"/>
-    <col customWidth="1" max="13" min="13" style="42" width="39.88671875"/>
+    <col customWidth="1" max="4" min="4" style="42" width="39.68359375"/>
+    <col customWidth="1" max="5" min="5" style="42" width="25.68359375"/>
+    <col customWidth="1" max="6" min="6" style="42" width="21.68359375"/>
+    <col customWidth="1" max="7" min="7" style="42" width="38.41796875"/>
+    <col customWidth="1" max="8" min="8" style="42" width="12.3125"/>
+    <col customWidth="1" max="9" min="9" style="42" width="38.41796875"/>
+    <col customWidth="1" max="11" min="10" style="42" width="11.5234375"/>
+    <col customWidth="1" max="12" min="12" style="42" width="73.5234375"/>
+    <col customWidth="1" max="13" min="13" style="42" width="39.89453125"/>
     <col customWidth="1" max="14" min="14" style="42" width="90"/>
   </cols>
   <sheetData>
@@ -62097,7 +62097,7 @@
       <c r="H15" s="16" t="n"/>
       <c r="I15" s="22" t="inlineStr">
         <is>
-          <t>    *) Selector: specify string to select index values, choose one of four options: 'All' or list of indices to select: '[0,1,10,15,28]', or 'All except [3,4,5,6,7]', or semi-open interval '[260:401)'</t>
+          <t>*) Selector: specify string to select index values, choose one of four options: 'All' or list of indices to select: '[0,1,10,15,28]', or 'All except [3,4,5,6,7]', or semi-open interval '[260:401)'</t>
         </is>
       </c>
     </row>
@@ -62331,7 +62331,7 @@
       </c>
       <c r="D22" s="70" t="inlineStr">
         <is>
-          <t>Engineering material production processes </t>
+          <t>Engineering material production processes</t>
         </is>
       </c>
       <c r="E22" s="70" t="inlineStr">
@@ -64615,7 +64615,7 @@
       <c r="K80" s="43" t="n"/>
       <c r="L80" t="inlineStr">
         <is>
-          <t>Global average only, is applied to all countries by model script. </t>
+          <t>Global average only, is applied to all countries by model script.</t>
         </is>
       </c>
       <c r="M80" t="inlineStr">
@@ -64686,7 +64686,7 @@
       <c r="K81" s="43" t="n"/>
       <c r="L81" t="inlineStr">
         <is>
-          <t>Global average only, is applied to all countries by model script. </t>
+          <t>Global average only, is applied to all countries by model script.</t>
         </is>
       </c>
       <c r="M81" s="39" t="n">
@@ -64824,7 +64824,7 @@
       <c r="K83" s="43" t="n"/>
       <c r="L83" t="inlineStr">
         <is>
-          <t>Global average only, is applied to all countries by model script. </t>
+          <t>Global average only, is applied to all countries by model script.</t>
         </is>
       </c>
       <c r="M83" t="inlineStr">
@@ -64895,7 +64895,7 @@
       <c r="K84" s="43" t="n"/>
       <c r="L84" t="inlineStr">
         <is>
-          <t>Global average only, is applied to all countries by model script. </t>
+          <t>Global average only, is applied to all countries by model script.</t>
         </is>
       </c>
       <c r="M84" t="inlineStr">

</xml_diff>